<commit_message>
working for multiple toc lookups
but not for NR_104_Delays (Falls over on writing to excel)
</commit_message>
<xml_diff>
--- a/DataValidation/data validation for 105_FMILEAGE.xlsx
+++ b/DataValidation/data validation for 105_FMILEAGE.xlsx
@@ -29,10 +29,10 @@
     <t>train_operating_company_key</t>
   </si>
   <si>
-    <t>train_operating_company_name</t>
+    <t>provisional</t>
   </si>
   <si>
-    <t>provisional</t>
+    <t>train_operating_company_key_toc_name</t>
   </si>
   <si>
     <t>trains_planned</t>
@@ -578,10 +578,10 @@
       <c r="B2" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="1" t="s"/>
+      <c r="D2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="1" t="s"/>
       <c r="E2" t="s"/>
       <c r="F2" t="s"/>
       <c r="G2" t="s"/>
@@ -610,10 +610,10 @@
       <c r="B3" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="1" t="s"/>
+      <c r="D3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="1" t="s"/>
       <c r="E3" t="s"/>
       <c r="F3" t="s"/>
       <c r="G3" t="s"/>
@@ -642,10 +642,10 @@
       <c r="B4" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="1" t="s"/>
+      <c r="D4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="1" t="s"/>
       <c r="E4" t="s"/>
       <c r="F4" t="s"/>
       <c r="G4" t="s"/>
@@ -674,10 +674,10 @@
       <c r="B5" s="1" t="n">
         <v>66</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="1" t="s"/>
+      <c r="D5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="1" t="s"/>
       <c r="E5" t="s"/>
       <c r="F5" t="s"/>
       <c r="G5" t="s"/>
@@ -706,10 +706,10 @@
       <c r="B6" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="1" t="s"/>
+      <c r="D6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="1" t="s"/>
       <c r="E6" t="s"/>
       <c r="F6" t="s"/>
       <c r="G6" t="s"/>
@@ -738,10 +738,10 @@
       <c r="B7" s="1" t="n">
         <v>83</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="1" t="s"/>
+      <c r="D7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="1" t="s"/>
       <c r="E7" t="s"/>
       <c r="F7" t="s"/>
       <c r="G7" t="s"/>
@@ -770,10 +770,10 @@
       <c r="B8" s="1" t="n">
         <v>151</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="1" t="s"/>
+      <c r="D8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="1" t="s"/>
       <c r="E8" t="s"/>
       <c r="F8" t="s"/>
       <c r="G8" t="s"/>
@@ -804,10 +804,10 @@
       <c r="B9" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="1" t="s"/>
+      <c r="D9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="1" t="s"/>
       <c r="E9" t="s"/>
       <c r="F9" t="s"/>
       <c r="G9" t="s"/>
@@ -836,10 +836,10 @@
       <c r="B10" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="1" t="s"/>
+      <c r="D10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="1" t="s"/>
       <c r="E10" t="s"/>
       <c r="F10" t="s"/>
       <c r="G10" t="s"/>
@@ -868,10 +868,10 @@
       <c r="B11" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="1" t="s"/>
+      <c r="D11" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="1" t="s"/>
       <c r="E11" t="s"/>
       <c r="F11" t="s"/>
       <c r="G11" t="s"/>
@@ -900,10 +900,10 @@
       <c r="B12" s="1" t="n">
         <v>66</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="1" t="s"/>
+      <c r="D12" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="1" t="s"/>
       <c r="E12" t="s"/>
       <c r="F12" t="s"/>
       <c r="G12" t="s"/>
@@ -932,10 +932,10 @@
       <c r="B13" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="1" t="s"/>
+      <c r="D13" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="1" t="s"/>
       <c r="E13" t="s"/>
       <c r="F13" t="s"/>
       <c r="G13" t="s"/>
@@ -964,10 +964,10 @@
       <c r="B14" s="1" t="n">
         <v>83</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="1" t="s"/>
+      <c r="D14" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="1" t="s"/>
       <c r="E14" t="s"/>
       <c r="F14" t="s"/>
       <c r="G14" t="s"/>
@@ -996,10 +996,10 @@
       <c r="B15" s="1" t="n">
         <v>151</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="1" t="s"/>
+      <c r="D15" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="1" t="s"/>
       <c r="E15" t="s"/>
       <c r="F15" t="s"/>
       <c r="G15" t="s"/>
@@ -1030,10 +1030,10 @@
       <c r="B16" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="1" t="s"/>
+      <c r="D16" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="1" t="s"/>
       <c r="E16" t="s"/>
       <c r="F16" t="s"/>
       <c r="G16" t="s"/>
@@ -1062,10 +1062,10 @@
       <c r="B17" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="1" t="s"/>
+      <c r="D17" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="1" t="s"/>
       <c r="E17" t="s"/>
       <c r="F17" t="s"/>
       <c r="G17" t="s"/>
@@ -1094,10 +1094,10 @@
       <c r="B18" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="1" t="s"/>
+      <c r="D18" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D18" s="1" t="s"/>
       <c r="E18" t="s"/>
       <c r="F18" t="s"/>
       <c r="G18" t="s"/>
@@ -1126,10 +1126,10 @@
       <c r="B19" s="1" t="n">
         <v>66</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="1" t="s"/>
+      <c r="D19" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D19" s="1" t="s"/>
       <c r="E19" t="s"/>
       <c r="F19" t="s"/>
       <c r="G19" t="s"/>
@@ -1158,10 +1158,10 @@
       <c r="B20" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="1" t="s"/>
+      <c r="D20" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D20" s="1" t="s"/>
       <c r="E20" t="s"/>
       <c r="F20" t="s"/>
       <c r="G20" t="s"/>
@@ -1190,10 +1190,10 @@
       <c r="B21" s="1" t="n">
         <v>83</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="1" t="s"/>
+      <c r="D21" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D21" s="1" t="s"/>
       <c r="E21" t="s"/>
       <c r="F21" t="s"/>
       <c r="G21" t="s"/>
@@ -1222,10 +1222,10 @@
       <c r="B22" s="1" t="n">
         <v>151</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="1" t="s"/>
+      <c r="D22" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D22" s="1" t="s"/>
       <c r="E22" t="s"/>
       <c r="F22" t="s"/>
       <c r="G22" t="s"/>
@@ -1256,10 +1256,10 @@
       <c r="B23" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="1" t="s"/>
+      <c r="D23" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D23" s="1" t="s"/>
       <c r="E23" t="s"/>
       <c r="F23" t="s"/>
       <c r="G23" t="s"/>
@@ -1288,10 +1288,10 @@
       <c r="B24" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" s="1" t="s"/>
+      <c r="D24" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D24" s="1" t="s"/>
       <c r="E24" t="s"/>
       <c r="F24" t="s"/>
       <c r="G24" t="s"/>
@@ -1320,10 +1320,10 @@
       <c r="B25" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" s="1" t="s"/>
+      <c r="D25" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D25" s="1" t="s"/>
       <c r="E25" t="s"/>
       <c r="F25" t="s"/>
       <c r="G25" t="s"/>
@@ -1352,10 +1352,10 @@
       <c r="B26" s="1" t="n">
         <v>66</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" s="1" t="s"/>
+      <c r="D26" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D26" s="1" t="s"/>
       <c r="E26" t="s"/>
       <c r="F26" t="s"/>
       <c r="G26" t="s"/>
@@ -1384,10 +1384,10 @@
       <c r="B27" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" s="1" t="s"/>
+      <c r="D27" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D27" s="1" t="s"/>
       <c r="E27" t="s"/>
       <c r="F27" t="s"/>
       <c r="G27" t="s"/>
@@ -1416,10 +1416,10 @@
       <c r="B28" s="1" t="n">
         <v>83</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" s="1" t="s"/>
+      <c r="D28" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D28" s="1" t="s"/>
       <c r="E28" t="s"/>
       <c r="F28" t="s"/>
       <c r="G28" t="s"/>
@@ -1448,10 +1448,10 @@
       <c r="B29" s="1" t="n">
         <v>151</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C29" s="1" t="s"/>
+      <c r="D29" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D29" s="1" t="s"/>
       <c r="E29" t="s"/>
       <c r="F29" t="s"/>
       <c r="G29" t="s"/>
@@ -1482,10 +1482,10 @@
       <c r="B30" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C30" s="1" t="s"/>
+      <c r="D30" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D30" s="1" t="s"/>
       <c r="E30" t="s"/>
       <c r="F30" t="s"/>
       <c r="G30" t="s"/>
@@ -1514,10 +1514,10 @@
       <c r="B31" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" s="1" t="s"/>
+      <c r="D31" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D31" s="1" t="s"/>
       <c r="E31" t="s"/>
       <c r="F31" t="s"/>
       <c r="G31" t="s"/>
@@ -1546,10 +1546,10 @@
       <c r="B32" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" s="1" t="s"/>
+      <c r="D32" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D32" s="1" t="s"/>
       <c r="E32" t="s"/>
       <c r="F32" t="s"/>
       <c r="G32" t="s"/>
@@ -1578,10 +1578,10 @@
       <c r="B33" s="1" t="n">
         <v>66</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C33" s="1" t="s"/>
+      <c r="D33" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D33" s="1" t="s"/>
       <c r="E33" t="s"/>
       <c r="F33" t="s"/>
       <c r="G33" t="s"/>
@@ -1610,10 +1610,10 @@
       <c r="B34" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C34" s="1" t="s"/>
+      <c r="D34" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D34" s="1" t="s"/>
       <c r="E34" t="s"/>
       <c r="F34" t="s"/>
       <c r="G34" t="s"/>
@@ -1642,10 +1642,10 @@
       <c r="B35" s="1" t="n">
         <v>83</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C35" s="1" t="s"/>
+      <c r="D35" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D35" s="1" t="s"/>
       <c r="E35" t="s"/>
       <c r="F35" t="s"/>
       <c r="G35" t="s"/>
@@ -1674,10 +1674,10 @@
       <c r="B36" s="1" t="n">
         <v>151</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C36" s="1" t="s"/>
+      <c r="D36" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D36" s="1" t="s"/>
       <c r="E36" t="s"/>
       <c r="F36" t="s"/>
       <c r="G36" t="s"/>
@@ -1708,10 +1708,10 @@
       <c r="B37" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C37" s="1" t="s"/>
+      <c r="D37" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D37" s="1" t="s"/>
       <c r="E37" t="s"/>
       <c r="F37" t="s"/>
       <c r="G37" t="s"/>
@@ -1740,10 +1740,10 @@
       <c r="B38" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C38" s="1" t="s"/>
+      <c r="D38" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D38" s="1" t="s"/>
       <c r="E38" t="s"/>
       <c r="F38" t="s"/>
       <c r="G38" t="s"/>
@@ -1772,10 +1772,10 @@
       <c r="B39" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C39" s="1" t="s"/>
+      <c r="D39" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D39" s="1" t="s"/>
       <c r="E39" t="s"/>
       <c r="F39" t="s"/>
       <c r="G39" t="s"/>
@@ -1804,10 +1804,10 @@
       <c r="B40" s="1" t="n">
         <v>66</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C40" s="1" t="s"/>
+      <c r="D40" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D40" s="1" t="s"/>
       <c r="E40" t="s"/>
       <c r="F40" t="s"/>
       <c r="G40" t="s"/>
@@ -1836,10 +1836,10 @@
       <c r="B41" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C41" s="1" t="s"/>
+      <c r="D41" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D41" s="1" t="s"/>
       <c r="E41" t="s"/>
       <c r="F41" t="s"/>
       <c r="G41" t="s"/>
@@ -1868,10 +1868,10 @@
       <c r="B42" s="1" t="n">
         <v>83</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C42" s="1" t="s"/>
+      <c r="D42" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D42" s="1" t="s"/>
       <c r="E42" t="s"/>
       <c r="F42" t="s"/>
       <c r="G42" t="s"/>
@@ -1900,10 +1900,10 @@
       <c r="B43" s="1" t="n">
         <v>151</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C43" s="1" t="s"/>
+      <c r="D43" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D43" s="1" t="s"/>
       <c r="E43" t="s"/>
       <c r="F43" t="s"/>
       <c r="G43" t="s"/>
@@ -1934,10 +1934,10 @@
       <c r="B44" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="C44" s="1" t="s"/>
+      <c r="D44" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D44" s="1" t="s"/>
       <c r="E44" t="s"/>
       <c r="F44" t="s"/>
       <c r="G44" t="s"/>
@@ -1966,10 +1966,10 @@
       <c r="B45" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C45" s="1" t="s"/>
+      <c r="D45" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D45" s="1" t="s"/>
       <c r="E45" t="s"/>
       <c r="F45" t="s"/>
       <c r="G45" t="s"/>
@@ -1998,10 +1998,10 @@
       <c r="B46" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C46" s="1" t="s"/>
+      <c r="D46" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D46" s="1" t="s"/>
       <c r="E46" t="s"/>
       <c r="F46" t="s"/>
       <c r="G46" t="s"/>
@@ -2030,10 +2030,10 @@
       <c r="B47" s="1" t="n">
         <v>66</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="C47" s="1" t="s"/>
+      <c r="D47" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D47" s="1" t="s"/>
       <c r="E47" t="s"/>
       <c r="F47" t="s"/>
       <c r="G47" t="s"/>
@@ -2062,10 +2062,10 @@
       <c r="B48" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C48" s="1" t="s"/>
+      <c r="D48" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D48" s="1" t="s"/>
       <c r="E48" t="s"/>
       <c r="F48" t="s"/>
       <c r="G48" t="s"/>
@@ -2094,10 +2094,10 @@
       <c r="B49" s="1" t="n">
         <v>83</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C49" s="1" t="s"/>
+      <c r="D49" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D49" s="1" t="s"/>
       <c r="E49" t="s"/>
       <c r="F49" t="s"/>
       <c r="G49" t="s"/>
@@ -2126,10 +2126,10 @@
       <c r="B50" s="1" t="n">
         <v>151</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C50" s="1" t="s"/>
+      <c r="D50" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D50" s="1" t="s"/>
       <c r="E50" t="s"/>
       <c r="F50" t="s"/>
       <c r="G50" t="s"/>
@@ -2160,10 +2160,10 @@
       <c r="B51" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C51" s="1" t="s"/>
+      <c r="D51" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D51" s="1" t="s"/>
       <c r="E51" t="s"/>
       <c r="F51" t="s"/>
       <c r="G51" t="s"/>
@@ -2192,10 +2192,10 @@
       <c r="B52" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="C52" s="1" t="s"/>
+      <c r="D52" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D52" s="1" t="s"/>
       <c r="E52" t="s"/>
       <c r="F52" t="s"/>
       <c r="G52" t="s"/>
@@ -2224,10 +2224,10 @@
       <c r="B53" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="C53" s="1" t="s"/>
+      <c r="D53" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D53" s="1" t="s"/>
       <c r="E53" t="s"/>
       <c r="F53" t="s"/>
       <c r="G53" t="s"/>
@@ -2256,10 +2256,10 @@
       <c r="B54" s="1" t="n">
         <v>66</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="C54" s="1" t="s"/>
+      <c r="D54" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D54" s="1" t="s"/>
       <c r="E54" t="s"/>
       <c r="F54" t="s"/>
       <c r="G54" t="s"/>
@@ -2288,10 +2288,10 @@
       <c r="B55" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="C55" s="1" t="s"/>
+      <c r="D55" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D55" s="1" t="s"/>
       <c r="E55" t="s"/>
       <c r="F55" t="s"/>
       <c r="G55" t="s"/>
@@ -2320,10 +2320,10 @@
       <c r="B56" s="1" t="n">
         <v>83</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="C56" s="1" t="s"/>
+      <c r="D56" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D56" s="1" t="s"/>
       <c r="E56" t="s"/>
       <c r="F56" t="s"/>
       <c r="G56" t="s"/>
@@ -2352,10 +2352,10 @@
       <c r="B57" s="1" t="n">
         <v>151</v>
       </c>
-      <c r="C57" s="1" t="s">
+      <c r="C57" s="1" t="s"/>
+      <c r="D57" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D57" s="1" t="s"/>
       <c r="E57" t="s"/>
       <c r="F57" t="s"/>
       <c r="G57" t="s"/>
@@ -2386,10 +2386,10 @@
       <c r="B58" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="C58" s="1" t="s"/>
+      <c r="D58" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D58" s="1" t="s"/>
       <c r="E58" t="s"/>
       <c r="F58" t="s"/>
       <c r="G58" t="s"/>
@@ -2418,10 +2418,10 @@
       <c r="B59" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C59" s="1" t="s">
+      <c r="C59" s="1" t="s"/>
+      <c r="D59" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D59" s="1" t="s"/>
       <c r="E59" t="s"/>
       <c r="F59" t="s"/>
       <c r="G59" t="s"/>
@@ -2450,10 +2450,10 @@
       <c r="B60" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="C60" s="1" t="s"/>
+      <c r="D60" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D60" s="1" t="s"/>
       <c r="E60" t="s"/>
       <c r="F60" t="s"/>
       <c r="G60" t="s"/>
@@ -2482,10 +2482,10 @@
       <c r="B61" s="1" t="n">
         <v>66</v>
       </c>
-      <c r="C61" s="1" t="s">
+      <c r="C61" s="1" t="s"/>
+      <c r="D61" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D61" s="1" t="s"/>
       <c r="E61" t="s"/>
       <c r="F61" t="s"/>
       <c r="G61" t="s"/>
@@ -2514,10 +2514,10 @@
       <c r="B62" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="C62" s="1" t="s">
+      <c r="C62" s="1" t="s"/>
+      <c r="D62" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D62" s="1" t="s"/>
       <c r="E62" t="s"/>
       <c r="F62" t="s"/>
       <c r="G62" t="s"/>
@@ -2546,10 +2546,10 @@
       <c r="B63" s="1" t="n">
         <v>83</v>
       </c>
-      <c r="C63" s="1" t="s">
+      <c r="C63" s="1" t="s"/>
+      <c r="D63" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D63" s="1" t="s"/>
       <c r="E63" t="s"/>
       <c r="F63" t="s"/>
       <c r="G63" t="s"/>
@@ -2578,10 +2578,10 @@
       <c r="B64" s="1" t="n">
         <v>151</v>
       </c>
-      <c r="C64" s="1" t="s">
+      <c r="C64" s="1" t="s"/>
+      <c r="D64" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D64" s="1" t="s"/>
       <c r="E64" t="s"/>
       <c r="F64" t="s"/>
       <c r="G64" t="s"/>
@@ -2612,10 +2612,10 @@
       <c r="B65" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C65" s="1" t="s">
+      <c r="C65" s="1" t="s"/>
+      <c r="D65" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D65" s="1" t="s"/>
       <c r="E65" t="s"/>
       <c r="F65" t="s"/>
       <c r="G65" t="s"/>
@@ -2644,10 +2644,10 @@
       <c r="B66" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C66" s="1" t="s">
+      <c r="C66" s="1" t="s"/>
+      <c r="D66" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D66" s="1" t="s"/>
       <c r="E66" t="s"/>
       <c r="F66" t="s"/>
       <c r="G66" t="s"/>
@@ -2676,10 +2676,10 @@
       <c r="B67" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="C67" s="1" t="s">
+      <c r="C67" s="1" t="s"/>
+      <c r="D67" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D67" s="1" t="s"/>
       <c r="E67" t="s"/>
       <c r="F67" t="s"/>
       <c r="G67" t="s"/>
@@ -2708,10 +2708,10 @@
       <c r="B68" s="1" t="n">
         <v>66</v>
       </c>
-      <c r="C68" s="1" t="s">
+      <c r="C68" s="1" t="s"/>
+      <c r="D68" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D68" s="1" t="s"/>
       <c r="E68" t="s"/>
       <c r="F68" t="s"/>
       <c r="G68" t="s"/>
@@ -2740,10 +2740,10 @@
       <c r="B69" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="C69" s="1" t="s">
+      <c r="C69" s="1" t="s"/>
+      <c r="D69" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D69" s="1" t="s"/>
       <c r="E69" t="s"/>
       <c r="F69" t="s"/>
       <c r="G69" t="s"/>
@@ -2772,10 +2772,10 @@
       <c r="B70" s="1" t="n">
         <v>83</v>
       </c>
-      <c r="C70" s="1" t="s">
+      <c r="C70" s="1" t="s"/>
+      <c r="D70" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D70" s="1" t="s"/>
       <c r="E70" t="s"/>
       <c r="F70" t="s"/>
       <c r="G70" t="s"/>
@@ -2804,10 +2804,10 @@
       <c r="B71" s="1" t="n">
         <v>151</v>
       </c>
-      <c r="C71" s="1" t="s">
+      <c r="C71" s="1" t="s"/>
+      <c r="D71" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D71" s="1" t="s"/>
       <c r="E71" t="s"/>
       <c r="F71" t="s"/>
       <c r="G71" t="s"/>
@@ -2838,10 +2838,10 @@
       <c r="B72" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C72" s="1" t="s">
+      <c r="C72" s="1" t="s"/>
+      <c r="D72" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D72" s="1" t="s"/>
       <c r="E72" t="s"/>
       <c r="F72" t="s"/>
       <c r="G72" t="s"/>
@@ -2870,10 +2870,10 @@
       <c r="B73" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C73" s="1" t="s">
+      <c r="C73" s="1" t="s"/>
+      <c r="D73" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D73" s="1" t="s"/>
       <c r="E73" t="s"/>
       <c r="F73" t="s"/>
       <c r="G73" t="s"/>
@@ -2902,10 +2902,10 @@
       <c r="B74" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="C74" s="1" t="s">
+      <c r="C74" s="1" t="s"/>
+      <c r="D74" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D74" s="1" t="s"/>
       <c r="E74" t="s"/>
       <c r="F74" t="s"/>
       <c r="G74" t="s"/>
@@ -2934,10 +2934,10 @@
       <c r="B75" s="1" t="n">
         <v>66</v>
       </c>
-      <c r="C75" s="1" t="s">
+      <c r="C75" s="1" t="s"/>
+      <c r="D75" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D75" s="1" t="s"/>
       <c r="E75" t="s"/>
       <c r="F75" t="s"/>
       <c r="G75" t="s"/>
@@ -2966,10 +2966,10 @@
       <c r="B76" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="C76" s="1" t="s">
+      <c r="C76" s="1" t="s"/>
+      <c r="D76" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D76" s="1" t="s"/>
       <c r="E76" t="s"/>
       <c r="F76" t="s"/>
       <c r="G76" t="s"/>
@@ -2998,10 +2998,10 @@
       <c r="B77" s="1" t="n">
         <v>83</v>
       </c>
-      <c r="C77" s="1" t="s">
+      <c r="C77" s="1" t="s"/>
+      <c r="D77" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D77" s="1" t="s"/>
       <c r="E77" t="s"/>
       <c r="F77" t="s"/>
       <c r="G77" t="s"/>
@@ -3030,10 +3030,10 @@
       <c r="B78" s="1" t="n">
         <v>151</v>
       </c>
-      <c r="C78" s="1" t="s">
+      <c r="C78" s="1" t="s"/>
+      <c r="D78" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D78" s="1" t="s"/>
       <c r="E78" t="s"/>
       <c r="F78" t="s"/>
       <c r="G78" t="s"/>
@@ -3064,10 +3064,10 @@
       <c r="B79" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C79" s="1" t="s">
+      <c r="C79" s="1" t="s"/>
+      <c r="D79" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D79" s="1" t="s"/>
       <c r="E79" t="s"/>
       <c r="F79" t="s"/>
       <c r="G79" t="s"/>
@@ -3096,10 +3096,10 @@
       <c r="B80" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C80" s="1" t="s">
+      <c r="C80" s="1" t="s"/>
+      <c r="D80" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D80" s="1" t="s"/>
       <c r="E80" t="s"/>
       <c r="F80" t="s"/>
       <c r="G80" t="s"/>
@@ -3128,10 +3128,10 @@
       <c r="B81" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="C81" s="1" t="s">
+      <c r="C81" s="1" t="s"/>
+      <c r="D81" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D81" s="1" t="s"/>
       <c r="E81" t="s"/>
       <c r="F81" t="s"/>
       <c r="G81" t="s"/>
@@ -3160,10 +3160,10 @@
       <c r="B82" s="1" t="n">
         <v>66</v>
       </c>
-      <c r="C82" s="1" t="s">
+      <c r="C82" s="1" t="s"/>
+      <c r="D82" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D82" s="1" t="s"/>
       <c r="E82" t="s"/>
       <c r="F82" t="s"/>
       <c r="G82" t="s"/>
@@ -3192,10 +3192,10 @@
       <c r="B83" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="C83" s="1" t="s">
+      <c r="C83" s="1" t="s"/>
+      <c r="D83" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D83" s="1" t="s"/>
       <c r="E83" t="s"/>
       <c r="F83" t="s"/>
       <c r="G83" t="s"/>
@@ -3224,10 +3224,10 @@
       <c r="B84" s="1" t="n">
         <v>83</v>
       </c>
-      <c r="C84" s="1" t="s">
+      <c r="C84" s="1" t="s"/>
+      <c r="D84" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D84" s="1" t="s"/>
       <c r="E84" t="s"/>
       <c r="F84" t="s"/>
       <c r="G84" t="s"/>
@@ -3256,10 +3256,10 @@
       <c r="B85" s="1" t="n">
         <v>151</v>
       </c>
-      <c r="C85" s="1" t="s">
+      <c r="C85" s="1" t="s"/>
+      <c r="D85" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D85" s="1" t="s"/>
       <c r="E85" t="s"/>
       <c r="F85" t="s"/>
       <c r="G85" t="s"/>
@@ -3290,10 +3290,10 @@
       <c r="B86" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C86" s="1" t="s">
+      <c r="C86" s="1" t="s"/>
+      <c r="D86" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D86" s="1" t="s"/>
       <c r="E86" t="s"/>
       <c r="F86" t="s"/>
       <c r="G86" t="s"/>
@@ -3322,10 +3322,10 @@
       <c r="B87" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C87" s="1" t="s">
+      <c r="C87" s="1" t="s"/>
+      <c r="D87" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D87" s="1" t="s"/>
       <c r="E87" t="s"/>
       <c r="F87" t="s"/>
       <c r="G87" t="s"/>
@@ -3354,10 +3354,10 @@
       <c r="B88" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="C88" s="1" t="s">
+      <c r="C88" s="1" t="s"/>
+      <c r="D88" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D88" s="1" t="s"/>
       <c r="E88" t="s"/>
       <c r="F88" t="s"/>
       <c r="G88" t="s"/>
@@ -3386,10 +3386,10 @@
       <c r="B89" s="1" t="n">
         <v>66</v>
       </c>
-      <c r="C89" s="1" t="s">
+      <c r="C89" s="1" t="s"/>
+      <c r="D89" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D89" s="1" t="s"/>
       <c r="E89" t="s"/>
       <c r="F89" t="s"/>
       <c r="G89" t="s"/>
@@ -3418,10 +3418,10 @@
       <c r="B90" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="C90" s="1" t="s">
+      <c r="C90" s="1" t="s"/>
+      <c r="D90" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D90" s="1" t="s"/>
       <c r="E90" t="s"/>
       <c r="F90" t="s"/>
       <c r="G90" t="s"/>
@@ -3450,10 +3450,10 @@
       <c r="B91" s="1" t="n">
         <v>83</v>
       </c>
-      <c r="C91" s="1" t="s">
+      <c r="C91" s="1" t="s"/>
+      <c r="D91" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D91" s="1" t="s"/>
       <c r="E91" t="s"/>
       <c r="F91" t="s"/>
       <c r="G91" t="s"/>
@@ -3482,10 +3482,10 @@
       <c r="B92" s="1" t="n">
         <v>151</v>
       </c>
-      <c r="C92" s="1" t="s">
+      <c r="C92" s="1" t="s"/>
+      <c r="D92" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D92" s="1" t="s"/>
       <c r="E92" t="s"/>
       <c r="F92" t="s"/>
       <c r="G92" t="s"/>
@@ -3516,10 +3516,10 @@
       <c r="B93" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C93" s="1" t="s">
+      <c r="C93" s="1" t="s"/>
+      <c r="D93" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D93" s="1" t="s"/>
       <c r="E93" t="s"/>
       <c r="F93" t="s"/>
       <c r="G93" t="s"/>
@@ -3548,10 +3548,10 @@
       <c r="B94" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C94" s="1" t="s">
+      <c r="C94" s="1" t="s"/>
+      <c r="D94" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D94" s="1" t="s"/>
       <c r="E94" t="s"/>
       <c r="F94" t="s"/>
       <c r="G94" t="s"/>
@@ -3580,10 +3580,10 @@
       <c r="B95" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="C95" s="1" t="s">
+      <c r="C95" s="1" t="s"/>
+      <c r="D95" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D95" s="1" t="s"/>
       <c r="E95" t="s"/>
       <c r="F95" t="s"/>
       <c r="G95" t="s"/>
@@ -3612,10 +3612,10 @@
       <c r="B96" s="1" t="n">
         <v>66</v>
       </c>
-      <c r="C96" s="1" t="s">
+      <c r="C96" s="1" t="s"/>
+      <c r="D96" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D96" s="1" t="s"/>
       <c r="E96" t="s"/>
       <c r="F96" t="s"/>
       <c r="G96" t="s"/>
@@ -3644,10 +3644,10 @@
       <c r="B97" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="C97" s="1" t="s">
+      <c r="C97" s="1" t="s"/>
+      <c r="D97" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D97" s="1" t="s"/>
       <c r="E97" t="s"/>
       <c r="F97" t="s"/>
       <c r="G97" t="s"/>
@@ -3676,10 +3676,10 @@
       <c r="B98" s="1" t="n">
         <v>83</v>
       </c>
-      <c r="C98" s="1" t="s">
+      <c r="C98" s="1" t="s"/>
+      <c r="D98" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D98" s="1" t="s"/>
       <c r="E98" t="s"/>
       <c r="F98" t="s"/>
       <c r="G98" t="s"/>
@@ -3708,10 +3708,10 @@
       <c r="B99" s="1" t="n">
         <v>151</v>
       </c>
-      <c r="C99" s="1" t="s">
+      <c r="C99" s="1" t="s"/>
+      <c r="D99" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D99" s="1" t="s"/>
       <c r="E99" t="s"/>
       <c r="F99" t="s"/>
       <c r="G99" t="s"/>
@@ -3742,10 +3742,10 @@
       <c r="B100" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C100" s="1" t="s">
+      <c r="C100" s="1" t="s"/>
+      <c r="D100" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D100" s="1" t="s"/>
       <c r="E100" t="s"/>
       <c r="F100" t="s"/>
       <c r="G100" t="s"/>
@@ -3774,10 +3774,10 @@
       <c r="B101" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C101" s="1" t="s">
+      <c r="C101" s="1" t="s"/>
+      <c r="D101" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D101" s="1" t="s"/>
       <c r="E101" t="s"/>
       <c r="F101" t="s"/>
       <c r="G101" t="s"/>
@@ -3806,10 +3806,10 @@
       <c r="B102" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="C102" s="1" t="s">
+      <c r="C102" s="1" t="s"/>
+      <c r="D102" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D102" s="1" t="s"/>
       <c r="E102" t="s"/>
       <c r="F102" t="s"/>
       <c r="G102" t="s"/>
@@ -3838,10 +3838,10 @@
       <c r="B103" s="1" t="n">
         <v>66</v>
       </c>
-      <c r="C103" s="1" t="s">
+      <c r="C103" s="1" t="s"/>
+      <c r="D103" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D103" s="1" t="s"/>
       <c r="E103" t="s"/>
       <c r="F103" t="s"/>
       <c r="G103" t="s"/>
@@ -3870,10 +3870,10 @@
       <c r="B104" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="C104" s="1" t="s">
+      <c r="C104" s="1" t="s"/>
+      <c r="D104" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D104" s="1" t="s"/>
       <c r="E104" t="s"/>
       <c r="F104" t="s"/>
       <c r="G104" t="s"/>
@@ -3902,10 +3902,10 @@
       <c r="B105" s="1" t="n">
         <v>83</v>
       </c>
-      <c r="C105" s="1" t="s">
+      <c r="C105" s="1" t="s"/>
+      <c r="D105" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D105" s="1" t="s"/>
       <c r="E105" t="s"/>
       <c r="F105" t="s"/>
       <c r="G105" t="s"/>
@@ -3934,10 +3934,10 @@
       <c r="B106" s="1" t="n">
         <v>151</v>
       </c>
-      <c r="C106" s="1" t="s">
+      <c r="C106" s="1" t="s"/>
+      <c r="D106" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D106" s="1" t="s"/>
       <c r="E106" t="s"/>
       <c r="F106" t="s"/>
       <c r="G106" t="s"/>
@@ -3968,10 +3968,10 @@
       <c r="B107" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C107" s="1" t="s">
+      <c r="C107" s="1" t="s"/>
+      <c r="D107" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D107" s="1" t="s"/>
       <c r="E107" t="s"/>
       <c r="F107" t="s"/>
       <c r="G107" t="s"/>
@@ -4000,10 +4000,10 @@
       <c r="B108" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C108" s="1" t="s">
+      <c r="C108" s="1" t="s"/>
+      <c r="D108" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D108" s="1" t="s"/>
       <c r="E108" t="s"/>
       <c r="F108" t="s"/>
       <c r="G108" t="s"/>
@@ -4032,10 +4032,10 @@
       <c r="B109" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="C109" s="1" t="s">
+      <c r="C109" s="1" t="s"/>
+      <c r="D109" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D109" s="1" t="s"/>
       <c r="E109" t="s"/>
       <c r="F109" t="s"/>
       <c r="G109" t="s"/>
@@ -4064,10 +4064,10 @@
       <c r="B110" s="1" t="n">
         <v>66</v>
       </c>
-      <c r="C110" s="1" t="s">
+      <c r="C110" s="1" t="s"/>
+      <c r="D110" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D110" s="1" t="s"/>
       <c r="E110" t="s"/>
       <c r="F110" t="s"/>
       <c r="G110" t="s"/>
@@ -4096,10 +4096,10 @@
       <c r="B111" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="C111" s="1" t="s">
+      <c r="C111" s="1" t="s"/>
+      <c r="D111" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D111" s="1" t="s"/>
       <c r="E111" t="s"/>
       <c r="F111" t="s"/>
       <c r="G111" t="s"/>
@@ -4128,10 +4128,10 @@
       <c r="B112" s="1" t="n">
         <v>83</v>
       </c>
-      <c r="C112" s="1" t="s">
+      <c r="C112" s="1" t="s"/>
+      <c r="D112" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D112" s="1" t="s"/>
       <c r="E112" t="s"/>
       <c r="F112" t="s"/>
       <c r="G112" t="s"/>
@@ -4160,10 +4160,10 @@
       <c r="B113" s="1" t="n">
         <v>151</v>
       </c>
-      <c r="C113" s="1" t="s">
+      <c r="C113" s="1" t="s"/>
+      <c r="D113" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D113" s="1" t="s"/>
       <c r="E113" t="s"/>
       <c r="F113" t="s"/>
       <c r="G113" t="s"/>
@@ -4194,10 +4194,10 @@
       <c r="B114" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C114" s="1" t="s">
+      <c r="C114" s="1" t="s"/>
+      <c r="D114" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D114" s="1" t="s"/>
       <c r="E114" t="s"/>
       <c r="F114" t="s"/>
       <c r="G114" t="s"/>
@@ -4226,10 +4226,10 @@
       <c r="B115" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C115" s="1" t="s">
+      <c r="C115" s="1" t="s"/>
+      <c r="D115" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D115" s="1" t="s"/>
       <c r="E115" t="s"/>
       <c r="F115" t="s"/>
       <c r="G115" t="s"/>
@@ -4258,10 +4258,10 @@
       <c r="B116" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="C116" s="1" t="s">
+      <c r="C116" s="1" t="s"/>
+      <c r="D116" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D116" s="1" t="s"/>
       <c r="E116" t="s"/>
       <c r="F116" t="s"/>
       <c r="G116" t="s"/>
@@ -4290,10 +4290,10 @@
       <c r="B117" s="1" t="n">
         <v>66</v>
       </c>
-      <c r="C117" s="1" t="s">
+      <c r="C117" s="1" t="s"/>
+      <c r="D117" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D117" s="1" t="s"/>
       <c r="E117" t="s"/>
       <c r="F117" t="s"/>
       <c r="G117" t="s"/>
@@ -4322,10 +4322,10 @@
       <c r="B118" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="C118" s="1" t="s">
+      <c r="C118" s="1" t="s"/>
+      <c r="D118" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D118" s="1" t="s"/>
       <c r="E118" t="s"/>
       <c r="F118" t="s"/>
       <c r="G118" t="s"/>
@@ -4354,10 +4354,10 @@
       <c r="B119" s="1" t="n">
         <v>83</v>
       </c>
-      <c r="C119" s="1" t="s">
+      <c r="C119" s="1" t="s"/>
+      <c r="D119" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D119" s="1" t="s"/>
       <c r="E119" t="s"/>
       <c r="F119" t="s"/>
       <c r="G119" t="s"/>
@@ -4386,10 +4386,10 @@
       <c r="B120" s="1" t="n">
         <v>151</v>
       </c>
-      <c r="C120" s="1" t="s">
+      <c r="C120" s="1" t="s"/>
+      <c r="D120" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D120" s="1" t="s"/>
       <c r="E120" t="s"/>
       <c r="F120" t="s"/>
       <c r="G120" t="s"/>
@@ -4420,10 +4420,10 @@
       <c r="B121" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C121" s="1" t="s">
+      <c r="C121" s="1" t="s"/>
+      <c r="D121" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D121" s="1" t="s"/>
       <c r="E121" t="s"/>
       <c r="F121" t="s"/>
       <c r="G121" t="s"/>
@@ -4452,10 +4452,10 @@
       <c r="B122" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C122" s="1" t="s">
+      <c r="C122" s="1" t="s"/>
+      <c r="D122" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D122" s="1" t="s"/>
       <c r="E122" t="s"/>
       <c r="F122" t="s"/>
       <c r="G122" t="s"/>
@@ -4484,10 +4484,10 @@
       <c r="B123" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="C123" s="1" t="s">
+      <c r="C123" s="1" t="s"/>
+      <c r="D123" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D123" s="1" t="s"/>
       <c r="E123" t="s"/>
       <c r="F123" t="s"/>
       <c r="G123" t="s"/>
@@ -4516,10 +4516,10 @@
       <c r="B124" s="1" t="n">
         <v>66</v>
       </c>
-      <c r="C124" s="1" t="s">
+      <c r="C124" s="1" t="s"/>
+      <c r="D124" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D124" s="1" t="s"/>
       <c r="E124" t="s"/>
       <c r="F124" t="s"/>
       <c r="G124" t="s"/>
@@ -4548,10 +4548,10 @@
       <c r="B125" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="C125" s="1" t="s">
+      <c r="C125" s="1" t="s"/>
+      <c r="D125" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D125" s="1" t="s"/>
       <c r="E125" t="s"/>
       <c r="F125" t="s"/>
       <c r="G125" t="s"/>
@@ -4580,10 +4580,10 @@
       <c r="B126" s="1" t="n">
         <v>83</v>
       </c>
-      <c r="C126" s="1" t="s">
+      <c r="C126" s="1" t="s"/>
+      <c r="D126" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D126" s="1" t="s"/>
       <c r="E126" t="s"/>
       <c r="F126" t="s"/>
       <c r="G126" t="s"/>
@@ -4612,10 +4612,10 @@
       <c r="B127" s="1" t="n">
         <v>151</v>
       </c>
-      <c r="C127" s="1" t="s">
+      <c r="C127" s="1" t="s"/>
+      <c r="D127" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D127" s="1" t="s"/>
       <c r="E127" t="s"/>
       <c r="F127" t="s"/>
       <c r="G127" t="s"/>
@@ -4753,10 +4753,10 @@
       <c r="B2" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="1" t="s"/>
+      <c r="D2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="1" t="s"/>
       <c r="E2" t="s"/>
       <c r="F2" t="s"/>
       <c r="G2" t="s"/>
@@ -4785,10 +4785,10 @@
       <c r="B3" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="1" t="s"/>
+      <c r="D3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="1" t="s"/>
       <c r="E3" t="s"/>
       <c r="F3" t="s"/>
       <c r="G3" t="s"/>
@@ -4817,10 +4817,10 @@
       <c r="B4" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="1" t="s"/>
+      <c r="D4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="1" t="s"/>
       <c r="E4" t="s"/>
       <c r="F4" t="s"/>
       <c r="G4" t="s"/>
@@ -4849,10 +4849,10 @@
       <c r="B5" s="1" t="n">
         <v>66</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="1" t="s"/>
+      <c r="D5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="1" t="s"/>
       <c r="E5" t="s"/>
       <c r="F5" t="s"/>
       <c r="G5" t="s"/>
@@ -4881,10 +4881,10 @@
       <c r="B6" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="1" t="s"/>
+      <c r="D6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="1" t="s"/>
       <c r="E6" t="s"/>
       <c r="F6" t="s"/>
       <c r="G6" t="s"/>
@@ -4913,10 +4913,10 @@
       <c r="B7" s="1" t="n">
         <v>83</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="1" t="s"/>
+      <c r="D7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="1" t="s"/>
       <c r="E7" t="s"/>
       <c r="F7" t="s"/>
       <c r="G7" t="s"/>
@@ -4945,10 +4945,10 @@
       <c r="B8" s="1" t="n">
         <v>151</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="1" t="s"/>
+      <c r="D8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="1" t="s"/>
       <c r="E8" t="s"/>
       <c r="F8" t="s"/>
       <c r="G8" t="s"/>
@@ -4979,10 +4979,10 @@
       <c r="B9" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="1" t="s"/>
+      <c r="D9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="1" t="s"/>
       <c r="E9" t="s"/>
       <c r="F9" t="s"/>
       <c r="G9" t="s"/>
@@ -5011,10 +5011,10 @@
       <c r="B10" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="1" t="s"/>
+      <c r="D10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="1" t="s"/>
       <c r="E10" t="s"/>
       <c r="F10" t="s"/>
       <c r="G10" t="s"/>
@@ -5043,10 +5043,10 @@
       <c r="B11" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="1" t="s"/>
+      <c r="D11" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="1" t="s"/>
       <c r="E11" t="s"/>
       <c r="F11" t="s"/>
       <c r="G11" t="s"/>
@@ -5075,10 +5075,10 @@
       <c r="B12" s="1" t="n">
         <v>66</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="1" t="s"/>
+      <c r="D12" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="1" t="s"/>
       <c r="E12" t="s"/>
       <c r="F12" t="s"/>
       <c r="G12" t="s"/>
@@ -5107,10 +5107,10 @@
       <c r="B13" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="1" t="s"/>
+      <c r="D13" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="1" t="s"/>
       <c r="E13" t="s"/>
       <c r="F13" t="s"/>
       <c r="G13" t="s"/>
@@ -5139,10 +5139,10 @@
       <c r="B14" s="1" t="n">
         <v>83</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="1" t="s"/>
+      <c r="D14" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="1" t="s"/>
       <c r="E14" t="s"/>
       <c r="F14" t="s"/>
       <c r="G14" t="s"/>
@@ -5171,10 +5171,10 @@
       <c r="B15" s="1" t="n">
         <v>151</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="1" t="s"/>
+      <c r="D15" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="1" t="s"/>
       <c r="E15" t="s"/>
       <c r="F15" t="s"/>
       <c r="G15" t="s"/>
@@ -5205,10 +5205,10 @@
       <c r="B16" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="1" t="s"/>
+      <c r="D16" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="1" t="s"/>
       <c r="E16" t="s"/>
       <c r="F16" t="s"/>
       <c r="G16" t="s"/>
@@ -5237,10 +5237,10 @@
       <c r="B17" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="1" t="s"/>
+      <c r="D17" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="1" t="s"/>
       <c r="E17" t="s"/>
       <c r="F17" t="s"/>
       <c r="G17" t="s"/>
@@ -5269,10 +5269,10 @@
       <c r="B18" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="1" t="s"/>
+      <c r="D18" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D18" s="1" t="s"/>
       <c r="E18" t="s"/>
       <c r="F18" t="s"/>
       <c r="G18" t="s"/>
@@ -5301,10 +5301,10 @@
       <c r="B19" s="1" t="n">
         <v>66</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="1" t="s"/>
+      <c r="D19" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D19" s="1" t="s"/>
       <c r="E19" t="s"/>
       <c r="F19" t="s"/>
       <c r="G19" t="s"/>
@@ -5333,10 +5333,10 @@
       <c r="B20" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="1" t="s"/>
+      <c r="D20" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D20" s="1" t="s"/>
       <c r="E20" t="s"/>
       <c r="F20" t="s"/>
       <c r="G20" t="s"/>
@@ -5365,10 +5365,10 @@
       <c r="B21" s="1" t="n">
         <v>83</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="1" t="s"/>
+      <c r="D21" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D21" s="1" t="s"/>
       <c r="E21" t="s"/>
       <c r="F21" t="s"/>
       <c r="G21" t="s"/>
@@ -5397,10 +5397,10 @@
       <c r="B22" s="1" t="n">
         <v>151</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="1" t="s"/>
+      <c r="D22" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D22" s="1" t="s"/>
       <c r="E22" t="s"/>
       <c r="F22" t="s"/>
       <c r="G22" t="s"/>
@@ -5431,10 +5431,10 @@
       <c r="B23" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="1" t="s"/>
+      <c r="D23" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D23" s="1" t="s"/>
       <c r="E23" t="s"/>
       <c r="F23" t="s"/>
       <c r="G23" t="s"/>
@@ -5463,10 +5463,10 @@
       <c r="B24" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" s="1" t="s"/>
+      <c r="D24" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D24" s="1" t="s"/>
       <c r="E24" t="s"/>
       <c r="F24" t="s"/>
       <c r="G24" t="s"/>
@@ -5495,10 +5495,10 @@
       <c r="B25" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" s="1" t="s"/>
+      <c r="D25" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D25" s="1" t="s"/>
       <c r="E25" t="s"/>
       <c r="F25" t="s"/>
       <c r="G25" t="s"/>
@@ -5527,10 +5527,10 @@
       <c r="B26" s="1" t="n">
         <v>66</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" s="1" t="s"/>
+      <c r="D26" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D26" s="1" t="s"/>
       <c r="E26" t="s"/>
       <c r="F26" t="s"/>
       <c r="G26" t="s"/>
@@ -5559,10 +5559,10 @@
       <c r="B27" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" s="1" t="s"/>
+      <c r="D27" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D27" s="1" t="s"/>
       <c r="E27" t="s"/>
       <c r="F27" t="s"/>
       <c r="G27" t="s"/>
@@ -5591,10 +5591,10 @@
       <c r="B28" s="1" t="n">
         <v>83</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" s="1" t="s"/>
+      <c r="D28" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D28" s="1" t="s"/>
       <c r="E28" t="s"/>
       <c r="F28" t="s"/>
       <c r="G28" t="s"/>
@@ -5623,10 +5623,10 @@
       <c r="B29" s="1" t="n">
         <v>151</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C29" s="1" t="s"/>
+      <c r="D29" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D29" s="1" t="s"/>
       <c r="E29" t="s"/>
       <c r="F29" t="s"/>
       <c r="G29" t="s"/>
@@ -5657,10 +5657,10 @@
       <c r="B30" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C30" s="1" t="s"/>
+      <c r="D30" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D30" s="1" t="s"/>
       <c r="E30" t="s"/>
       <c r="F30" t="s"/>
       <c r="G30" t="s"/>
@@ -5689,10 +5689,10 @@
       <c r="B31" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" s="1" t="s"/>
+      <c r="D31" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D31" s="1" t="s"/>
       <c r="E31" t="s"/>
       <c r="F31" t="s"/>
       <c r="G31" t="s"/>
@@ -5721,10 +5721,10 @@
       <c r="B32" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" s="1" t="s"/>
+      <c r="D32" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D32" s="1" t="s"/>
       <c r="E32" t="s"/>
       <c r="F32" t="s"/>
       <c r="G32" t="s"/>
@@ -5753,10 +5753,10 @@
       <c r="B33" s="1" t="n">
         <v>66</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C33" s="1" t="s"/>
+      <c r="D33" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D33" s="1" t="s"/>
       <c r="E33" t="s"/>
       <c r="F33" t="s"/>
       <c r="G33" t="s"/>
@@ -5785,10 +5785,10 @@
       <c r="B34" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C34" s="1" t="s"/>
+      <c r="D34" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D34" s="1" t="s"/>
       <c r="E34" t="s"/>
       <c r="F34" t="s"/>
       <c r="G34" t="s"/>
@@ -5817,10 +5817,10 @@
       <c r="B35" s="1" t="n">
         <v>83</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C35" s="1" t="s"/>
+      <c r="D35" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D35" s="1" t="s"/>
       <c r="E35" t="s"/>
       <c r="F35" t="s"/>
       <c r="G35" t="s"/>
@@ -5849,10 +5849,10 @@
       <c r="B36" s="1" t="n">
         <v>151</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C36" s="1" t="s"/>
+      <c r="D36" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D36" s="1" t="s"/>
       <c r="E36" t="s"/>
       <c r="F36" t="s"/>
       <c r="G36" t="s"/>
@@ -5883,10 +5883,10 @@
       <c r="B37" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C37" s="1" t="s"/>
+      <c r="D37" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D37" s="1" t="s"/>
       <c r="E37" t="s"/>
       <c r="F37" t="s"/>
       <c r="G37" t="s"/>
@@ -5915,10 +5915,10 @@
       <c r="B38" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C38" s="1" t="s"/>
+      <c r="D38" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D38" s="1" t="s"/>
       <c r="E38" t="s"/>
       <c r="F38" t="s"/>
       <c r="G38" t="s"/>
@@ -5947,10 +5947,10 @@
       <c r="B39" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C39" s="1" t="s"/>
+      <c r="D39" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D39" s="1" t="s"/>
       <c r="E39" t="s"/>
       <c r="F39" t="s"/>
       <c r="G39" t="s"/>
@@ -5979,10 +5979,10 @@
       <c r="B40" s="1" t="n">
         <v>66</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C40" s="1" t="s"/>
+      <c r="D40" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D40" s="1" t="s"/>
       <c r="E40" t="s"/>
       <c r="F40" t="s"/>
       <c r="G40" t="s"/>
@@ -6011,10 +6011,10 @@
       <c r="B41" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C41" s="1" t="s"/>
+      <c r="D41" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D41" s="1" t="s"/>
       <c r="E41" t="s"/>
       <c r="F41" t="s"/>
       <c r="G41" t="s"/>
@@ -6043,10 +6043,10 @@
       <c r="B42" s="1" t="n">
         <v>83</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C42" s="1" t="s"/>
+      <c r="D42" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D42" s="1" t="s"/>
       <c r="E42" t="s"/>
       <c r="F42" t="s"/>
       <c r="G42" t="s"/>
@@ -6075,10 +6075,10 @@
       <c r="B43" s="1" t="n">
         <v>151</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C43" s="1" t="s"/>
+      <c r="D43" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D43" s="1" t="s"/>
       <c r="E43" t="s"/>
       <c r="F43" t="s"/>
       <c r="G43" t="s"/>
@@ -6109,10 +6109,10 @@
       <c r="B44" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="C44" s="1" t="s"/>
+      <c r="D44" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D44" s="1" t="s"/>
       <c r="E44" t="s"/>
       <c r="F44" t="s"/>
       <c r="G44" t="s"/>
@@ -6141,10 +6141,10 @@
       <c r="B45" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C45" s="1" t="s"/>
+      <c r="D45" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D45" s="1" t="s"/>
       <c r="E45" t="s"/>
       <c r="F45" t="s"/>
       <c r="G45" t="s"/>
@@ -6173,10 +6173,10 @@
       <c r="B46" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C46" s="1" t="s"/>
+      <c r="D46" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D46" s="1" t="s"/>
       <c r="E46" t="s"/>
       <c r="F46" t="s"/>
       <c r="G46" t="s"/>
@@ -6205,10 +6205,10 @@
       <c r="B47" s="1" t="n">
         <v>66</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="C47" s="1" t="s"/>
+      <c r="D47" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D47" s="1" t="s"/>
       <c r="E47" t="s"/>
       <c r="F47" t="s"/>
       <c r="G47" t="s"/>
@@ -6237,10 +6237,10 @@
       <c r="B48" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C48" s="1" t="s"/>
+      <c r="D48" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D48" s="1" t="s"/>
       <c r="E48" t="s"/>
       <c r="F48" t="s"/>
       <c r="G48" t="s"/>
@@ -6269,10 +6269,10 @@
       <c r="B49" s="1" t="n">
         <v>83</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C49" s="1" t="s"/>
+      <c r="D49" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D49" s="1" t="s"/>
       <c r="E49" t="s"/>
       <c r="F49" t="s"/>
       <c r="G49" t="s"/>
@@ -6301,10 +6301,10 @@
       <c r="B50" s="1" t="n">
         <v>151</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C50" s="1" t="s"/>
+      <c r="D50" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D50" s="1" t="s"/>
       <c r="E50" t="s"/>
       <c r="F50" t="s"/>
       <c r="G50" t="s"/>
@@ -6335,10 +6335,10 @@
       <c r="B51" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C51" s="1" t="s"/>
+      <c r="D51" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D51" s="1" t="s"/>
       <c r="E51" t="s"/>
       <c r="F51" t="s"/>
       <c r="G51" t="s"/>
@@ -6367,10 +6367,10 @@
       <c r="B52" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="C52" s="1" t="s"/>
+      <c r="D52" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D52" s="1" t="s"/>
       <c r="E52" t="s"/>
       <c r="F52" t="s"/>
       <c r="G52" t="s"/>
@@ -6399,10 +6399,10 @@
       <c r="B53" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="C53" s="1" t="s"/>
+      <c r="D53" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D53" s="1" t="s"/>
       <c r="E53" t="s"/>
       <c r="F53" t="s"/>
       <c r="G53" t="s"/>
@@ -6431,10 +6431,10 @@
       <c r="B54" s="1" t="n">
         <v>66</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="C54" s="1" t="s"/>
+      <c r="D54" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D54" s="1" t="s"/>
       <c r="E54" t="s"/>
       <c r="F54" t="s"/>
       <c r="G54" t="s"/>
@@ -6463,10 +6463,10 @@
       <c r="B55" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="C55" s="1" t="s"/>
+      <c r="D55" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D55" s="1" t="s"/>
       <c r="E55" t="s"/>
       <c r="F55" t="s"/>
       <c r="G55" t="s"/>
@@ -6495,10 +6495,10 @@
       <c r="B56" s="1" t="n">
         <v>83</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="C56" s="1" t="s"/>
+      <c r="D56" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D56" s="1" t="s"/>
       <c r="E56" t="s"/>
       <c r="F56" t="s"/>
       <c r="G56" t="s"/>
@@ -6527,10 +6527,10 @@
       <c r="B57" s="1" t="n">
         <v>151</v>
       </c>
-      <c r="C57" s="1" t="s">
+      <c r="C57" s="1" t="s"/>
+      <c r="D57" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D57" s="1" t="s"/>
       <c r="E57" t="s"/>
       <c r="F57" t="s"/>
       <c r="G57" t="s"/>
@@ -6561,10 +6561,10 @@
       <c r="B58" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="C58" s="1" t="s"/>
+      <c r="D58" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D58" s="1" t="s"/>
       <c r="E58" t="s"/>
       <c r="F58" t="s"/>
       <c r="G58" t="s"/>
@@ -6593,10 +6593,10 @@
       <c r="B59" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C59" s="1" t="s">
+      <c r="C59" s="1" t="s"/>
+      <c r="D59" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D59" s="1" t="s"/>
       <c r="E59" t="s"/>
       <c r="F59" t="s"/>
       <c r="G59" t="s"/>
@@ -6625,10 +6625,10 @@
       <c r="B60" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="C60" s="1" t="s"/>
+      <c r="D60" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D60" s="1" t="s"/>
       <c r="E60" t="s"/>
       <c r="F60" t="s"/>
       <c r="G60" t="s"/>
@@ -6657,10 +6657,10 @@
       <c r="B61" s="1" t="n">
         <v>66</v>
       </c>
-      <c r="C61" s="1" t="s">
+      <c r="C61" s="1" t="s"/>
+      <c r="D61" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D61" s="1" t="s"/>
       <c r="E61" t="s"/>
       <c r="F61" t="s"/>
       <c r="G61" t="s"/>
@@ -6689,10 +6689,10 @@
       <c r="B62" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="C62" s="1" t="s">
+      <c r="C62" s="1" t="s"/>
+      <c r="D62" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D62" s="1" t="s"/>
       <c r="E62" t="s"/>
       <c r="F62" t="s"/>
       <c r="G62" t="s"/>
@@ -6721,10 +6721,10 @@
       <c r="B63" s="1" t="n">
         <v>83</v>
       </c>
-      <c r="C63" s="1" t="s">
+      <c r="C63" s="1" t="s"/>
+      <c r="D63" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D63" s="1" t="s"/>
       <c r="E63" t="s"/>
       <c r="F63" t="s"/>
       <c r="G63" t="s"/>
@@ -6753,10 +6753,10 @@
       <c r="B64" s="1" t="n">
         <v>151</v>
       </c>
-      <c r="C64" s="1" t="s">
+      <c r="C64" s="1" t="s"/>
+      <c r="D64" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D64" s="1" t="s"/>
       <c r="E64" t="s"/>
       <c r="F64" t="s"/>
       <c r="G64" t="s"/>
@@ -6787,10 +6787,10 @@
       <c r="B65" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C65" s="1" t="s">
+      <c r="C65" s="1" t="s"/>
+      <c r="D65" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D65" s="1" t="s"/>
       <c r="E65" t="s"/>
       <c r="F65" t="s"/>
       <c r="G65" t="s"/>
@@ -6819,10 +6819,10 @@
       <c r="B66" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C66" s="1" t="s">
+      <c r="C66" s="1" t="s"/>
+      <c r="D66" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D66" s="1" t="s"/>
       <c r="E66" t="s"/>
       <c r="F66" t="s"/>
       <c r="G66" t="s"/>
@@ -6851,10 +6851,10 @@
       <c r="B67" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="C67" s="1" t="s">
+      <c r="C67" s="1" t="s"/>
+      <c r="D67" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D67" s="1" t="s"/>
       <c r="E67" t="s"/>
       <c r="F67" t="s"/>
       <c r="G67" t="s"/>
@@ -6883,10 +6883,10 @@
       <c r="B68" s="1" t="n">
         <v>66</v>
       </c>
-      <c r="C68" s="1" t="s">
+      <c r="C68" s="1" t="s"/>
+      <c r="D68" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D68" s="1" t="s"/>
       <c r="E68" t="s"/>
       <c r="F68" t="s"/>
       <c r="G68" t="s"/>
@@ -6915,10 +6915,10 @@
       <c r="B69" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="C69" s="1" t="s">
+      <c r="C69" s="1" t="s"/>
+      <c r="D69" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D69" s="1" t="s"/>
       <c r="E69" t="s"/>
       <c r="F69" t="s"/>
       <c r="G69" t="s"/>
@@ -6947,10 +6947,10 @@
       <c r="B70" s="1" t="n">
         <v>83</v>
       </c>
-      <c r="C70" s="1" t="s">
+      <c r="C70" s="1" t="s"/>
+      <c r="D70" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D70" s="1" t="s"/>
       <c r="E70" t="s"/>
       <c r="F70" t="s"/>
       <c r="G70" t="s"/>
@@ -6979,10 +6979,10 @@
       <c r="B71" s="1" t="n">
         <v>151</v>
       </c>
-      <c r="C71" s="1" t="s">
+      <c r="C71" s="1" t="s"/>
+      <c r="D71" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D71" s="1" t="s"/>
       <c r="E71" t="s"/>
       <c r="F71" t="s"/>
       <c r="G71" t="s"/>
@@ -7013,10 +7013,10 @@
       <c r="B72" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C72" s="1" t="s">
+      <c r="C72" s="1" t="s"/>
+      <c r="D72" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D72" s="1" t="s"/>
       <c r="E72" t="s"/>
       <c r="F72" t="s"/>
       <c r="G72" t="s"/>
@@ -7045,10 +7045,10 @@
       <c r="B73" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C73" s="1" t="s">
+      <c r="C73" s="1" t="s"/>
+      <c r="D73" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D73" s="1" t="s"/>
       <c r="E73" t="s"/>
       <c r="F73" t="s"/>
       <c r="G73" t="s"/>
@@ -7077,10 +7077,10 @@
       <c r="B74" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="C74" s="1" t="s">
+      <c r="C74" s="1" t="s"/>
+      <c r="D74" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D74" s="1" t="s"/>
       <c r="E74" t="s"/>
       <c r="F74" t="s"/>
       <c r="G74" t="s"/>
@@ -7109,10 +7109,10 @@
       <c r="B75" s="1" t="n">
         <v>66</v>
       </c>
-      <c r="C75" s="1" t="s">
+      <c r="C75" s="1" t="s"/>
+      <c r="D75" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D75" s="1" t="s"/>
       <c r="E75" t="s"/>
       <c r="F75" t="s"/>
       <c r="G75" t="s"/>
@@ -7141,10 +7141,10 @@
       <c r="B76" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="C76" s="1" t="s">
+      <c r="C76" s="1" t="s"/>
+      <c r="D76" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D76" s="1" t="s"/>
       <c r="E76" t="s"/>
       <c r="F76" t="s"/>
       <c r="G76" t="s"/>
@@ -7173,10 +7173,10 @@
       <c r="B77" s="1" t="n">
         <v>83</v>
       </c>
-      <c r="C77" s="1" t="s">
+      <c r="C77" s="1" t="s"/>
+      <c r="D77" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D77" s="1" t="s"/>
       <c r="E77" t="s"/>
       <c r="F77" t="s"/>
       <c r="G77" t="s"/>
@@ -7205,10 +7205,10 @@
       <c r="B78" s="1" t="n">
         <v>151</v>
       </c>
-      <c r="C78" s="1" t="s">
+      <c r="C78" s="1" t="s"/>
+      <c r="D78" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D78" s="1" t="s"/>
       <c r="E78" t="s"/>
       <c r="F78" t="s"/>
       <c r="G78" t="s"/>
@@ -7239,10 +7239,10 @@
       <c r="B79" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C79" s="1" t="s">
+      <c r="C79" s="1" t="s"/>
+      <c r="D79" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D79" s="1" t="s"/>
       <c r="E79" t="s"/>
       <c r="F79" t="s"/>
       <c r="G79" t="s"/>
@@ -7271,10 +7271,10 @@
       <c r="B80" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C80" s="1" t="s">
+      <c r="C80" s="1" t="s"/>
+      <c r="D80" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D80" s="1" t="s"/>
       <c r="E80" t="s"/>
       <c r="F80" t="s"/>
       <c r="G80" t="s"/>
@@ -7303,10 +7303,10 @@
       <c r="B81" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="C81" s="1" t="s">
+      <c r="C81" s="1" t="s"/>
+      <c r="D81" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D81" s="1" t="s"/>
       <c r="E81" t="s"/>
       <c r="F81" t="s"/>
       <c r="G81" t="s"/>
@@ -7335,10 +7335,10 @@
       <c r="B82" s="1" t="n">
         <v>66</v>
       </c>
-      <c r="C82" s="1" t="s">
+      <c r="C82" s="1" t="s"/>
+      <c r="D82" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D82" s="1" t="s"/>
       <c r="E82" t="s"/>
       <c r="F82" t="s"/>
       <c r="G82" t="s"/>
@@ -7367,10 +7367,10 @@
       <c r="B83" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="C83" s="1" t="s">
+      <c r="C83" s="1" t="s"/>
+      <c r="D83" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D83" s="1" t="s"/>
       <c r="E83" t="s"/>
       <c r="F83" t="s"/>
       <c r="G83" t="s"/>
@@ -7399,10 +7399,10 @@
       <c r="B84" s="1" t="n">
         <v>83</v>
       </c>
-      <c r="C84" s="1" t="s">
+      <c r="C84" s="1" t="s"/>
+      <c r="D84" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D84" s="1" t="s"/>
       <c r="E84" t="s"/>
       <c r="F84" t="s"/>
       <c r="G84" t="s"/>
@@ -7431,10 +7431,10 @@
       <c r="B85" s="1" t="n">
         <v>151</v>
       </c>
-      <c r="C85" s="1" t="s">
+      <c r="C85" s="1" t="s"/>
+      <c r="D85" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D85" s="1" t="s"/>
       <c r="E85" t="s"/>
       <c r="F85" t="s"/>
       <c r="G85" t="s"/>
@@ -7465,10 +7465,10 @@
       <c r="B86" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C86" s="1" t="s">
+      <c r="C86" s="1" t="s"/>
+      <c r="D86" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D86" s="1" t="s"/>
       <c r="E86" t="s"/>
       <c r="F86" t="s"/>
       <c r="G86" t="s"/>
@@ -7497,10 +7497,10 @@
       <c r="B87" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C87" s="1" t="s">
+      <c r="C87" s="1" t="s"/>
+      <c r="D87" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D87" s="1" t="s"/>
       <c r="E87" t="s"/>
       <c r="F87" t="s"/>
       <c r="G87" t="s"/>
@@ -7529,10 +7529,10 @@
       <c r="B88" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="C88" s="1" t="s">
+      <c r="C88" s="1" t="s"/>
+      <c r="D88" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D88" s="1" t="s"/>
       <c r="E88" t="s"/>
       <c r="F88" t="s"/>
       <c r="G88" t="s"/>
@@ -7561,10 +7561,10 @@
       <c r="B89" s="1" t="n">
         <v>66</v>
       </c>
-      <c r="C89" s="1" t="s">
+      <c r="C89" s="1" t="s"/>
+      <c r="D89" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D89" s="1" t="s"/>
       <c r="E89" t="s"/>
       <c r="F89" t="s"/>
       <c r="G89" t="s"/>
@@ -7593,10 +7593,10 @@
       <c r="B90" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="C90" s="1" t="s">
+      <c r="C90" s="1" t="s"/>
+      <c r="D90" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D90" s="1" t="s"/>
       <c r="E90" t="s"/>
       <c r="F90" t="s"/>
       <c r="G90" t="s"/>
@@ -7625,10 +7625,10 @@
       <c r="B91" s="1" t="n">
         <v>83</v>
       </c>
-      <c r="C91" s="1" t="s">
+      <c r="C91" s="1" t="s"/>
+      <c r="D91" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D91" s="1" t="s"/>
       <c r="E91" t="s"/>
       <c r="F91" t="s"/>
       <c r="G91" t="s"/>
@@ -7657,10 +7657,10 @@
       <c r="B92" s="1" t="n">
         <v>151</v>
       </c>
-      <c r="C92" s="1" t="s">
+      <c r="C92" s="1" t="s"/>
+      <c r="D92" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D92" s="1" t="s"/>
       <c r="E92" t="s"/>
       <c r="F92" t="s"/>
       <c r="G92" t="s"/>
@@ -7691,10 +7691,10 @@
       <c r="B93" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C93" s="1" t="s">
+      <c r="C93" s="1" t="s"/>
+      <c r="D93" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D93" s="1" t="s"/>
       <c r="E93" t="s"/>
       <c r="F93" t="s"/>
       <c r="G93" t="s"/>
@@ -7723,10 +7723,10 @@
       <c r="B94" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C94" s="1" t="s">
+      <c r="C94" s="1" t="s"/>
+      <c r="D94" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D94" s="1" t="s"/>
       <c r="E94" t="s"/>
       <c r="F94" t="s"/>
       <c r="G94" t="s"/>
@@ -7755,10 +7755,10 @@
       <c r="B95" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="C95" s="1" t="s">
+      <c r="C95" s="1" t="s"/>
+      <c r="D95" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D95" s="1" t="s"/>
       <c r="E95" t="s"/>
       <c r="F95" t="s"/>
       <c r="G95" t="s"/>
@@ -7787,10 +7787,10 @@
       <c r="B96" s="1" t="n">
         <v>66</v>
       </c>
-      <c r="C96" s="1" t="s">
+      <c r="C96" s="1" t="s"/>
+      <c r="D96" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D96" s="1" t="s"/>
       <c r="E96" t="s"/>
       <c r="F96" t="s"/>
       <c r="G96" t="s"/>
@@ -7819,10 +7819,10 @@
       <c r="B97" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="C97" s="1" t="s">
+      <c r="C97" s="1" t="s"/>
+      <c r="D97" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D97" s="1" t="s"/>
       <c r="E97" t="s"/>
       <c r="F97" t="s"/>
       <c r="G97" t="s"/>
@@ -7851,10 +7851,10 @@
       <c r="B98" s="1" t="n">
         <v>83</v>
       </c>
-      <c r="C98" s="1" t="s">
+      <c r="C98" s="1" t="s"/>
+      <c r="D98" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D98" s="1" t="s"/>
       <c r="E98" t="s"/>
       <c r="F98" t="s"/>
       <c r="G98" t="s"/>
@@ -7883,10 +7883,10 @@
       <c r="B99" s="1" t="n">
         <v>151</v>
       </c>
-      <c r="C99" s="1" t="s">
+      <c r="C99" s="1" t="s"/>
+      <c r="D99" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D99" s="1" t="s"/>
       <c r="E99" t="s"/>
       <c r="F99" t="s"/>
       <c r="G99" t="s"/>
@@ -7917,10 +7917,10 @@
       <c r="B100" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C100" s="1" t="s">
+      <c r="C100" s="1" t="s"/>
+      <c r="D100" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D100" s="1" t="s"/>
       <c r="E100" t="s"/>
       <c r="F100" t="s"/>
       <c r="G100" t="s"/>
@@ -7949,10 +7949,10 @@
       <c r="B101" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C101" s="1" t="s">
+      <c r="C101" s="1" t="s"/>
+      <c r="D101" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D101" s="1" t="s"/>
       <c r="E101" t="s"/>
       <c r="F101" t="s"/>
       <c r="G101" t="s"/>
@@ -7981,10 +7981,10 @@
       <c r="B102" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="C102" s="1" t="s">
+      <c r="C102" s="1" t="s"/>
+      <c r="D102" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D102" s="1" t="s"/>
       <c r="E102" t="s"/>
       <c r="F102" t="s"/>
       <c r="G102" t="s"/>
@@ -8013,10 +8013,10 @@
       <c r="B103" s="1" t="n">
         <v>66</v>
       </c>
-      <c r="C103" s="1" t="s">
+      <c r="C103" s="1" t="s"/>
+      <c r="D103" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D103" s="1" t="s"/>
       <c r="E103" t="s"/>
       <c r="F103" t="s"/>
       <c r="G103" t="s"/>
@@ -8045,10 +8045,10 @@
       <c r="B104" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="C104" s="1" t="s">
+      <c r="C104" s="1" t="s"/>
+      <c r="D104" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D104" s="1" t="s"/>
       <c r="E104" t="s"/>
       <c r="F104" t="s"/>
       <c r="G104" t="s"/>
@@ -8077,10 +8077,10 @@
       <c r="B105" s="1" t="n">
         <v>83</v>
       </c>
-      <c r="C105" s="1" t="s">
+      <c r="C105" s="1" t="s"/>
+      <c r="D105" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D105" s="1" t="s"/>
       <c r="E105" t="s"/>
       <c r="F105" t="s"/>
       <c r="G105" t="s"/>
@@ -8109,10 +8109,10 @@
       <c r="B106" s="1" t="n">
         <v>151</v>
       </c>
-      <c r="C106" s="1" t="s">
+      <c r="C106" s="1" t="s"/>
+      <c r="D106" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D106" s="1" t="s"/>
       <c r="E106" t="s"/>
       <c r="F106" t="s"/>
       <c r="G106" t="s"/>
@@ -8143,10 +8143,10 @@
       <c r="B107" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C107" s="1" t="s">
+      <c r="C107" s="1" t="s"/>
+      <c r="D107" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D107" s="1" t="s"/>
       <c r="E107" t="s"/>
       <c r="F107" t="s"/>
       <c r="G107" t="s"/>
@@ -8175,10 +8175,10 @@
       <c r="B108" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C108" s="1" t="s">
+      <c r="C108" s="1" t="s"/>
+      <c r="D108" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D108" s="1" t="s"/>
       <c r="E108" t="s"/>
       <c r="F108" t="s"/>
       <c r="G108" t="s"/>
@@ -8207,10 +8207,10 @@
       <c r="B109" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="C109" s="1" t="s">
+      <c r="C109" s="1" t="s"/>
+      <c r="D109" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D109" s="1" t="s"/>
       <c r="E109" t="s"/>
       <c r="F109" t="s"/>
       <c r="G109" t="s"/>
@@ -8239,10 +8239,10 @@
       <c r="B110" s="1" t="n">
         <v>66</v>
       </c>
-      <c r="C110" s="1" t="s">
+      <c r="C110" s="1" t="s"/>
+      <c r="D110" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D110" s="1" t="s"/>
       <c r="E110" t="s"/>
       <c r="F110" t="s"/>
       <c r="G110" t="s"/>
@@ -8271,10 +8271,10 @@
       <c r="B111" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="C111" s="1" t="s">
+      <c r="C111" s="1" t="s"/>
+      <c r="D111" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D111" s="1" t="s"/>
       <c r="E111" t="s"/>
       <c r="F111" t="s"/>
       <c r="G111" t="s"/>
@@ -8303,10 +8303,10 @@
       <c r="B112" s="1" t="n">
         <v>83</v>
       </c>
-      <c r="C112" s="1" t="s">
+      <c r="C112" s="1" t="s"/>
+      <c r="D112" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D112" s="1" t="s"/>
       <c r="E112" t="s"/>
       <c r="F112" t="s"/>
       <c r="G112" t="s"/>
@@ -8335,10 +8335,10 @@
       <c r="B113" s="1" t="n">
         <v>151</v>
       </c>
-      <c r="C113" s="1" t="s">
+      <c r="C113" s="1" t="s"/>
+      <c r="D113" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D113" s="1" t="s"/>
       <c r="E113" t="s"/>
       <c r="F113" t="s"/>
       <c r="G113" t="s"/>
@@ -8369,10 +8369,10 @@
       <c r="B114" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C114" s="1" t="s">
+      <c r="C114" s="1" t="s"/>
+      <c r="D114" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D114" s="1" t="s"/>
       <c r="E114" t="s"/>
       <c r="F114" t="s"/>
       <c r="G114" t="s"/>
@@ -8401,10 +8401,10 @@
       <c r="B115" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C115" s="1" t="s">
+      <c r="C115" s="1" t="s"/>
+      <c r="D115" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D115" s="1" t="s"/>
       <c r="E115" t="s"/>
       <c r="F115" t="s"/>
       <c r="G115" t="s"/>
@@ -8433,10 +8433,10 @@
       <c r="B116" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="C116" s="1" t="s">
+      <c r="C116" s="1" t="s"/>
+      <c r="D116" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D116" s="1" t="s"/>
       <c r="E116" t="s"/>
       <c r="F116" t="s"/>
       <c r="G116" t="s"/>
@@ -8465,10 +8465,10 @@
       <c r="B117" s="1" t="n">
         <v>66</v>
       </c>
-      <c r="C117" s="1" t="s">
+      <c r="C117" s="1" t="s"/>
+      <c r="D117" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D117" s="1" t="s"/>
       <c r="E117" t="s"/>
       <c r="F117" t="s"/>
       <c r="G117" t="s"/>
@@ -8497,10 +8497,10 @@
       <c r="B118" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="C118" s="1" t="s">
+      <c r="C118" s="1" t="s"/>
+      <c r="D118" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D118" s="1" t="s"/>
       <c r="E118" t="s"/>
       <c r="F118" t="s"/>
       <c r="G118" t="s"/>
@@ -8529,10 +8529,10 @@
       <c r="B119" s="1" t="n">
         <v>83</v>
       </c>
-      <c r="C119" s="1" t="s">
+      <c r="C119" s="1" t="s"/>
+      <c r="D119" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D119" s="1" t="s"/>
       <c r="E119" t="s"/>
       <c r="F119" t="s"/>
       <c r="G119" t="s"/>
@@ -8561,10 +8561,10 @@
       <c r="B120" s="1" t="n">
         <v>151</v>
       </c>
-      <c r="C120" s="1" t="s">
+      <c r="C120" s="1" t="s"/>
+      <c r="D120" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D120" s="1" t="s"/>
       <c r="E120" t="s"/>
       <c r="F120" t="s"/>
       <c r="G120" t="s"/>
@@ -8595,10 +8595,10 @@
       <c r="B121" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C121" s="1" t="s">
+      <c r="C121" s="1" t="s"/>
+      <c r="D121" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D121" s="1" t="s"/>
       <c r="E121" t="s"/>
       <c r="F121" t="s"/>
       <c r="G121" t="s"/>
@@ -8627,10 +8627,10 @@
       <c r="B122" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C122" s="1" t="s">
+      <c r="C122" s="1" t="s"/>
+      <c r="D122" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D122" s="1" t="s"/>
       <c r="E122" t="s"/>
       <c r="F122" t="s"/>
       <c r="G122" t="s"/>
@@ -8659,10 +8659,10 @@
       <c r="B123" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="C123" s="1" t="s">
+      <c r="C123" s="1" t="s"/>
+      <c r="D123" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D123" s="1" t="s"/>
       <c r="E123" t="s"/>
       <c r="F123" t="s"/>
       <c r="G123" t="s"/>
@@ -8691,10 +8691,10 @@
       <c r="B124" s="1" t="n">
         <v>66</v>
       </c>
-      <c r="C124" s="1" t="s">
+      <c r="C124" s="1" t="s"/>
+      <c r="D124" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D124" s="1" t="s"/>
       <c r="E124" t="s"/>
       <c r="F124" t="s"/>
       <c r="G124" t="s"/>
@@ -8723,10 +8723,10 @@
       <c r="B125" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="C125" s="1" t="s">
+      <c r="C125" s="1" t="s"/>
+      <c r="D125" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D125" s="1" t="s"/>
       <c r="E125" t="s"/>
       <c r="F125" t="s"/>
       <c r="G125" t="s"/>
@@ -8755,10 +8755,10 @@
       <c r="B126" s="1" t="n">
         <v>83</v>
       </c>
-      <c r="C126" s="1" t="s">
+      <c r="C126" s="1" t="s"/>
+      <c r="D126" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D126" s="1" t="s"/>
       <c r="E126" t="s"/>
       <c r="F126" t="s"/>
       <c r="G126" t="s"/>
@@ -8787,10 +8787,10 @@
       <c r="B127" s="1" t="n">
         <v>151</v>
       </c>
-      <c r="C127" s="1" t="s">
+      <c r="C127" s="1" t="s"/>
+      <c r="D127" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D127" s="1" t="s"/>
       <c r="E127" t="s"/>
       <c r="F127" t="s"/>
       <c r="G127" t="s"/>
@@ -8880,10 +8880,10 @@
       <c r="B2" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="1" t="s"/>
+      <c r="D2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="1" t="s"/>
       <c r="E2" t="n">
         <v>12.40234375</v>
       </c>
@@ -8894,10 +8894,10 @@
       <c r="B3" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="1" t="s"/>
+      <c r="D3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="1" t="s"/>
       <c r="E3" t="n">
         <v>36.375</v>
       </c>
@@ -8908,10 +8908,10 @@
       <c r="B4" s="1" t="n">
         <v>151</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="1" t="s"/>
+      <c r="D4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="1" t="s"/>
       <c r="E4" t="n">
         <v>48.7734375</v>
       </c>
@@ -8924,10 +8924,10 @@
       <c r="B5" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="1" t="s"/>
+      <c r="D5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="1" t="s"/>
       <c r="E5" t="n">
         <v>17.60009765625</v>
       </c>
@@ -8938,10 +8938,10 @@
       <c r="B6" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="1" t="s"/>
+      <c r="D6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="1" t="s"/>
       <c r="E6" t="n">
         <v>13.69140625</v>
       </c>
@@ -8952,10 +8952,10 @@
       <c r="B7" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="1" t="s"/>
+      <c r="D7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="1" t="s"/>
       <c r="E7" t="n">
         <v>13</v>
       </c>
@@ -8966,10 +8966,10 @@
       <c r="B8" s="1" t="n">
         <v>151</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="1" t="s"/>
+      <c r="D8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="1" t="s"/>
       <c r="E8" t="n">
         <v>44.2890625</v>
       </c>
@@ -8982,10 +8982,10 @@
       <c r="B9" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="1" t="s"/>
+      <c r="D9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="1" t="s"/>
       <c r="E9" t="n">
         <v>-4.328125</v>
       </c>
@@ -8996,10 +8996,10 @@
       <c r="B10" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="1" t="s"/>
+      <c r="D10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="1" t="s"/>
       <c r="E10" t="n">
         <v>-3.671875</v>
       </c>
@@ -9010,10 +9010,10 @@
       <c r="B11" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="1" t="s"/>
+      <c r="D11" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="1" t="s"/>
       <c r="E11" t="n">
         <v>-2.455078125</v>
       </c>
@@ -9024,10 +9024,10 @@
       <c r="B12" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="1" t="s"/>
+      <c r="D12" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="1" t="s"/>
       <c r="E12" t="n">
         <v>-5.41015625</v>
       </c>
@@ -9038,10 +9038,10 @@
       <c r="B13" s="1" t="n">
         <v>151</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="1" t="s"/>
+      <c r="D13" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="1" t="s"/>
       <c r="E13" t="n">
         <v>-15.859375</v>
       </c>
@@ -9054,10 +9054,10 @@
       <c r="B14" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="1" t="s"/>
+      <c r="D14" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="1" t="s"/>
       <c r="E14" t="n">
         <v>-6.240234375</v>
       </c>
@@ -9068,10 +9068,10 @@
       <c r="B15" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="1" t="s"/>
+      <c r="D15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="1" t="s"/>
       <c r="E15" t="n">
         <v>-1.689453125</v>
       </c>
@@ -9082,10 +9082,10 @@
       <c r="B16" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="1" t="s"/>
+      <c r="D16" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D16" s="1" t="s"/>
       <c r="E16" t="n">
         <v>1.640625</v>
       </c>
@@ -9096,10 +9096,10 @@
       <c r="B17" s="1" t="n">
         <v>151</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="1" t="s"/>
+      <c r="D17" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="1" t="s"/>
       <c r="E17" t="n">
         <v>-6.296875</v>
       </c>
@@ -9112,10 +9112,10 @@
       <c r="B18" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="1" t="s"/>
+      <c r="D18" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D18" s="1" t="s"/>
       <c r="E18" t="n">
         <v>-2.48046875</v>
       </c>
@@ -9126,10 +9126,10 @@
       <c r="B19" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="1" t="s"/>
+      <c r="D19" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D19" s="1" t="s"/>
       <c r="E19" t="n">
         <v>-7.01953125</v>
       </c>
@@ -9140,10 +9140,10 @@
       <c r="B20" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="1" t="s"/>
+      <c r="D20" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D20" s="1" t="s"/>
       <c r="E20" t="n">
         <v>-8.36328125</v>
       </c>
@@ -9154,10 +9154,10 @@
       <c r="B21" s="1" t="n">
         <v>151</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="1" t="s"/>
+      <c r="D21" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D21" s="1" t="s"/>
       <c r="E21" t="n">
         <v>-17.859375</v>
       </c>
@@ -9170,10 +9170,10 @@
       <c r="B22" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="1" t="s"/>
+      <c r="D22" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D22" s="1" t="s"/>
       <c r="E22" t="n">
         <v>1.375</v>
       </c>
@@ -9184,10 +9184,10 @@
       <c r="B23" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="1" t="s"/>
+      <c r="D23" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D23" s="1" t="s"/>
       <c r="E23" t="n">
         <v>1.40234375</v>
       </c>
@@ -9198,10 +9198,10 @@
       <c r="B24" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" s="1" t="s"/>
+      <c r="D24" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D24" s="1" t="s"/>
       <c r="E24" t="n">
         <v>0.291015625</v>
       </c>
@@ -9212,10 +9212,10 @@
       <c r="B25" s="1" t="n">
         <v>151</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" s="1" t="s"/>
+      <c r="D25" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D25" s="1" t="s"/>
       <c r="E25" t="n">
         <v>3.06640625</v>
       </c>
@@ -9228,10 +9228,10 @@
       <c r="B26" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" s="1" t="s"/>
+      <c r="D26" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D26" s="1" t="s"/>
       <c r="E26" t="n">
         <v>-2.01171875</v>
       </c>
@@ -9242,10 +9242,10 @@
       <c r="B27" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" s="1" t="s"/>
+      <c r="D27" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D27" s="1" t="s"/>
       <c r="E27" t="n">
         <v>25.779296875</v>
       </c>
@@ -9256,10 +9256,10 @@
       <c r="B28" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" s="1" t="s"/>
+      <c r="D28" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D28" s="1" t="s"/>
       <c r="E28" t="n">
         <v>-18.92578125</v>
       </c>
@@ -9270,10 +9270,10 @@
       <c r="B29" s="1" t="n">
         <v>151</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C29" s="1" t="s"/>
+      <c r="D29" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D29" s="1" t="s"/>
       <c r="E29" t="n">
         <v>4.84375</v>
       </c>
@@ -9286,10 +9286,10 @@
       <c r="B30" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C30" s="1" t="s"/>
+      <c r="D30" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D30" s="1" t="s"/>
       <c r="E30" t="n">
         <v>-0.1904296875</v>
       </c>
@@ -9300,10 +9300,10 @@
       <c r="B31" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" s="1" t="s"/>
+      <c r="D31" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D31" s="1" t="s"/>
       <c r="E31" t="n">
         <v>-0.1875</v>
       </c>
@@ -9314,10 +9314,10 @@
       <c r="B32" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" s="1" t="s"/>
+      <c r="D32" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D32" s="1" t="s"/>
       <c r="E32" t="n">
         <v>-0.8515625</v>
       </c>
@@ -9328,10 +9328,10 @@
       <c r="B33" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C33" s="1" t="s"/>
+      <c r="D33" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D33" s="1" t="s"/>
       <c r="E33" t="n">
         <v>54.306640625</v>
       </c>
@@ -9342,10 +9342,10 @@
       <c r="B34" s="1" t="n">
         <v>83</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C34" s="1" t="s"/>
+      <c r="D34" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D34" s="1" t="s"/>
       <c r="E34" t="n">
         <v>-1.257080078125</v>
       </c>
@@ -9356,10 +9356,10 @@
       <c r="B35" s="1" t="n">
         <v>151</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C35" s="1" t="s"/>
+      <c r="D35" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D35" s="1" t="s"/>
       <c r="E35" t="n">
         <v>51.8203125</v>
       </c>
@@ -9372,10 +9372,10 @@
       <c r="B36" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C36" s="1" t="s"/>
+      <c r="D36" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D36" s="1" t="s"/>
       <c r="E36" t="n">
         <v>-0.09912109375</v>
       </c>
@@ -9386,10 +9386,10 @@
       <c r="B37" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C37" s="1" t="s"/>
+      <c r="D37" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D37" s="1" t="s"/>
       <c r="E37" t="n">
         <v>-10.85546875</v>
       </c>
@@ -9400,10 +9400,10 @@
       <c r="B38" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C38" s="1" t="s"/>
+      <c r="D38" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D38" s="1" t="s"/>
       <c r="E38" t="n">
         <v>-14.6015625</v>
       </c>
@@ -9416,10 +9416,10 @@
       <c r="B39" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C39" s="1" t="s"/>
+      <c r="D39" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D39" s="1" t="s"/>
       <c r="E39" t="n">
         <v>62.322265625</v>
       </c>
@@ -9430,10 +9430,10 @@
       <c r="B40" s="1" t="n">
         <v>151</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C40" s="1" t="s"/>
+      <c r="D40" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D40" s="1" t="s"/>
       <c r="E40" t="n">
         <v>36.765625</v>
       </c>
@@ -9448,10 +9448,10 @@
       <c r="B41" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C41" s="1" t="s"/>
+      <c r="D41" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D41" s="1" t="s"/>
       <c r="E41" t="n">
         <v>53</v>
       </c>
@@ -9462,10 +9462,10 @@
       <c r="B42" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C42" s="1" t="s"/>
+      <c r="D42" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D42" s="1" t="s"/>
       <c r="E42" t="n">
         <v>-72.87890625</v>
       </c>
@@ -9476,10 +9476,10 @@
       <c r="B43" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C43" s="1" t="s"/>
+      <c r="D43" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D43" s="1" t="s"/>
       <c r="E43" t="n">
         <v>12.87890625</v>
       </c>
@@ -9492,10 +9492,10 @@
       <c r="B44" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="C44" s="1" t="s"/>
+      <c r="D44" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D44" s="1" t="s"/>
       <c r="E44" t="n">
         <v>45.37109375</v>
       </c>
@@ -9506,10 +9506,10 @@
       <c r="B45" s="1" t="n">
         <v>83</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C45" s="1" t="s"/>
+      <c r="D45" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D45" s="1" t="s"/>
       <c r="E45" t="n">
         <v>-1.159912109375</v>
       </c>
@@ -9520,10 +9520,10 @@
       <c r="B46" s="1" t="n">
         <v>151</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C46" s="1" t="s"/>
+      <c r="D46" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D46" s="1" t="s"/>
       <c r="E46" t="n">
         <v>37.2109375</v>
       </c>
@@ -9538,10 +9538,10 @@
       <c r="B47" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="C47" s="1" t="s"/>
+      <c r="D47" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D47" s="1" t="s"/>
       <c r="E47" t="n">
         <v>34.01611328125</v>
       </c>
@@ -9552,10 +9552,10 @@
       <c r="B48" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C48" s="1" t="s"/>
+      <c r="D48" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D48" s="1" t="s"/>
       <c r="E48" t="n">
         <v>18.380859375</v>
       </c>
@@ -9566,10 +9566,10 @@
       <c r="B49" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C49" s="1" t="s"/>
+      <c r="D49" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D49" s="1" t="s"/>
       <c r="E49" t="n">
         <v>53.6650390625</v>
       </c>
@@ -9582,10 +9582,10 @@
       <c r="B50" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C50" s="1" t="s"/>
+      <c r="D50" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D50" s="1" t="s"/>
       <c r="E50" t="n">
         <v>64.2265625</v>
       </c>
@@ -9596,10 +9596,10 @@
       <c r="B51" s="1" t="n">
         <v>83</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C51" s="1" t="s"/>
+      <c r="D51" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D51" s="1" t="s"/>
       <c r="E51" t="n">
         <v>19.375</v>
       </c>
@@ -9610,10 +9610,10 @@
       <c r="B52" s="1" t="n">
         <v>151</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="C52" s="1" t="s"/>
+      <c r="D52" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D52" s="1" t="s"/>
       <c r="E52" t="n">
         <v>189.6640625</v>
       </c>
@@ -9628,10 +9628,10 @@
       <c r="B53" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="C53" s="1" t="s"/>
+      <c r="D53" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D53" s="1" t="s"/>
       <c r="E53" t="n">
         <v>168.0380859375</v>
       </c>
@@ -9642,10 +9642,10 @@
       <c r="B54" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="C54" s="1" t="s"/>
+      <c r="D54" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D54" s="1" t="s"/>
       <c r="E54" t="n">
         <v>4.138671875</v>
       </c>
@@ -9656,10 +9656,10 @@
       <c r="B55" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="C55" s="1" t="s"/>
+      <c r="D55" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D55" s="1" t="s"/>
       <c r="E55" t="n">
         <v>123.466796875</v>
       </c>
@@ -9672,10 +9672,10 @@
       <c r="B56" s="1" t="n">
         <v>66</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="C56" s="1" t="s"/>
+      <c r="D56" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D56" s="1" t="s"/>
       <c r="E56" t="n">
         <v>2.4530029296875</v>
       </c>
@@ -9686,10 +9686,10 @@
       <c r="B57" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="C57" s="1" t="s">
+      <c r="C57" s="1" t="s"/>
+      <c r="D57" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D57" s="1" t="s"/>
       <c r="E57" t="n">
         <v>133.064453125</v>
       </c>
@@ -9700,10 +9700,10 @@
       <c r="B58" s="1" t="n">
         <v>83</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="C58" s="1" t="s"/>
+      <c r="D58" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D58" s="1" t="s"/>
       <c r="E58" t="n">
         <v>11.50390625</v>
       </c>
@@ -9714,10 +9714,10 @@
       <c r="B59" s="1" t="n">
         <v>151</v>
       </c>
-      <c r="C59" s="1" t="s">
+      <c r="C59" s="1" t="s"/>
+      <c r="D59" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D59" s="1" t="s"/>
       <c r="E59" t="n">
         <v>442.6640625</v>
       </c>
@@ -9732,10 +9732,10 @@
       <c r="B60" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="C60" s="1" t="s"/>
+      <c r="D60" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D60" s="1" t="s"/>
       <c r="E60" t="n">
         <v>184.7626953125</v>
       </c>
@@ -9746,10 +9746,10 @@
       <c r="B61" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C61" s="1" t="s">
+      <c r="C61" s="1" t="s"/>
+      <c r="D61" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D61" s="1" t="s"/>
       <c r="E61" t="n">
         <v>249.984375</v>
       </c>
@@ -9760,10 +9760,10 @@
       <c r="B62" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="C62" s="1" t="s">
+      <c r="C62" s="1" t="s"/>
+      <c r="D62" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D62" s="1" t="s"/>
       <c r="E62" t="n">
         <v>-5.326171875</v>
       </c>
@@ -9776,10 +9776,10 @@
       <c r="B63" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="C63" s="1" t="s">
+      <c r="C63" s="1" t="s"/>
+      <c r="D63" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D63" s="1" t="s"/>
       <c r="E63" t="n">
         <v>-13.109375</v>
       </c>
@@ -9790,10 +9790,10 @@
       <c r="B64" s="1" t="n">
         <v>83</v>
       </c>
-      <c r="C64" s="1" t="s">
+      <c r="C64" s="1" t="s"/>
+      <c r="D64" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D64" s="1" t="s"/>
       <c r="E64" t="n">
         <v>80.60302734375</v>
       </c>
@@ -9804,10 +9804,10 @@
       <c r="B65" s="1" t="n">
         <v>151</v>
       </c>
-      <c r="C65" s="1" t="s">
+      <c r="C65" s="1" t="s"/>
+      <c r="D65" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D65" s="1" t="s"/>
       <c r="E65" t="n">
         <v>493.3984375</v>
       </c>
@@ -9876,10 +9876,10 @@
       <c r="B2" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="1" t="s"/>
+      <c r="D2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="1" t="s"/>
       <c r="E2" t="n">
         <v>0.05766226114883929</v>
       </c>
@@ -9890,10 +9890,10 @@
       <c r="B3" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="1" t="s"/>
+      <c r="D3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="1" t="s"/>
       <c r="E3" t="n">
         <v>0.1066398906483046</v>
       </c>
@@ -9904,10 +9904,10 @@
       <c r="B4" s="1" t="n">
         <v>151</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="1" t="s"/>
+      <c r="D4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="1" t="s"/>
       <c r="E4" t="n">
         <v>0.05791419292912511</v>
       </c>
@@ -9920,10 +9920,10 @@
       <c r="B5" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="1" t="s"/>
+      <c r="D5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="1" t="s"/>
       <c r="E5" t="n">
         <v>0.224577928073755</v>
       </c>
@@ -9934,10 +9934,10 @@
       <c r="B6" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="1" t="s"/>
+      <c r="D6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="1" t="s"/>
       <c r="E6" t="n">
         <v>0.06076691838560763</v>
       </c>
@@ -9948,10 +9948,10 @@
       <c r="B7" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="1" t="s"/>
+      <c r="D7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="1" t="s"/>
       <c r="E7" t="n">
         <v>0.03530781240517922</v>
       </c>
@@ -9962,10 +9962,10 @@
       <c r="B8" s="1" t="n">
         <v>151</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="1" t="s"/>
+      <c r="D8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="1" t="s"/>
       <c r="E8" t="n">
         <v>0.04273402475663693</v>
       </c>
@@ -9978,10 +9978,10 @@
       <c r="B9" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="1" t="s"/>
+      <c r="D9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="1" t="s"/>
       <c r="E9" t="n">
         <v>-0.086777044378176</v>
       </c>
@@ -9992,10 +9992,10 @@
       <c r="B10" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="1" t="s"/>
+      <c r="D10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="1" t="s"/>
       <c r="E10" t="n">
         <v>-0.01827900272483538</v>
       </c>
@@ -10006,10 +10006,10 @@
       <c r="B11" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="1" t="s"/>
+      <c r="D11" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="1" t="s"/>
       <c r="E11" t="n">
         <v>-0.01288196644601303</v>
       </c>
@@ -10020,10 +10020,10 @@
       <c r="B12" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="1" t="s"/>
+      <c r="D12" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="1" t="s"/>
       <c r="E12" t="n">
         <v>-0.02058909029445893</v>
       </c>
@@ -10034,10 +10034,10 @@
       <c r="B13" s="1" t="n">
         <v>151</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="1" t="s"/>
+      <c r="D13" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="1" t="s"/>
       <c r="E13" t="n">
         <v>-0.02120417573937289</v>
       </c>
@@ -10050,10 +10050,10 @@
       <c r="B14" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="1" t="s"/>
+      <c r="D14" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="1" t="s"/>
       <c r="E14" t="n">
         <v>-0.02295474316121084</v>
       </c>
@@ -10064,10 +10064,10 @@
       <c r="B15" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="1" t="s"/>
+      <c r="D15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="1" t="s"/>
       <c r="E15" t="n">
         <v>-0.006359615135207624</v>
       </c>
@@ -10078,10 +10078,10 @@
       <c r="B16" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="1" t="s"/>
+      <c r="D16" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D16" s="1" t="s"/>
       <c r="E16" t="n">
         <v>0.004970567141710869</v>
       </c>
@@ -10092,10 +10092,10 @@
       <c r="B17" s="1" t="n">
         <v>151</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="1" t="s"/>
+      <c r="D17" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="1" t="s"/>
       <c r="E17" t="n">
         <v>-0.006288303256623316</v>
       </c>
@@ -10108,10 +10108,10 @@
       <c r="B18" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="1" t="s"/>
+      <c r="D18" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D18" s="1" t="s"/>
       <c r="E18" t="n">
         <v>-0.008372252220228997</v>
       </c>
@@ -10122,10 +10122,10 @@
       <c r="B19" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="1" t="s"/>
+      <c r="D19" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D19" s="1" t="s"/>
       <c r="E19" t="n">
         <v>-0.02315123476472896</v>
       </c>
@@ -10136,10 +10136,10 @@
       <c r="B20" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="1" t="s"/>
+      <c r="D20" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D20" s="1" t="s"/>
       <c r="E20" t="n">
         <v>-0.02194128630662871</v>
       </c>
@@ -10150,10 +10150,10 @@
       <c r="B21" s="1" t="n">
         <v>151</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="1" t="s"/>
+      <c r="D21" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D21" s="1" t="s"/>
       <c r="E21" t="n">
         <v>-0.01577696043399202</v>
       </c>
@@ -10166,10 +10166,10 @@
       <c r="B22" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="1" t="s"/>
+      <c r="D22" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D22" s="1" t="s"/>
       <c r="E22" t="n">
         <v>0.02755588408640844</v>
       </c>
@@ -10180,10 +10180,10 @@
       <c r="B23" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="1" t="s"/>
+      <c r="D23" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D23" s="1" t="s"/>
       <c r="E23" t="n">
         <v>0.008781833151407917</v>
       </c>
@@ -10194,10 +10194,10 @@
       <c r="B24" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" s="1" t="s"/>
+      <c r="D24" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D24" s="1" t="s"/>
       <c r="E24" t="n">
         <v>0.001583810185982897</v>
       </c>
@@ -10208,10 +10208,10 @@
       <c r="B25" s="1" t="n">
         <v>151</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" s="1" t="s"/>
+      <c r="D25" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D25" s="1" t="s"/>
       <c r="E25" t="n">
         <v>0.005357770408549446</v>
       </c>
@@ -10224,10 +10224,10 @@
       <c r="B26" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" s="1" t="s"/>
+      <c r="D26" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D26" s="1" t="s"/>
       <c r="E26" t="n">
         <v>-0.009072542996807169</v>
       </c>
@@ -10238,10 +10238,10 @@
       <c r="B27" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" s="1" t="s"/>
+      <c r="D27" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D27" s="1" t="s"/>
       <c r="E27" t="n">
         <v>0.1401539835576303</v>
       </c>
@@ -10252,10 +10252,10 @@
       <c r="B28" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" s="1" t="s"/>
+      <c r="D28" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D28" s="1" t="s"/>
       <c r="E28" t="n">
         <v>-0.06826609885804695</v>
       </c>
@@ -10266,10 +10266,10 @@
       <c r="B29" s="1" t="n">
         <v>151</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C29" s="1" t="s"/>
+      <c r="D29" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D29" s="1" t="s"/>
       <c r="E29" t="n">
         <v>0.00594667919689522</v>
       </c>
@@ -10282,10 +10282,10 @@
       <c r="B30" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C30" s="1" t="s"/>
+      <c r="D30" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D30" s="1" t="s"/>
       <c r="E30" t="n">
         <v>-0.00278435194208548</v>
       </c>
@@ -10296,10 +10296,10 @@
       <c r="B31" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" s="1" t="s"/>
+      <c r="D31" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D31" s="1" t="s"/>
       <c r="E31" t="n">
         <v>-0.0008390299240896416</v>
       </c>
@@ -10310,10 +10310,10 @@
       <c r="B32" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" s="1" t="s"/>
+      <c r="D32" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D32" s="1" t="s"/>
       <c r="E32" t="n">
         <v>-0.003968873833870223</v>
       </c>
@@ -10324,10 +10324,10 @@
       <c r="B33" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C33" s="1" t="s"/>
+      <c r="D33" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D33" s="1" t="s"/>
       <c r="E33" t="n">
         <v>0.2039009952685876</v>
       </c>
@@ -10338,10 +10338,10 @@
       <c r="B34" s="1" t="n">
         <v>83</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C34" s="1" t="s"/>
+      <c r="D34" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D34" s="1" t="s"/>
       <c r="E34" t="n">
         <v>-0.05780866644983271</v>
       </c>
@@ -10352,10 +10352,10 @@
       <c r="B35" s="1" t="n">
         <v>151</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C35" s="1" t="s"/>
+      <c r="D35" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D35" s="1" t="s"/>
       <c r="E35" t="n">
         <v>0.06350768057082422</v>
       </c>
@@ -10368,10 +10368,10 @@
       <c r="B36" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C36" s="1" t="s"/>
+      <c r="D36" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D36" s="1" t="s"/>
       <c r="E36" t="n">
         <v>-0.001937781557035164</v>
       </c>
@@ -10382,10 +10382,10 @@
       <c r="B37" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C37" s="1" t="s"/>
+      <c r="D37" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D37" s="1" t="s"/>
       <c r="E37" t="n">
         <v>-0.07386825932198028</v>
       </c>
@@ -10396,10 +10396,10 @@
       <c r="B38" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C38" s="1" t="s"/>
+      <c r="D38" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D38" s="1" t="s"/>
       <c r="E38" t="n">
         <v>-0.08631361212768596</v>
       </c>
@@ -10412,10 +10412,10 @@
       <c r="B39" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C39" s="1" t="s"/>
+      <c r="D39" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D39" s="1" t="s"/>
       <c r="E39" t="n">
         <v>0.2574222376542363</v>
       </c>
@@ -10426,10 +10426,10 @@
       <c r="B40" s="1" t="n">
         <v>151</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C40" s="1" t="s"/>
+      <c r="D40" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D40" s="1" t="s"/>
       <c r="E40" t="n">
         <v>0.05737160512730986</v>
       </c>
@@ -10444,10 +10444,10 @@
       <c r="B41" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C41" s="1" t="s"/>
+      <c r="D41" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D41" s="1" t="s"/>
       <c r="E41" t="n">
         <v>0.9579291841601735</v>
       </c>
@@ -10458,10 +10458,10 @@
       <c r="B42" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C42" s="1" t="s"/>
+      <c r="D42" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D42" s="1" t="s"/>
       <c r="E42" t="n">
         <v>-0.4235199897939332</v>
       </c>
@@ -10472,10 +10472,10 @@
       <c r="B43" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C43" s="1" t="s"/>
+      <c r="D43" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D43" s="1" t="s"/>
       <c r="E43" t="n">
         <v>0.07455381340381236</v>
       </c>
@@ -10488,10 +10488,10 @@
       <c r="B44" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="C44" s="1" t="s"/>
+      <c r="D44" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D44" s="1" t="s"/>
       <c r="E44" t="n">
         <v>0.1908430497885939</v>
       </c>
@@ -10502,10 +10502,10 @@
       <c r="B45" s="1" t="n">
         <v>83</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C45" s="1" t="s"/>
+      <c r="D45" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D45" s="1" t="s"/>
       <c r="E45" t="n">
         <v>-0.0531713206587648</v>
       </c>
@@ -10516,10 +10516,10 @@
       <c r="B46" s="1" t="n">
         <v>151</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C46" s="1" t="s"/>
+      <c r="D46" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D46" s="1" t="s"/>
       <c r="E46" t="n">
         <v>0.0543813089968127</v>
       </c>
@@ -10534,10 +10534,10 @@
       <c r="B47" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="C47" s="1" t="s"/>
+      <c r="D47" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D47" s="1" t="s"/>
       <c r="E47" t="n">
         <v>0.5640964226335258</v>
       </c>
@@ -10548,10 +10548,10 @@
       <c r="B48" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C48" s="1" t="s"/>
+      <c r="D48" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D48" s="1" t="s"/>
       <c r="E48" t="n">
         <v>0.1059350294419686</v>
       </c>
@@ -10562,10 +10562,10 @@
       <c r="B49" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C49" s="1" t="s"/>
+      <c r="D49" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D49" s="1" t="s"/>
       <c r="E49" t="n">
         <v>0.3609306866352791</v>
       </c>
@@ -10578,10 +10578,10 @@
       <c r="B50" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C50" s="1" t="s"/>
+      <c r="D50" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D50" s="1" t="s"/>
       <c r="E50" t="n">
         <v>0.228724051707049</v>
       </c>
@@ -10592,10 +10592,10 @@
       <c r="B51" s="1" t="n">
         <v>83</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C51" s="1" t="s"/>
+      <c r="D51" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D51" s="1" t="s"/>
       <c r="E51" t="n">
         <v>0.9319303335103406</v>
       </c>
@@ -10606,10 +10606,10 @@
       <c r="B52" s="1" t="n">
         <v>151</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="C52" s="1" t="s"/>
+      <c r="D52" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D52" s="1" t="s"/>
       <c r="E52" t="n">
         <v>0.2692656004516413</v>
       </c>
@@ -10624,10 +10624,10 @@
       <c r="B53" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="C53" s="1" t="s"/>
+      <c r="D53" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D53" s="1" t="s"/>
       <c r="E53" t="n">
         <v>2.326153419383071</v>
       </c>
@@ -10638,10 +10638,10 @@
       <c r="B54" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="C54" s="1" t="s"/>
+      <c r="D54" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D54" s="1" t="s"/>
       <c r="E54" t="n">
         <v>0.02225240315977824</v>
       </c>
@@ -10652,10 +10652,10 @@
       <c r="B55" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="C55" s="1" t="s"/>
+      <c r="D55" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D55" s="1" t="s"/>
       <c r="E55" t="n">
         <v>0.7438252444274587</v>
       </c>
@@ -10668,10 +10668,10 @@
       <c r="B56" s="1" t="n">
         <v>66</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="C56" s="1" t="s"/>
+      <c r="D56" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D56" s="1" t="s"/>
       <c r="E56" t="n">
         <v>0.1508994228876165</v>
       </c>
@@ -10682,10 +10682,10 @@
       <c r="B57" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="C57" s="1" t="s">
+      <c r="C57" s="1" t="s"/>
+      <c r="D57" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D57" s="1" t="s"/>
       <c r="E57" t="n">
         <v>0.4911289831916514</v>
       </c>
@@ -10696,10 +10696,10 @@
       <c r="B58" s="1" t="n">
         <v>83</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="C58" s="1" t="s"/>
+      <c r="D58" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D58" s="1" t="s"/>
       <c r="E58" t="n">
         <v>0.3309652786377155</v>
       </c>
@@ -10710,10 +10710,10 @@
       <c r="B59" s="1" t="n">
         <v>151</v>
       </c>
-      <c r="C59" s="1" t="s">
+      <c r="C59" s="1" t="s"/>
+      <c r="D59" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D59" s="1" t="s"/>
       <c r="E59" t="n">
         <v>0.5898918515989056</v>
       </c>
@@ -10728,10 +10728,10 @@
       <c r="B60" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="C60" s="1" t="s"/>
+      <c r="D60" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D60" s="1" t="s"/>
       <c r="E60" t="n">
         <v>2.500645162143042</v>
       </c>
@@ -10742,10 +10742,10 @@
       <c r="B61" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C61" s="1" t="s">
+      <c r="C61" s="1" t="s"/>
+      <c r="D61" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D61" s="1" t="s"/>
       <c r="E61" t="n">
         <v>1.027471158366322</v>
       </c>
@@ -10756,10 +10756,10 @@
       <c r="B62" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="C62" s="1" t="s">
+      <c r="C62" s="1" t="s"/>
+      <c r="D62" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D62" s="1" t="s"/>
       <c r="E62" t="n">
         <v>-0.02349608269380391</v>
       </c>
@@ -10772,10 +10772,10 @@
       <c r="B63" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="C63" s="1" t="s">
+      <c r="C63" s="1" t="s"/>
+      <c r="D63" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D63" s="1" t="s"/>
       <c r="E63" t="n">
         <v>-0.03822258161876505</v>
       </c>
@@ -10786,10 +10786,10 @@
       <c r="B64" s="1" t="n">
         <v>83</v>
       </c>
-      <c r="C64" s="1" t="s">
+      <c r="C64" s="1" t="s"/>
+      <c r="D64" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D64" s="1" t="s"/>
       <c r="E64" t="n">
         <v>1.146861413912862</v>
       </c>
@@ -10800,10 +10800,10 @@
       <c r="B65" s="1" t="n">
         <v>151</v>
       </c>
-      <c r="C65" s="1" t="s">
+      <c r="C65" s="1" t="s"/>
+      <c r="D65" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D65" s="1" t="s"/>
       <c r="E65" t="n">
         <v>0.5038794046763168</v>
       </c>

</xml_diff>

<commit_message>
224_section d, G H, I added and working
</commit_message>
<xml_diff>
--- a/DataValidation/data validation for 105_FMILEAGE.xlsx
+++ b/DataValidation/data validation for 105_FMILEAGE.xlsx
@@ -11,8 +11,8 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Latest_DW_load" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="absolute revisions" sheetId="3" state="visible" r:id="rId3"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="percentage revisions" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PonP change for 2018201908" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="YonY change for 20182019" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PonP change for 2019202008" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="YonY change for 20192020" sheetId="6" state="visible" r:id="rId6"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Summary_Data" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
@@ -26,10 +26,10 @@
     <t>financial_period_key</t>
   </si>
   <si>
-    <t>provisional</t>
+    <t>toc_name</t>
   </si>
   <si>
-    <t>toc_name</t>
+    <t>provisional</t>
   </si>
   <si>
     <t>trains_planned</t>
@@ -110,7 +110,7 @@
     <t>a</t>
   </si>
   <si>
-    <t>No data shows as having significant Period on Period change for 2018201908</t>
+    <t>No data shows as having significant Period on Period change for 2019202008</t>
   </si>
   <si>
     <t>No data shows as being outside 95% confidence interval for Year on Year change</t>
@@ -492,7 +492,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U57"/>
+  <dimension ref="A1:U50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -567,20 +567,20 @@
     </row>
     <row r="2" spans="1:21">
       <c r="A2" s="1" t="n">
-        <v>2018201901</v>
-      </c>
-      <c r="B2" s="1" t="s"/>
-      <c r="C2" s="1" t="s">
+        <v>2019202001</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="C2" s="1" t="s"/>
       <c r="D2" t="s"/>
       <c r="E2" t="s"/>
       <c r="F2" t="s"/>
       <c r="G2" t="n">
-        <v>2568.5</v>
+        <v>1225.475952148438</v>
       </c>
       <c r="H2" t="n">
-        <v>78433.828125</v>
+        <v>53692.3671875</v>
       </c>
       <c r="I2" t="s"/>
       <c r="J2" t="s"/>
@@ -598,18 +598,18 @@
     </row>
     <row r="3" spans="1:21">
       <c r="A3" s="1" t="n"/>
-      <c r="B3" s="1" t="n"/>
-      <c r="C3" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="C3" s="1" t="s"/>
       <c r="D3" t="s"/>
       <c r="E3" t="s"/>
       <c r="F3" t="s"/>
       <c r="G3" t="n">
-        <v>34146.5</v>
+        <v>24272.455078125</v>
       </c>
       <c r="H3" t="n">
-        <v>940600.5625</v>
+        <v>840809.9375</v>
       </c>
       <c r="I3" t="s"/>
       <c r="J3" t="s"/>
@@ -627,18 +627,18 @@
     </row>
     <row r="4" spans="1:21">
       <c r="A4" s="1" t="n"/>
-      <c r="B4" s="1" t="n"/>
-      <c r="C4" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="C4" s="1" t="s"/>
       <c r="D4" t="s"/>
       <c r="E4" t="s"/>
       <c r="F4" t="s"/>
       <c r="G4" t="n">
-        <v>2088</v>
+        <v>1460.93505859375</v>
       </c>
       <c r="H4" t="n">
-        <v>89638.578125</v>
+        <v>94161.609375</v>
       </c>
       <c r="I4" t="s"/>
       <c r="J4" t="s"/>
@@ -656,18 +656,18 @@
     </row>
     <row r="5" spans="1:21">
       <c r="A5" s="1" t="n"/>
-      <c r="B5" s="1" t="n"/>
-      <c r="C5" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="C5" s="1" t="s"/>
       <c r="D5" t="s"/>
       <c r="E5" t="s"/>
       <c r="F5" t="s"/>
       <c r="G5" t="n">
-        <v>6161.5</v>
+        <v>5115.0849609375</v>
       </c>
       <c r="H5" t="n">
-        <v>154372.921875</v>
+        <v>162021.828125</v>
       </c>
       <c r="I5" t="s"/>
       <c r="J5" t="s"/>
@@ -685,18 +685,18 @@
     </row>
     <row r="6" spans="1:21">
       <c r="A6" s="1" t="n"/>
-      <c r="B6" s="1" t="n"/>
-      <c r="C6" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="C6" s="1" t="s"/>
       <c r="D6" t="s"/>
       <c r="E6" t="s"/>
       <c r="F6" t="s"/>
       <c r="G6" t="n">
-        <v>21521</v>
+        <v>14684.859375</v>
       </c>
       <c r="H6" t="n">
-        <v>679445.0625</v>
+        <v>630008.375</v>
       </c>
       <c r="I6" t="s"/>
       <c r="J6" t="s"/>
@@ -714,18 +714,18 @@
     </row>
     <row r="7" spans="1:21">
       <c r="A7" s="1" t="n"/>
-      <c r="B7" s="1" t="n"/>
-      <c r="C7" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="C7" s="1" t="s"/>
       <c r="D7" t="s"/>
       <c r="E7" t="s"/>
       <c r="F7" t="s"/>
       <c r="G7" t="n">
-        <v>17175</v>
+        <v>16902.26953125</v>
       </c>
       <c r="H7" t="n">
-        <v>400602.4375</v>
+        <v>459627.34375</v>
       </c>
       <c r="I7" t="s"/>
       <c r="J7" t="s"/>
@@ -743,18 +743,18 @@
     </row>
     <row r="8" spans="1:21">
       <c r="A8" s="1" t="n"/>
-      <c r="B8" s="1" t="n"/>
-      <c r="C8" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="C8" s="1" t="s"/>
       <c r="D8" t="s"/>
       <c r="E8" t="s"/>
       <c r="F8" t="s"/>
       <c r="G8" t="n">
-        <v>84265.5</v>
+        <v>64120.078125</v>
       </c>
       <c r="H8" t="n">
-        <v>2346576.5</v>
+        <v>2251425.25</v>
       </c>
       <c r="I8" t="s"/>
       <c r="J8" t="s"/>
@@ -772,20 +772,20 @@
     </row>
     <row r="9" spans="1:21">
       <c r="A9" s="1" t="n">
-        <v>2018201902</v>
-      </c>
-      <c r="B9" s="1" t="s"/>
-      <c r="C9" s="1" t="s">
+        <v>2019202002</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="C9" s="1" t="s"/>
       <c r="D9" t="s"/>
       <c r="E9" t="s"/>
       <c r="F9" t="s"/>
       <c r="G9" t="n">
-        <v>2096</v>
+        <v>1996.659057617188</v>
       </c>
       <c r="H9" t="n">
-        <v>76520.640625</v>
+        <v>59987.203125</v>
       </c>
       <c r="I9" t="s"/>
       <c r="J9" t="s"/>
@@ -803,18 +803,18 @@
     </row>
     <row r="10" spans="1:21">
       <c r="A10" s="1" t="n"/>
-      <c r="B10" s="1" t="n"/>
-      <c r="C10" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="C10" s="1" t="s"/>
       <c r="D10" t="s"/>
       <c r="E10" t="s"/>
       <c r="F10" t="s"/>
       <c r="G10" t="n">
-        <v>32796.5</v>
+        <v>23819.40625</v>
       </c>
       <c r="H10" t="n">
-        <v>938742.6875</v>
+        <v>900849.9375</v>
       </c>
       <c r="I10" t="s"/>
       <c r="J10" t="s"/>
@@ -832,18 +832,18 @@
     </row>
     <row r="11" spans="1:21">
       <c r="A11" s="1" t="n"/>
-      <c r="B11" s="1" t="n"/>
-      <c r="C11" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="C11" s="1" t="s"/>
       <c r="D11" t="s"/>
       <c r="E11" t="s"/>
       <c r="F11" t="s"/>
       <c r="G11" t="n">
-        <v>1926.5</v>
+        <v>2180.302001953125</v>
       </c>
       <c r="H11" t="n">
-        <v>90237.8359375</v>
+        <v>96634.0390625</v>
       </c>
       <c r="I11" t="s"/>
       <c r="J11" t="s"/>
@@ -861,18 +861,18 @@
     </row>
     <row r="12" spans="1:21">
       <c r="A12" s="1" t="n"/>
-      <c r="B12" s="1" t="n"/>
-      <c r="C12" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="C12" s="1" t="s"/>
       <c r="D12" t="s"/>
       <c r="E12" t="s"/>
       <c r="F12" t="s"/>
       <c r="G12" t="n">
-        <v>7105</v>
+        <v>5585.76806640625</v>
       </c>
       <c r="H12" t="n">
-        <v>174321.203125</v>
+        <v>142190.765625</v>
       </c>
       <c r="I12" t="s"/>
       <c r="J12" t="s"/>
@@ -890,18 +890,18 @@
     </row>
     <row r="13" spans="1:21">
       <c r="A13" s="1" t="n"/>
-      <c r="B13" s="1" t="n"/>
-      <c r="C13" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="C13" s="1" t="s"/>
       <c r="D13" t="s"/>
       <c r="E13" t="s"/>
       <c r="F13" t="s"/>
       <c r="G13" t="n">
-        <v>19823.5</v>
+        <v>17135.0234375</v>
       </c>
       <c r="H13" t="n">
-        <v>681201.4375</v>
+        <v>655153</v>
       </c>
       <c r="I13" t="s"/>
       <c r="J13" t="s"/>
@@ -919,18 +919,18 @@
     </row>
     <row r="14" spans="1:21">
       <c r="A14" s="1" t="n"/>
-      <c r="B14" s="1" t="n"/>
-      <c r="C14" s="1" t="s">
+      <c r="B14" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="C14" s="1" t="s"/>
       <c r="D14" t="s"/>
       <c r="E14" t="s"/>
       <c r="F14" t="s"/>
       <c r="G14" t="n">
-        <v>17686</v>
+        <v>17287.5234375</v>
       </c>
       <c r="H14" t="n">
-        <v>416378.53125</v>
+        <v>456724.625</v>
       </c>
       <c r="I14" t="s"/>
       <c r="J14" t="s"/>
@@ -948,18 +948,18 @@
     </row>
     <row r="15" spans="1:21">
       <c r="A15" s="1" t="n"/>
-      <c r="B15" s="1" t="n"/>
-      <c r="C15" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="C15" s="1" t="s"/>
       <c r="D15" t="s"/>
       <c r="E15" t="s"/>
       <c r="F15" t="s"/>
       <c r="G15" t="n">
-        <v>81512.5</v>
+        <v>68463.1796875</v>
       </c>
       <c r="H15" t="n">
-        <v>2378403.5</v>
+        <v>2323295.5</v>
       </c>
       <c r="I15" t="s"/>
       <c r="J15" t="s"/>
@@ -977,20 +977,20 @@
     </row>
     <row r="16" spans="1:21">
       <c r="A16" s="1" t="n">
-        <v>2018201903</v>
-      </c>
-      <c r="B16" s="1" t="s"/>
-      <c r="C16" s="1" t="s">
+        <v>2019202003</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="C16" s="1" t="s"/>
       <c r="D16" t="s"/>
       <c r="E16" t="s"/>
       <c r="F16" t="s"/>
       <c r="G16" t="n">
-        <v>2160.5</v>
+        <v>1722.369018554688</v>
       </c>
       <c r="H16" t="n">
-        <v>58088.03125</v>
+        <v>55559.9765625</v>
       </c>
       <c r="I16" t="s"/>
       <c r="J16" t="s"/>
@@ -1008,18 +1008,18 @@
     </row>
     <row r="17" spans="1:21">
       <c r="A17" s="1" t="n"/>
-      <c r="B17" s="1" t="n"/>
-      <c r="C17" s="1" t="s">
+      <c r="B17" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="C17" s="1" t="s"/>
       <c r="D17" t="s"/>
       <c r="E17" t="s"/>
       <c r="F17" t="s"/>
       <c r="G17" t="n">
-        <v>32687.625</v>
+        <v>28144.59765625</v>
       </c>
       <c r="H17" t="n">
-        <v>889398.5625</v>
+        <v>908492.3125</v>
       </c>
       <c r="I17" t="s"/>
       <c r="J17" t="s"/>
@@ -1037,18 +1037,18 @@
     </row>
     <row r="18" spans="1:21">
       <c r="A18" s="1" t="n"/>
-      <c r="B18" s="1" t="n"/>
-      <c r="C18" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="C18" s="1" t="s"/>
       <c r="D18" t="s"/>
       <c r="E18" t="s"/>
       <c r="F18" t="s"/>
       <c r="G18" t="n">
-        <v>2639.5</v>
+        <v>2098.39306640625</v>
       </c>
       <c r="H18" t="n">
-        <v>95119.765625</v>
+        <v>96165.4296875</v>
       </c>
       <c r="I18" t="s"/>
       <c r="J18" t="s"/>
@@ -1066,18 +1066,18 @@
     </row>
     <row r="19" spans="1:21">
       <c r="A19" s="1" t="n"/>
-      <c r="B19" s="1" t="n"/>
-      <c r="C19" s="1" t="s">
+      <c r="B19" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="C19" s="1" t="s"/>
       <c r="D19" t="s"/>
       <c r="E19" t="s"/>
       <c r="F19" t="s"/>
       <c r="G19" t="n">
-        <v>7016</v>
+        <v>6064.2109375</v>
       </c>
       <c r="H19" t="n">
-        <v>168166.90625</v>
+        <v>139014.609375</v>
       </c>
       <c r="I19" t="s"/>
       <c r="J19" t="s"/>
@@ -1095,18 +1095,18 @@
     </row>
     <row r="20" spans="1:21">
       <c r="A20" s="1" t="n"/>
-      <c r="B20" s="1" t="n"/>
-      <c r="C20" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="C20" s="1" t="s"/>
       <c r="D20" t="s"/>
       <c r="E20" t="s"/>
       <c r="F20" t="s"/>
       <c r="G20" t="n">
-        <v>22095.865234375</v>
+        <v>17369.44921875</v>
       </c>
       <c r="H20" t="n">
-        <v>674842.375</v>
+        <v>621661.875</v>
       </c>
       <c r="I20" t="s"/>
       <c r="J20" t="s"/>
@@ -1124,18 +1124,18 @@
     </row>
     <row r="21" spans="1:21">
       <c r="A21" s="1" t="n"/>
-      <c r="B21" s="1" t="n"/>
-      <c r="C21" s="1" t="s">
+      <c r="B21" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="C21" s="1" t="s"/>
       <c r="D21" t="s"/>
       <c r="E21" t="s"/>
       <c r="F21" t="s"/>
       <c r="G21" t="n">
-        <v>20327.1484375</v>
+        <v>14922.181640625</v>
       </c>
       <c r="H21" t="n">
-        <v>402526.125</v>
+        <v>479572.0625</v>
       </c>
       <c r="I21" t="s"/>
       <c r="J21" t="s"/>
@@ -1153,18 +1153,18 @@
     </row>
     <row r="22" spans="1:21">
       <c r="A22" s="1" t="n"/>
-      <c r="B22" s="1" t="n"/>
-      <c r="C22" s="1" t="s">
+      <c r="B22" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="C22" s="1" t="s"/>
       <c r="D22" t="s"/>
       <c r="E22" t="s"/>
       <c r="F22" t="s"/>
       <c r="G22" t="n">
-        <v>87201.640625</v>
+        <v>70627.203125</v>
       </c>
       <c r="H22" t="n">
-        <v>2290444.5</v>
+        <v>2308368.5</v>
       </c>
       <c r="I22" t="s"/>
       <c r="J22" t="s"/>
@@ -1182,20 +1182,20 @@
     </row>
     <row r="23" spans="1:21">
       <c r="A23" s="1" t="n">
-        <v>2018201904</v>
-      </c>
-      <c r="B23" s="1" t="s"/>
-      <c r="C23" s="1" t="s">
+        <v>2019202004</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="C23" s="1" t="s"/>
       <c r="D23" t="s"/>
       <c r="E23" t="s"/>
       <c r="F23" t="s"/>
       <c r="G23" t="n">
-        <v>2905.5</v>
+        <v>1628.041015625</v>
       </c>
       <c r="H23" t="n">
-        <v>70121.7421875</v>
+        <v>58410.75390625</v>
       </c>
       <c r="I23" t="s"/>
       <c r="J23" t="s"/>
@@ -1213,18 +1213,18 @@
     </row>
     <row r="24" spans="1:21">
       <c r="A24" s="1" t="n"/>
-      <c r="B24" s="1" t="n"/>
-      <c r="C24" s="1" t="s">
+      <c r="B24" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="C24" s="1" t="s"/>
       <c r="D24" t="s"/>
       <c r="E24" t="s"/>
       <c r="F24" t="s"/>
       <c r="G24" t="n">
-        <v>36832.046875</v>
+        <v>27226.650390625</v>
       </c>
       <c r="H24" t="n">
-        <v>903191.125</v>
+        <v>940037.875</v>
       </c>
       <c r="I24" t="s"/>
       <c r="J24" t="s"/>
@@ -1242,18 +1242,18 @@
     </row>
     <row r="25" spans="1:21">
       <c r="A25" s="1" t="n"/>
-      <c r="B25" s="1" t="n"/>
-      <c r="C25" s="1" t="s">
+      <c r="B25" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="C25" s="1" t="s"/>
       <c r="D25" t="s"/>
       <c r="E25" t="s"/>
       <c r="F25" t="s"/>
       <c r="G25" t="n">
-        <v>3399.5</v>
+        <v>3487.368896484375</v>
       </c>
       <c r="H25" t="n">
-        <v>97447.1171875</v>
+        <v>132760.125</v>
       </c>
       <c r="I25" t="s"/>
       <c r="J25" t="s"/>
@@ -1271,18 +1271,18 @@
     </row>
     <row r="26" spans="1:21">
       <c r="A26" s="1" t="n"/>
-      <c r="B26" s="1" t="n"/>
-      <c r="C26" s="1" t="s">
+      <c r="B26" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="C26" s="1" t="s"/>
       <c r="D26" t="s"/>
       <c r="E26" t="s"/>
       <c r="F26" t="s"/>
       <c r="G26" t="n">
-        <v>7854.56689453125</v>
+        <v>7391.89892578125</v>
       </c>
       <c r="H26" t="n">
-        <v>150260.3125</v>
+        <v>152723.859375</v>
       </c>
       <c r="I26" t="s"/>
       <c r="J26" t="s"/>
@@ -1300,18 +1300,18 @@
     </row>
     <row r="27" spans="1:21">
       <c r="A27" s="1" t="n"/>
-      <c r="B27" s="1" t="n"/>
-      <c r="C27" s="1" t="s">
+      <c r="B27" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="C27" s="1" t="s"/>
       <c r="D27" t="s"/>
       <c r="E27" t="s"/>
       <c r="F27" t="s"/>
       <c r="G27" t="n">
-        <v>30022.83984375</v>
+        <v>18602.90234375</v>
       </c>
       <c r="H27" t="n">
-        <v>701971.875</v>
+        <v>633689.9375</v>
       </c>
       <c r="I27" t="s"/>
       <c r="J27" t="s"/>
@@ -1329,18 +1329,18 @@
     </row>
     <row r="28" spans="1:21">
       <c r="A28" s="1" t="n"/>
-      <c r="B28" s="1" t="n"/>
-      <c r="C28" s="1" t="s">
+      <c r="B28" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="C28" s="1" t="s"/>
       <c r="D28" t="s"/>
       <c r="E28" t="s"/>
       <c r="F28" t="s"/>
       <c r="G28" t="n">
-        <v>22544.7109375</v>
+        <v>16722.365234375</v>
       </c>
       <c r="H28" t="n">
-        <v>427442.375</v>
+        <v>484801.875</v>
       </c>
       <c r="I28" t="s"/>
       <c r="J28" t="s"/>
@@ -1358,18 +1358,18 @@
     </row>
     <row r="29" spans="1:21">
       <c r="A29" s="1" t="n"/>
-      <c r="B29" s="1" t="n"/>
-      <c r="C29" s="1" t="s">
+      <c r="B29" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="C29" s="1" t="s"/>
       <c r="D29" t="s"/>
       <c r="E29" t="s"/>
       <c r="F29" t="s"/>
       <c r="G29" t="n">
-        <v>103683.1640625</v>
+        <v>75484.2265625</v>
       </c>
       <c r="H29" t="n">
-        <v>2354051</v>
+        <v>2409430</v>
       </c>
       <c r="I29" t="s"/>
       <c r="J29" t="s"/>
@@ -1387,20 +1387,20 @@
     </row>
     <row r="30" spans="1:21">
       <c r="A30" s="1" t="n">
-        <v>2018201905</v>
-      </c>
-      <c r="B30" s="1" t="s"/>
-      <c r="C30" s="1" t="s">
+        <v>2019202005</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="C30" s="1" t="s"/>
       <c r="D30" t="s"/>
       <c r="E30" t="s"/>
       <c r="F30" t="s"/>
       <c r="G30" t="n">
-        <v>1598.5</v>
+        <v>1674.829956054688</v>
       </c>
       <c r="H30" t="n">
-        <v>67051.984375</v>
+        <v>55063.25390625</v>
       </c>
       <c r="I30" t="s"/>
       <c r="J30" t="s"/>
@@ -1418,18 +1418,18 @@
     </row>
     <row r="31" spans="1:21">
       <c r="A31" s="1" t="n"/>
-      <c r="B31" s="1" t="n"/>
-      <c r="C31" s="1" t="s">
+      <c r="B31" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="C31" s="1" t="s"/>
       <c r="D31" t="s"/>
       <c r="E31" t="s"/>
       <c r="F31" t="s"/>
       <c r="G31" t="n">
-        <v>32199.1015625</v>
+        <v>34284.3515625</v>
       </c>
       <c r="H31" t="n">
-        <v>847716.6875</v>
+        <v>863191</v>
       </c>
       <c r="I31" t="s"/>
       <c r="J31" t="s"/>
@@ -1447,18 +1447,18 @@
     </row>
     <row r="32" spans="1:21">
       <c r="A32" s="1" t="n"/>
-      <c r="B32" s="1" t="n"/>
-      <c r="C32" s="1" t="s">
+      <c r="B32" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="C32" s="1" t="s"/>
       <c r="D32" t="s"/>
       <c r="E32" t="s"/>
       <c r="F32" t="s"/>
       <c r="G32" t="n">
-        <v>1662.984985351562</v>
+        <v>7108.7431640625</v>
       </c>
       <c r="H32" t="n">
-        <v>93476.078125</v>
+        <v>135978.84375</v>
       </c>
       <c r="I32" t="s"/>
       <c r="J32" t="s"/>
@@ -1476,18 +1476,18 @@
     </row>
     <row r="33" spans="1:21">
       <c r="A33" s="1" t="n"/>
-      <c r="B33" s="1" t="n"/>
-      <c r="C33" s="1" t="s">
+      <c r="B33" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="C33" s="1" t="s"/>
       <c r="D33" t="s"/>
       <c r="E33" t="s"/>
       <c r="F33" t="s"/>
       <c r="G33" t="n">
-        <v>6239</v>
+        <v>7573.36376953125</v>
       </c>
       <c r="H33" t="n">
-        <v>147110.28125</v>
+        <v>130492.015625</v>
       </c>
       <c r="I33" t="s"/>
       <c r="J33" t="s"/>
@@ -1505,18 +1505,18 @@
     </row>
     <row r="34" spans="1:21">
       <c r="A34" s="1" t="n"/>
-      <c r="B34" s="1" t="n"/>
-      <c r="C34" s="1" t="s">
+      <c r="B34" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="C34" s="1" t="s"/>
       <c r="D34" t="s"/>
       <c r="E34" t="s"/>
       <c r="F34" t="s"/>
       <c r="G34" t="n">
-        <v>32101.33984375</v>
+        <v>24580.046875</v>
       </c>
       <c r="H34" t="n">
-        <v>688156.25</v>
+        <v>616340.5</v>
       </c>
       <c r="I34" t="s"/>
       <c r="J34" t="s"/>
@@ -1534,18 +1534,18 @@
     </row>
     <row r="35" spans="1:21">
       <c r="A35" s="1" t="n"/>
-      <c r="B35" s="1" t="n"/>
-      <c r="C35" s="1" t="s">
+      <c r="B35" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="C35" s="1" t="s"/>
       <c r="D35" t="s"/>
       <c r="E35" t="s"/>
       <c r="F35" t="s"/>
       <c r="G35" t="n">
-        <v>22808</v>
+        <v>22663.013671875</v>
       </c>
       <c r="H35" t="n">
-        <v>431512.53125</v>
+        <v>453371.5</v>
       </c>
       <c r="I35" t="s"/>
       <c r="J35" t="s"/>
@@ -1563,18 +1563,18 @@
     </row>
     <row r="36" spans="1:21">
       <c r="A36" s="1" t="n"/>
-      <c r="B36" s="1" t="n"/>
-      <c r="C36" s="1" t="s">
+      <c r="B36" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="C36" s="1" t="s"/>
       <c r="D36" t="s"/>
       <c r="E36" t="s"/>
       <c r="F36" t="s"/>
       <c r="G36" t="n">
-        <v>96847.9296875</v>
+        <v>98413.34375</v>
       </c>
       <c r="H36" t="n">
-        <v>2277824</v>
+        <v>2265295.5</v>
       </c>
       <c r="I36" t="s"/>
       <c r="J36" t="s"/>
@@ -1592,20 +1592,20 @@
     </row>
     <row r="37" spans="1:21">
       <c r="A37" s="1" t="n">
-        <v>2018201906</v>
-      </c>
-      <c r="B37" s="1" t="s"/>
-      <c r="C37" s="1" t="s">
+        <v>2019202006</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="C37" s="1" t="s"/>
       <c r="D37" t="s"/>
       <c r="E37" t="s"/>
       <c r="F37" t="s"/>
       <c r="G37" t="n">
-        <v>2635.5</v>
+        <v>1117.740966796875</v>
       </c>
       <c r="H37" t="n">
-        <v>72434.046875</v>
+        <v>55899.56640625</v>
       </c>
       <c r="I37" t="s"/>
       <c r="J37" t="s"/>
@@ -1623,18 +1623,18 @@
     </row>
     <row r="38" spans="1:21">
       <c r="A38" s="1" t="n"/>
-      <c r="B38" s="1" t="n"/>
-      <c r="C38" s="1" t="s">
+      <c r="B38" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="C38" s="1" t="s"/>
       <c r="D38" t="s"/>
       <c r="E38" t="s"/>
       <c r="F38" t="s"/>
       <c r="G38" t="n">
-        <v>26271.400390625</v>
+        <v>22961.87890625</v>
       </c>
       <c r="H38" t="n">
-        <v>881453.5</v>
+        <v>904859.75</v>
       </c>
       <c r="I38" t="s"/>
       <c r="J38" t="s"/>
@@ -1652,18 +1652,18 @@
     </row>
     <row r="39" spans="1:21">
       <c r="A39" s="1" t="n"/>
-      <c r="B39" s="1" t="n"/>
-      <c r="C39" s="1" t="s">
+      <c r="B39" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="C39" s="1" t="s"/>
       <c r="D39" t="s"/>
       <c r="E39" t="s"/>
       <c r="F39" t="s"/>
       <c r="G39" t="n">
-        <v>1334</v>
+        <v>3174.431884765625</v>
       </c>
       <c r="H39" t="n">
-        <v>96437.6875</v>
+        <v>144902.59375</v>
       </c>
       <c r="I39" t="s"/>
       <c r="J39" t="s"/>
@@ -1681,18 +1681,18 @@
     </row>
     <row r="40" spans="1:21">
       <c r="A40" s="1" t="n"/>
-      <c r="B40" s="1" t="n"/>
-      <c r="C40" s="1" t="s">
+      <c r="B40" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="C40" s="1" t="s"/>
       <c r="D40" t="s"/>
       <c r="E40" t="s"/>
       <c r="F40" t="s"/>
       <c r="G40" t="n">
-        <v>4983.31005859375</v>
+        <v>6561.40478515625</v>
       </c>
       <c r="H40" t="n">
-        <v>164134.546875</v>
+        <v>133770.265625</v>
       </c>
       <c r="I40" t="s"/>
       <c r="J40" t="s"/>
@@ -1710,18 +1710,18 @@
     </row>
     <row r="41" spans="1:21">
       <c r="A41" s="1" t="n"/>
-      <c r="B41" s="1" t="n"/>
-      <c r="C41" s="1" t="s">
+      <c r="B41" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="C41" s="1" t="s"/>
       <c r="D41" t="s"/>
       <c r="E41" t="s"/>
       <c r="F41" t="s"/>
       <c r="G41" t="n">
-        <v>20084.267578125</v>
+        <v>17776.931640625</v>
       </c>
       <c r="H41" t="n">
-        <v>650669.3125</v>
+        <v>613752.1875</v>
       </c>
       <c r="I41" t="s"/>
       <c r="J41" t="s"/>
@@ -1739,18 +1739,18 @@
     </row>
     <row r="42" spans="1:21">
       <c r="A42" s="1" t="n"/>
-      <c r="B42" s="1" t="n"/>
-      <c r="C42" s="1" t="s">
+      <c r="B42" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="C42" s="1" t="s"/>
       <c r="D42" t="s"/>
       <c r="E42" t="s"/>
       <c r="F42" t="s"/>
       <c r="G42" t="n">
-        <v>19055.80078125</v>
+        <v>17114.26171875</v>
       </c>
       <c r="H42" t="n">
-        <v>467116.25</v>
+        <v>463333.375</v>
       </c>
       <c r="I42" t="s"/>
       <c r="J42" t="s"/>
@@ -1768,18 +1768,18 @@
     </row>
     <row r="43" spans="1:21">
       <c r="A43" s="1" t="n"/>
-      <c r="B43" s="1" t="n"/>
-      <c r="C43" s="1" t="s">
+      <c r="B43" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="C43" s="1" t="s"/>
       <c r="D43" t="s"/>
       <c r="E43" t="s"/>
       <c r="F43" t="s"/>
       <c r="G43" t="n">
-        <v>74777.78125</v>
+        <v>69080.6484375</v>
       </c>
       <c r="H43" t="n">
-        <v>2338246.75</v>
+        <v>2323086</v>
       </c>
       <c r="I43" t="s"/>
       <c r="J43" t="s"/>
@@ -1797,20 +1797,20 @@
     </row>
     <row r="44" spans="1:21">
       <c r="A44" s="1" t="n">
-        <v>2018201907</v>
-      </c>
-      <c r="B44" s="1" t="s"/>
-      <c r="C44" s="1" t="s">
+        <v>2019202007</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="C44" s="1" t="s"/>
       <c r="D44" t="s"/>
       <c r="E44" t="s"/>
       <c r="F44" t="s"/>
       <c r="G44" t="n">
-        <v>2788.35595703125</v>
+        <v>1039.89697265625</v>
       </c>
       <c r="H44" t="n">
-        <v>64237.8984375</v>
+        <v>51477.0390625</v>
       </c>
       <c r="I44" t="s"/>
       <c r="J44" t="s"/>
@@ -1828,18 +1828,18 @@
     </row>
     <row r="45" spans="1:21">
       <c r="A45" s="1" t="n"/>
-      <c r="B45" s="1" t="n"/>
-      <c r="C45" s="1" t="s">
+      <c r="B45" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="C45" s="1" t="s"/>
       <c r="D45" t="s"/>
       <c r="E45" t="s"/>
       <c r="F45" t="s"/>
       <c r="G45" t="n">
-        <v>38255.88671875</v>
+        <v>27668.080078125</v>
       </c>
       <c r="H45" t="n">
-        <v>915260.0625</v>
+        <v>924610.25</v>
       </c>
       <c r="I45" t="s"/>
       <c r="J45" t="s"/>
@@ -1857,18 +1857,18 @@
     </row>
     <row r="46" spans="1:21">
       <c r="A46" s="1" t="n"/>
-      <c r="B46" s="1" t="n"/>
-      <c r="C46" s="1" t="s">
+      <c r="B46" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="C46" s="1" t="s"/>
       <c r="D46" t="s"/>
       <c r="E46" t="s"/>
       <c r="F46" t="s"/>
       <c r="G46" t="n">
-        <v>6288</v>
+        <v>2099.591064453125</v>
       </c>
       <c r="H46" t="n">
-        <v>98271.03125</v>
+        <v>139688.171875</v>
       </c>
       <c r="I46" t="s"/>
       <c r="J46" t="s"/>
@@ -1886,18 +1886,18 @@
     </row>
     <row r="47" spans="1:21">
       <c r="A47" s="1" t="n"/>
-      <c r="B47" s="1" t="n"/>
-      <c r="C47" s="1" t="s">
+      <c r="B47" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="C47" s="1" t="s"/>
       <c r="D47" t="s"/>
       <c r="E47" t="s"/>
       <c r="F47" t="s"/>
       <c r="G47" t="n">
-        <v>8036.5</v>
+        <v>7425.51416015625</v>
       </c>
       <c r="H47" t="n">
-        <v>156371.453125</v>
+        <v>134571.5625</v>
       </c>
       <c r="I47" t="s"/>
       <c r="J47" t="s"/>
@@ -1915,18 +1915,18 @@
     </row>
     <row r="48" spans="1:21">
       <c r="A48" s="1" t="n"/>
-      <c r="B48" s="1" t="n"/>
-      <c r="C48" s="1" t="s">
+      <c r="B48" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="C48" s="1" t="s"/>
       <c r="D48" t="s"/>
       <c r="E48" t="s"/>
       <c r="F48" t="s"/>
       <c r="G48" t="n">
-        <v>31406.876953125</v>
+        <v>22409.703125</v>
       </c>
       <c r="H48" t="n">
-        <v>669377.375</v>
+        <v>643245.1875</v>
       </c>
       <c r="I48" t="s"/>
       <c r="J48" t="s"/>
@@ -1944,18 +1944,18 @@
     </row>
     <row r="49" spans="1:21">
       <c r="A49" s="1" t="n"/>
-      <c r="B49" s="1" t="n"/>
-      <c r="C49" s="1" t="s">
+      <c r="B49" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="C49" s="1" t="s"/>
       <c r="D49" t="s"/>
       <c r="E49" t="s"/>
       <c r="F49" t="s"/>
       <c r="G49" t="n">
-        <v>36561.9921875</v>
+        <v>20054.080078125</v>
       </c>
       <c r="H49" t="n">
-        <v>511708.28125</v>
+        <v>442925.90625</v>
       </c>
       <c r="I49" t="s"/>
       <c r="J49" t="s"/>
@@ -1973,18 +1973,18 @@
     </row>
     <row r="50" spans="1:21">
       <c r="A50" s="1" t="n"/>
-      <c r="B50" s="1" t="n"/>
-      <c r="C50" s="1" t="s">
+      <c r="B50" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="C50" s="1" t="s"/>
       <c r="D50" t="s"/>
       <c r="E50" t="s"/>
       <c r="F50" t="s"/>
       <c r="G50" t="n">
-        <v>123846.109375</v>
+        <v>80931.734375</v>
       </c>
       <c r="H50" t="n">
-        <v>2422237</v>
+        <v>2341969.25</v>
       </c>
       <c r="I50" t="s"/>
       <c r="J50" t="s"/>
@@ -2000,213 +2000,8 @@
       <c r="T50" t="s"/>
       <c r="U50" t="s"/>
     </row>
-    <row r="51" spans="1:21">
-      <c r="A51" s="1" t="n">
-        <v>2018201908</v>
-      </c>
-      <c r="B51" s="1" t="s"/>
-      <c r="C51" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D51" t="s"/>
-      <c r="E51" t="s"/>
-      <c r="F51" t="s"/>
-      <c r="G51" t="n">
-        <v>1652</v>
-      </c>
-      <c r="H51" t="n">
-        <v>70021.1875</v>
-      </c>
-      <c r="I51" t="s"/>
-      <c r="J51" t="s"/>
-      <c r="K51" t="s"/>
-      <c r="L51" t="s"/>
-      <c r="M51" t="s"/>
-      <c r="N51" t="s"/>
-      <c r="O51" t="s"/>
-      <c r="P51" t="s"/>
-      <c r="Q51" t="s"/>
-      <c r="R51" t="s"/>
-      <c r="S51" t="s"/>
-      <c r="T51" t="s"/>
-      <c r="U51" t="s"/>
-    </row>
-    <row r="52" spans="1:21">
-      <c r="A52" s="1" t="n"/>
-      <c r="B52" s="1" t="n"/>
-      <c r="C52" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D52" t="s"/>
-      <c r="E52" t="s"/>
-      <c r="F52" t="s"/>
-      <c r="G52" t="n">
-        <v>33008.4375</v>
-      </c>
-      <c r="H52" t="n">
-        <v>922584.625</v>
-      </c>
-      <c r="I52" t="s"/>
-      <c r="J52" t="s"/>
-      <c r="K52" t="s"/>
-      <c r="L52" t="s"/>
-      <c r="M52" t="s"/>
-      <c r="N52" t="s"/>
-      <c r="O52" t="s"/>
-      <c r="P52" t="s"/>
-      <c r="Q52" t="s"/>
-      <c r="R52" t="s"/>
-      <c r="S52" t="s"/>
-      <c r="T52" t="s"/>
-      <c r="U52" t="s"/>
-    </row>
-    <row r="53" spans="1:21">
-      <c r="A53" s="1" t="n"/>
-      <c r="B53" s="1" t="n"/>
-      <c r="C53" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D53" t="s"/>
-      <c r="E53" t="s"/>
-      <c r="F53" t="s"/>
-      <c r="G53" t="n">
-        <v>2706</v>
-      </c>
-      <c r="H53" t="n">
-        <v>101066.03125</v>
-      </c>
-      <c r="I53" t="s"/>
-      <c r="J53" t="s"/>
-      <c r="K53" t="s"/>
-      <c r="L53" t="s"/>
-      <c r="M53" t="s"/>
-      <c r="N53" t="s"/>
-      <c r="O53" t="s"/>
-      <c r="P53" t="s"/>
-      <c r="Q53" t="s"/>
-      <c r="R53" t="s"/>
-      <c r="S53" t="s"/>
-      <c r="T53" t="s"/>
-      <c r="U53" t="s"/>
-    </row>
-    <row r="54" spans="1:21">
-      <c r="A54" s="1" t="n"/>
-      <c r="B54" s="1" t="n"/>
-      <c r="C54" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D54" t="s"/>
-      <c r="E54" t="s"/>
-      <c r="F54" t="s"/>
-      <c r="G54" t="n">
-        <v>8600.728515625</v>
-      </c>
-      <c r="H54" t="n">
-        <v>157653.25</v>
-      </c>
-      <c r="I54" t="s"/>
-      <c r="J54" t="s"/>
-      <c r="K54" t="s"/>
-      <c r="L54" t="s"/>
-      <c r="M54" t="s"/>
-      <c r="N54" t="s"/>
-      <c r="O54" t="s"/>
-      <c r="P54" t="s"/>
-      <c r="Q54" t="s"/>
-      <c r="R54" t="s"/>
-      <c r="S54" t="s"/>
-      <c r="T54" t="s"/>
-      <c r="U54" t="s"/>
-    </row>
-    <row r="55" spans="1:21">
-      <c r="A55" s="1" t="n"/>
-      <c r="B55" s="1" t="n"/>
-      <c r="C55" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D55" t="s"/>
-      <c r="E55" t="s"/>
-      <c r="F55" t="s"/>
-      <c r="G55" t="n">
-        <v>27178.705078125</v>
-      </c>
-      <c r="H55" t="n">
-        <v>673084.125</v>
-      </c>
-      <c r="I55" t="s"/>
-      <c r="J55" t="s"/>
-      <c r="K55" t="s"/>
-      <c r="L55" t="s"/>
-      <c r="M55" t="s"/>
-      <c r="N55" t="s"/>
-      <c r="O55" t="s"/>
-      <c r="P55" t="s"/>
-      <c r="Q55" t="s"/>
-      <c r="R55" t="s"/>
-      <c r="S55" t="s"/>
-      <c r="T55" t="s"/>
-      <c r="U55" t="s"/>
-    </row>
-    <row r="56" spans="1:21">
-      <c r="A56" s="1" t="n"/>
-      <c r="B56" s="1" t="n"/>
-      <c r="C56" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D56" t="s"/>
-      <c r="E56" t="s"/>
-      <c r="F56" t="s"/>
-      <c r="G56" t="n">
-        <v>26563.646484375</v>
-      </c>
-      <c r="H56" t="n">
-        <v>521973.59375</v>
-      </c>
-      <c r="I56" t="s"/>
-      <c r="J56" t="s"/>
-      <c r="K56" t="s"/>
-      <c r="L56" t="s"/>
-      <c r="M56" t="s"/>
-      <c r="N56" t="s"/>
-      <c r="O56" t="s"/>
-      <c r="P56" t="s"/>
-      <c r="Q56" t="s"/>
-      <c r="R56" t="s"/>
-      <c r="S56" t="s"/>
-      <c r="T56" t="s"/>
-      <c r="U56" t="s"/>
-    </row>
-    <row r="57" spans="1:21">
-      <c r="A57" s="1" t="n"/>
-      <c r="B57" s="1" t="n"/>
-      <c r="C57" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D57" t="s"/>
-      <c r="E57" t="s"/>
-      <c r="F57" t="s"/>
-      <c r="G57" t="n">
-        <v>100130.015625</v>
-      </c>
-      <c r="H57" t="n">
-        <v>2452644.25</v>
-      </c>
-      <c r="I57" t="s"/>
-      <c r="J57" t="s"/>
-      <c r="K57" t="s"/>
-      <c r="L57" t="s"/>
-      <c r="M57" t="s"/>
-      <c r="N57" t="s"/>
-      <c r="O57" t="s"/>
-      <c r="P57" t="s"/>
-      <c r="Q57" t="s"/>
-      <c r="R57" t="s"/>
-      <c r="S57" t="s"/>
-      <c r="T57" t="s"/>
-      <c r="U57" t="s"/>
-    </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="7">
     <mergeCell ref="A2:A8"/>
     <mergeCell ref="A9:A15"/>
     <mergeCell ref="A16:A22"/>
@@ -2214,15 +2009,6 @@
     <mergeCell ref="A30:A36"/>
     <mergeCell ref="A37:A43"/>
     <mergeCell ref="A44:A50"/>
-    <mergeCell ref="A51:A57"/>
-    <mergeCell ref="B2:B8"/>
-    <mergeCell ref="B9:B15"/>
-    <mergeCell ref="B16:B22"/>
-    <mergeCell ref="B23:B29"/>
-    <mergeCell ref="B30:B36"/>
-    <mergeCell ref="B37:B43"/>
-    <mergeCell ref="B44:B50"/>
-    <mergeCell ref="B51:B57"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
@@ -2309,20 +2095,20 @@
     </row>
     <row r="2" spans="1:21">
       <c r="A2" s="1" t="n">
-        <v>2018201901</v>
-      </c>
-      <c r="B2" s="1" t="s"/>
-      <c r="C2" s="1" t="s">
+        <v>2019202001</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="C2" s="1" t="s"/>
       <c r="D2" t="s"/>
       <c r="E2" t="s"/>
       <c r="F2" t="s"/>
       <c r="G2" t="n">
-        <v>2568.5</v>
+        <v>1225.475952148438</v>
       </c>
       <c r="H2" t="n">
-        <v>78433.828125</v>
+        <v>53692.3671875</v>
       </c>
       <c r="I2" t="s"/>
       <c r="J2" t="s"/>
@@ -2340,18 +2126,18 @@
     </row>
     <row r="3" spans="1:21">
       <c r="A3" s="1" t="n"/>
-      <c r="B3" s="1" t="n"/>
-      <c r="C3" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="C3" s="1" t="s"/>
       <c r="D3" t="s"/>
       <c r="E3" t="s"/>
       <c r="F3" t="s"/>
       <c r="G3" t="n">
-        <v>34146.5</v>
+        <v>24299.642578125</v>
       </c>
       <c r="H3" t="n">
-        <v>940600.5625</v>
+        <v>840809.9375</v>
       </c>
       <c r="I3" t="s"/>
       <c r="J3" t="s"/>
@@ -2369,18 +2155,18 @@
     </row>
     <row r="4" spans="1:21">
       <c r="A4" s="1" t="n"/>
-      <c r="B4" s="1" t="n"/>
-      <c r="C4" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="C4" s="1" t="s"/>
       <c r="D4" t="s"/>
       <c r="E4" t="s"/>
       <c r="F4" t="s"/>
       <c r="G4" t="n">
-        <v>2088</v>
+        <v>1460.93505859375</v>
       </c>
       <c r="H4" t="n">
-        <v>89638.578125</v>
+        <v>94161.609375</v>
       </c>
       <c r="I4" t="s"/>
       <c r="J4" t="s"/>
@@ -2398,18 +2184,18 @@
     </row>
     <row r="5" spans="1:21">
       <c r="A5" s="1" t="n"/>
-      <c r="B5" s="1" t="n"/>
-      <c r="C5" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="C5" s="1" t="s"/>
       <c r="D5" t="s"/>
       <c r="E5" t="s"/>
       <c r="F5" t="s"/>
       <c r="G5" t="n">
-        <v>6161.5</v>
+        <v>5137.1650390625</v>
       </c>
       <c r="H5" t="n">
-        <v>154372.921875</v>
+        <v>162021.828125</v>
       </c>
       <c r="I5" t="s"/>
       <c r="J5" t="s"/>
@@ -2427,18 +2213,18 @@
     </row>
     <row r="6" spans="1:21">
       <c r="A6" s="1" t="n"/>
-      <c r="B6" s="1" t="n"/>
-      <c r="C6" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="C6" s="1" t="s"/>
       <c r="D6" t="s"/>
       <c r="E6" t="s"/>
       <c r="F6" t="s"/>
       <c r="G6" t="n">
-        <v>21521</v>
+        <v>14684.859375</v>
       </c>
       <c r="H6" t="n">
-        <v>679445.0625</v>
+        <v>630008.375</v>
       </c>
       <c r="I6" t="s"/>
       <c r="J6" t="s"/>
@@ -2456,18 +2242,18 @@
     </row>
     <row r="7" spans="1:21">
       <c r="A7" s="1" t="n"/>
-      <c r="B7" s="1" t="n"/>
-      <c r="C7" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="C7" s="1" t="s"/>
       <c r="D7" t="s"/>
       <c r="E7" t="s"/>
       <c r="F7" t="s"/>
       <c r="G7" t="n">
-        <v>17175</v>
+        <v>16902.26953125</v>
       </c>
       <c r="H7" t="n">
-        <v>400602.4375</v>
+        <v>459627.34375</v>
       </c>
       <c r="I7" t="s"/>
       <c r="J7" t="s"/>
@@ -2485,18 +2271,18 @@
     </row>
     <row r="8" spans="1:21">
       <c r="A8" s="1" t="n"/>
-      <c r="B8" s="1" t="n"/>
-      <c r="C8" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="C8" s="1" t="s"/>
       <c r="D8" t="s"/>
       <c r="E8" t="s"/>
       <c r="F8" t="s"/>
       <c r="G8" t="n">
-        <v>84265.5</v>
+        <v>64169.34765625</v>
       </c>
       <c r="H8" t="n">
-        <v>2346576.5</v>
+        <v>2251425.25</v>
       </c>
       <c r="I8" t="s"/>
       <c r="J8" t="s"/>
@@ -2514,20 +2300,20 @@
     </row>
     <row r="9" spans="1:21">
       <c r="A9" s="1" t="n">
-        <v>2018201902</v>
-      </c>
-      <c r="B9" s="1" t="s"/>
-      <c r="C9" s="1" t="s">
+        <v>2019202002</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="C9" s="1" t="s"/>
       <c r="D9" t="s"/>
       <c r="E9" t="s"/>
       <c r="F9" t="s"/>
       <c r="G9" t="n">
-        <v>2096</v>
+        <v>1998.159057617188</v>
       </c>
       <c r="H9" t="n">
-        <v>76520.640625</v>
+        <v>59987.203125</v>
       </c>
       <c r="I9" t="s"/>
       <c r="J9" t="s"/>
@@ -2545,18 +2331,18 @@
     </row>
     <row r="10" spans="1:21">
       <c r="A10" s="1" t="n"/>
-      <c r="B10" s="1" t="n"/>
-      <c r="C10" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="C10" s="1" t="s"/>
       <c r="D10" t="s"/>
       <c r="E10" t="s"/>
       <c r="F10" t="s"/>
       <c r="G10" t="n">
-        <v>32796.5</v>
+        <v>23819.220703125</v>
       </c>
       <c r="H10" t="n">
-        <v>938742.6875</v>
+        <v>900849.9375</v>
       </c>
       <c r="I10" t="s"/>
       <c r="J10" t="s"/>
@@ -2574,18 +2360,18 @@
     </row>
     <row r="11" spans="1:21">
       <c r="A11" s="1" t="n"/>
-      <c r="B11" s="1" t="n"/>
-      <c r="C11" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="C11" s="1" t="s"/>
       <c r="D11" t="s"/>
       <c r="E11" t="s"/>
       <c r="F11" t="s"/>
       <c r="G11" t="n">
-        <v>1926.5</v>
+        <v>2180.302001953125</v>
       </c>
       <c r="H11" t="n">
-        <v>90237.8359375</v>
+        <v>96634.0390625</v>
       </c>
       <c r="I11" t="s"/>
       <c r="J11" t="s"/>
@@ -2603,18 +2389,18 @@
     </row>
     <row r="12" spans="1:21">
       <c r="A12" s="1" t="n"/>
-      <c r="B12" s="1" t="n"/>
-      <c r="C12" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="C12" s="1" t="s"/>
       <c r="D12" t="s"/>
       <c r="E12" t="s"/>
       <c r="F12" t="s"/>
       <c r="G12" t="n">
-        <v>7105</v>
+        <v>5585.76806640625</v>
       </c>
       <c r="H12" t="n">
-        <v>174321.203125</v>
+        <v>142190.765625</v>
       </c>
       <c r="I12" t="s"/>
       <c r="J12" t="s"/>
@@ -2632,18 +2418,18 @@
     </row>
     <row r="13" spans="1:21">
       <c r="A13" s="1" t="n"/>
-      <c r="B13" s="1" t="n"/>
-      <c r="C13" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="C13" s="1" t="s"/>
       <c r="D13" t="s"/>
       <c r="E13" t="s"/>
       <c r="F13" t="s"/>
       <c r="G13" t="n">
-        <v>19823.5</v>
+        <v>17140.5234375</v>
       </c>
       <c r="H13" t="n">
-        <v>681201.4375</v>
+        <v>655153</v>
       </c>
       <c r="I13" t="s"/>
       <c r="J13" t="s"/>
@@ -2661,18 +2447,18 @@
     </row>
     <row r="14" spans="1:21">
       <c r="A14" s="1" t="n"/>
-      <c r="B14" s="1" t="n"/>
-      <c r="C14" s="1" t="s">
+      <c r="B14" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="C14" s="1" t="s"/>
       <c r="D14" t="s"/>
       <c r="E14" t="s"/>
       <c r="F14" t="s"/>
       <c r="G14" t="n">
-        <v>17686</v>
+        <v>17290.0234375</v>
       </c>
       <c r="H14" t="n">
-        <v>416378.53125</v>
+        <v>456724.625</v>
       </c>
       <c r="I14" t="s"/>
       <c r="J14" t="s"/>
@@ -2690,18 +2476,18 @@
     </row>
     <row r="15" spans="1:21">
       <c r="A15" s="1" t="n"/>
-      <c r="B15" s="1" t="n"/>
-      <c r="C15" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="C15" s="1" t="s"/>
       <c r="D15" t="s"/>
       <c r="E15" t="s"/>
       <c r="F15" t="s"/>
       <c r="G15" t="n">
-        <v>81512.5</v>
+        <v>68472.4921875</v>
       </c>
       <c r="H15" t="n">
-        <v>2378403.5</v>
+        <v>2323295.5</v>
       </c>
       <c r="I15" t="s"/>
       <c r="J15" t="s"/>
@@ -2719,20 +2505,20 @@
     </row>
     <row r="16" spans="1:21">
       <c r="A16" s="1" t="n">
-        <v>2018201903</v>
-      </c>
-      <c r="B16" s="1" t="s"/>
-      <c r="C16" s="1" t="s">
+        <v>2019202003</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="C16" s="1" t="s"/>
       <c r="D16" t="s"/>
       <c r="E16" t="s"/>
       <c r="F16" t="s"/>
       <c r="G16" t="n">
-        <v>2160.5</v>
+        <v>1721.984008789062</v>
       </c>
       <c r="H16" t="n">
-        <v>58088.03125</v>
+        <v>55559.9765625</v>
       </c>
       <c r="I16" t="s"/>
       <c r="J16" t="s"/>
@@ -2750,18 +2536,18 @@
     </row>
     <row r="17" spans="1:21">
       <c r="A17" s="1" t="n"/>
-      <c r="B17" s="1" t="n"/>
-      <c r="C17" s="1" t="s">
+      <c r="B17" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="C17" s="1" t="s"/>
       <c r="D17" t="s"/>
       <c r="E17" t="s"/>
       <c r="F17" t="s"/>
       <c r="G17" t="n">
-        <v>32687.625</v>
+        <v>28098.46875</v>
       </c>
       <c r="H17" t="n">
-        <v>889398.5625</v>
+        <v>908492.3125</v>
       </c>
       <c r="I17" t="s"/>
       <c r="J17" t="s"/>
@@ -2779,18 +2565,18 @@
     </row>
     <row r="18" spans="1:21">
       <c r="A18" s="1" t="n"/>
-      <c r="B18" s="1" t="n"/>
-      <c r="C18" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="C18" s="1" t="s"/>
       <c r="D18" t="s"/>
       <c r="E18" t="s"/>
       <c r="F18" t="s"/>
       <c r="G18" t="n">
-        <v>2639.5</v>
+        <v>2098.39306640625</v>
       </c>
       <c r="H18" t="n">
-        <v>95119.765625</v>
+        <v>96165.4296875</v>
       </c>
       <c r="I18" t="s"/>
       <c r="J18" t="s"/>
@@ -2808,18 +2594,18 @@
     </row>
     <row r="19" spans="1:21">
       <c r="A19" s="1" t="n"/>
-      <c r="B19" s="1" t="n"/>
-      <c r="C19" s="1" t="s">
+      <c r="B19" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="C19" s="1" t="s"/>
       <c r="D19" t="s"/>
       <c r="E19" t="s"/>
       <c r="F19" t="s"/>
       <c r="G19" t="n">
-        <v>7016</v>
+        <v>6064.166015625</v>
       </c>
       <c r="H19" t="n">
-        <v>168166.90625</v>
+        <v>139014.609375</v>
       </c>
       <c r="I19" t="s"/>
       <c r="J19" t="s"/>
@@ -2837,18 +2623,18 @@
     </row>
     <row r="20" spans="1:21">
       <c r="A20" s="1" t="n"/>
-      <c r="B20" s="1" t="n"/>
-      <c r="C20" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="C20" s="1" t="s"/>
       <c r="D20" t="s"/>
       <c r="E20" t="s"/>
       <c r="F20" t="s"/>
       <c r="G20" t="n">
-        <v>22095.865234375</v>
+        <v>17379.837890625</v>
       </c>
       <c r="H20" t="n">
-        <v>674842.375</v>
+        <v>621661.875</v>
       </c>
       <c r="I20" t="s"/>
       <c r="J20" t="s"/>
@@ -2866,18 +2652,18 @@
     </row>
     <row r="21" spans="1:21">
       <c r="A21" s="1" t="n"/>
-      <c r="B21" s="1" t="n"/>
-      <c r="C21" s="1" t="s">
+      <c r="B21" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="C21" s="1" t="s"/>
       <c r="D21" t="s"/>
       <c r="E21" t="s"/>
       <c r="F21" t="s"/>
       <c r="G21" t="n">
-        <v>20327.1484375</v>
+        <v>14917.8935546875</v>
       </c>
       <c r="H21" t="n">
-        <v>402526.125</v>
+        <v>479572.0625</v>
       </c>
       <c r="I21" t="s"/>
       <c r="J21" t="s"/>
@@ -2895,18 +2681,18 @@
     </row>
     <row r="22" spans="1:21">
       <c r="A22" s="1" t="n"/>
-      <c r="B22" s="1" t="n"/>
-      <c r="C22" s="1" t="s">
+      <c r="B22" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="C22" s="1" t="s"/>
       <c r="D22" t="s"/>
       <c r="E22" t="s"/>
       <c r="F22" t="s"/>
       <c r="G22" t="n">
-        <v>87201.640625</v>
+        <v>70586.7421875</v>
       </c>
       <c r="H22" t="n">
-        <v>2290444.5</v>
+        <v>2308368.5</v>
       </c>
       <c r="I22" t="s"/>
       <c r="J22" t="s"/>
@@ -2924,20 +2710,20 @@
     </row>
     <row r="23" spans="1:21">
       <c r="A23" s="1" t="n">
-        <v>2018201904</v>
-      </c>
-      <c r="B23" s="1" t="s"/>
-      <c r="C23" s="1" t="s">
+        <v>2019202004</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="C23" s="1" t="s"/>
       <c r="D23" t="s"/>
       <c r="E23" t="s"/>
       <c r="F23" t="s"/>
       <c r="G23" t="n">
-        <v>2905.5</v>
+        <v>1628.041015625</v>
       </c>
       <c r="H23" t="n">
-        <v>70121.7421875</v>
+        <v>58410.75390625</v>
       </c>
       <c r="I23" t="s"/>
       <c r="J23" t="s"/>
@@ -2955,18 +2741,18 @@
     </row>
     <row r="24" spans="1:21">
       <c r="A24" s="1" t="n"/>
-      <c r="B24" s="1" t="n"/>
-      <c r="C24" s="1" t="s">
+      <c r="B24" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="C24" s="1" t="s"/>
       <c r="D24" t="s"/>
       <c r="E24" t="s"/>
       <c r="F24" t="s"/>
       <c r="G24" t="n">
-        <v>36831.11328125</v>
+        <v>27287.68359375</v>
       </c>
       <c r="H24" t="n">
-        <v>903191.125</v>
+        <v>940037.875</v>
       </c>
       <c r="I24" t="s"/>
       <c r="J24" t="s"/>
@@ -2984,18 +2770,18 @@
     </row>
     <row r="25" spans="1:21">
       <c r="A25" s="1" t="n"/>
-      <c r="B25" s="1" t="n"/>
-      <c r="C25" s="1" t="s">
+      <c r="B25" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="C25" s="1" t="s"/>
       <c r="D25" t="s"/>
       <c r="E25" t="s"/>
       <c r="F25" t="s"/>
       <c r="G25" t="n">
-        <v>3399.5</v>
+        <v>3474.98388671875</v>
       </c>
       <c r="H25" t="n">
-        <v>97447.1171875</v>
+        <v>132760.125</v>
       </c>
       <c r="I25" t="s"/>
       <c r="J25" t="s"/>
@@ -3013,18 +2799,18 @@
     </row>
     <row r="26" spans="1:21">
       <c r="A26" s="1" t="n"/>
-      <c r="B26" s="1" t="n"/>
-      <c r="C26" s="1" t="s">
+      <c r="B26" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="C26" s="1" t="s"/>
       <c r="D26" t="s"/>
       <c r="E26" t="s"/>
       <c r="F26" t="s"/>
       <c r="G26" t="n">
-        <v>7854.56689453125</v>
+        <v>7393.01708984375</v>
       </c>
       <c r="H26" t="n">
-        <v>150260.3125</v>
+        <v>152723.859375</v>
       </c>
       <c r="I26" t="s"/>
       <c r="J26" t="s"/>
@@ -3042,18 +2828,18 @@
     </row>
     <row r="27" spans="1:21">
       <c r="A27" s="1" t="n"/>
-      <c r="B27" s="1" t="n"/>
-      <c r="C27" s="1" t="s">
+      <c r="B27" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="C27" s="1" t="s"/>
       <c r="D27" t="s"/>
       <c r="E27" t="s"/>
       <c r="F27" t="s"/>
       <c r="G27" t="n">
-        <v>30022.005859375</v>
+        <v>18626.560546875</v>
       </c>
       <c r="H27" t="n">
-        <v>701971.875</v>
+        <v>633689.9375</v>
       </c>
       <c r="I27" t="s"/>
       <c r="J27" t="s"/>
@@ -3071,18 +2857,18 @@
     </row>
     <row r="28" spans="1:21">
       <c r="A28" s="1" t="n"/>
-      <c r="B28" s="1" t="n"/>
-      <c r="C28" s="1" t="s">
+      <c r="B28" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="C28" s="1" t="s"/>
       <c r="D28" t="s"/>
       <c r="E28" t="s"/>
       <c r="F28" t="s"/>
       <c r="G28" t="n">
-        <v>22544.7109375</v>
+        <v>16824.890625</v>
       </c>
       <c r="H28" t="n">
-        <v>427442.375</v>
+        <v>484801.875</v>
       </c>
       <c r="I28" t="s"/>
       <c r="J28" t="s"/>
@@ -3100,18 +2886,18 @@
     </row>
     <row r="29" spans="1:21">
       <c r="A29" s="1" t="n"/>
-      <c r="B29" s="1" t="n"/>
-      <c r="C29" s="1" t="s">
+      <c r="B29" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="C29" s="1" t="s"/>
       <c r="D29" t="s"/>
       <c r="E29" t="s"/>
       <c r="F29" t="s"/>
       <c r="G29" t="n">
-        <v>103681.3984375</v>
+        <v>75660.1796875</v>
       </c>
       <c r="H29" t="n">
-        <v>2354051</v>
+        <v>2409430</v>
       </c>
       <c r="I29" t="s"/>
       <c r="J29" t="s"/>
@@ -3129,20 +2915,20 @@
     </row>
     <row r="30" spans="1:21">
       <c r="A30" s="1" t="n">
-        <v>2018201905</v>
-      </c>
-      <c r="B30" s="1" t="s"/>
-      <c r="C30" s="1" t="s">
+        <v>2019202005</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="C30" s="1" t="s"/>
       <c r="D30" t="s"/>
       <c r="E30" t="s"/>
       <c r="F30" t="s"/>
       <c r="G30" t="n">
-        <v>1598.5</v>
+        <v>1674.829956054688</v>
       </c>
       <c r="H30" t="n">
-        <v>67051.984375</v>
+        <v>55063.25390625</v>
       </c>
       <c r="I30" t="s"/>
       <c r="J30" t="s"/>
@@ -3160,18 +2946,18 @@
     </row>
     <row r="31" spans="1:21">
       <c r="A31" s="1" t="n"/>
-      <c r="B31" s="1" t="n"/>
-      <c r="C31" s="1" t="s">
+      <c r="B31" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="C31" s="1" t="s"/>
       <c r="D31" t="s"/>
       <c r="E31" t="s"/>
       <c r="F31" t="s"/>
       <c r="G31" t="n">
-        <v>32199.1015625</v>
+        <v>34271.46484375</v>
       </c>
       <c r="H31" t="n">
-        <v>847716.6875</v>
+        <v>863191</v>
       </c>
       <c r="I31" t="s"/>
       <c r="J31" t="s"/>
@@ -3189,18 +2975,18 @@
     </row>
     <row r="32" spans="1:21">
       <c r="A32" s="1" t="n"/>
-      <c r="B32" s="1" t="n"/>
-      <c r="C32" s="1" t="s">
+      <c r="B32" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="C32" s="1" t="s"/>
       <c r="D32" t="s"/>
       <c r="E32" t="s"/>
       <c r="F32" t="s"/>
       <c r="G32" t="n">
-        <v>1662.984985351562</v>
+        <v>7090.1591796875</v>
       </c>
       <c r="H32" t="n">
-        <v>93476.078125</v>
+        <v>135978.84375</v>
       </c>
       <c r="I32" t="s"/>
       <c r="J32" t="s"/>
@@ -3218,18 +3004,18 @@
     </row>
     <row r="33" spans="1:21">
       <c r="A33" s="1" t="n"/>
-      <c r="B33" s="1" t="n"/>
-      <c r="C33" s="1" t="s">
+      <c r="B33" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="C33" s="1" t="s"/>
       <c r="D33" t="s"/>
       <c r="E33" t="s"/>
       <c r="F33" t="s"/>
       <c r="G33" t="n">
-        <v>6239</v>
+        <v>7562.0751953125</v>
       </c>
       <c r="H33" t="n">
-        <v>147110.28125</v>
+        <v>130492.015625</v>
       </c>
       <c r="I33" t="s"/>
       <c r="J33" t="s"/>
@@ -3247,18 +3033,18 @@
     </row>
     <row r="34" spans="1:21">
       <c r="A34" s="1" t="n"/>
-      <c r="B34" s="1" t="n"/>
-      <c r="C34" s="1" t="s">
+      <c r="B34" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="C34" s="1" t="s"/>
       <c r="D34" t="s"/>
       <c r="E34" t="s"/>
       <c r="F34" t="s"/>
       <c r="G34" t="n">
-        <v>32101.33984375</v>
+        <v>24515.478515625</v>
       </c>
       <c r="H34" t="n">
-        <v>688156.25</v>
+        <v>616340.5</v>
       </c>
       <c r="I34" t="s"/>
       <c r="J34" t="s"/>
@@ -3276,18 +3062,18 @@
     </row>
     <row r="35" spans="1:21">
       <c r="A35" s="1" t="n"/>
-      <c r="B35" s="1" t="n"/>
-      <c r="C35" s="1" t="s">
+      <c r="B35" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="C35" s="1" t="s"/>
       <c r="D35" t="s"/>
       <c r="E35" t="s"/>
       <c r="F35" t="s"/>
       <c r="G35" t="n">
-        <v>22808</v>
+        <v>22654.337890625</v>
       </c>
       <c r="H35" t="n">
-        <v>431512.53125</v>
+        <v>453371.5</v>
       </c>
       <c r="I35" t="s"/>
       <c r="J35" t="s"/>
@@ -3305,18 +3091,18 @@
     </row>
     <row r="36" spans="1:21">
       <c r="A36" s="1" t="n"/>
-      <c r="B36" s="1" t="n"/>
-      <c r="C36" s="1" t="s">
+      <c r="B36" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="C36" s="1" t="s"/>
       <c r="D36" t="s"/>
       <c r="E36" t="s"/>
       <c r="F36" t="s"/>
       <c r="G36" t="n">
-        <v>96847.9296875</v>
+        <v>98297.34375</v>
       </c>
       <c r="H36" t="n">
-        <v>2277824</v>
+        <v>2265295.5</v>
       </c>
       <c r="I36" t="s"/>
       <c r="J36" t="s"/>
@@ -3334,20 +3120,20 @@
     </row>
     <row r="37" spans="1:21">
       <c r="A37" s="1" t="n">
-        <v>2018201906</v>
-      </c>
-      <c r="B37" s="1" t="s"/>
-      <c r="C37" s="1" t="s">
+        <v>2019202006</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="C37" s="1" t="s"/>
       <c r="D37" t="s"/>
       <c r="E37" t="s"/>
       <c r="F37" t="s"/>
       <c r="G37" t="n">
-        <v>2635.5</v>
+        <v>1114.5009765625</v>
       </c>
       <c r="H37" t="n">
-        <v>72434.046875</v>
+        <v>55899.56640625</v>
       </c>
       <c r="I37" t="s"/>
       <c r="J37" t="s"/>
@@ -3365,18 +3151,18 @@
     </row>
     <row r="38" spans="1:21">
       <c r="A38" s="1" t="n"/>
-      <c r="B38" s="1" t="n"/>
-      <c r="C38" s="1" t="s">
+      <c r="B38" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="C38" s="1" t="s"/>
       <c r="D38" t="s"/>
       <c r="E38" t="s"/>
       <c r="F38" t="s"/>
       <c r="G38" t="n">
-        <v>26271.400390625</v>
+        <v>22980.30859375</v>
       </c>
       <c r="H38" t="n">
-        <v>881453.5</v>
+        <v>904859.75</v>
       </c>
       <c r="I38" t="s"/>
       <c r="J38" t="s"/>
@@ -3394,18 +3180,18 @@
     </row>
     <row r="39" spans="1:21">
       <c r="A39" s="1" t="n"/>
-      <c r="B39" s="1" t="n"/>
-      <c r="C39" s="1" t="s">
+      <c r="B39" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="C39" s="1" t="s"/>
       <c r="D39" t="s"/>
       <c r="E39" t="s"/>
       <c r="F39" t="s"/>
       <c r="G39" t="n">
-        <v>1334</v>
+        <v>3180.931884765625</v>
       </c>
       <c r="H39" t="n">
-        <v>96437.6875</v>
+        <v>144902.59375</v>
       </c>
       <c r="I39" t="s"/>
       <c r="J39" t="s"/>
@@ -3423,18 +3209,18 @@
     </row>
     <row r="40" spans="1:21">
       <c r="A40" s="1" t="n"/>
-      <c r="B40" s="1" t="n"/>
-      <c r="C40" s="1" t="s">
+      <c r="B40" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="C40" s="1" t="s"/>
       <c r="D40" t="s"/>
       <c r="E40" t="s"/>
       <c r="F40" t="s"/>
       <c r="G40" t="n">
-        <v>4983.31005859375</v>
+        <v>6569.115234375</v>
       </c>
       <c r="H40" t="n">
-        <v>164134.546875</v>
+        <v>133770.265625</v>
       </c>
       <c r="I40" t="s"/>
       <c r="J40" t="s"/>
@@ -3452,18 +3238,18 @@
     </row>
     <row r="41" spans="1:21">
       <c r="A41" s="1" t="n"/>
-      <c r="B41" s="1" t="n"/>
-      <c r="C41" s="1" t="s">
+      <c r="B41" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="C41" s="1" t="s"/>
       <c r="D41" t="s"/>
       <c r="E41" t="s"/>
       <c r="F41" t="s"/>
       <c r="G41" t="n">
-        <v>20084.267578125</v>
+        <v>17786.1171875</v>
       </c>
       <c r="H41" t="n">
-        <v>650669.3125</v>
+        <v>613752.1875</v>
       </c>
       <c r="I41" t="s"/>
       <c r="J41" t="s"/>
@@ -3481,18 +3267,18 @@
     </row>
     <row r="42" spans="1:21">
       <c r="A42" s="1" t="n"/>
-      <c r="B42" s="1" t="n"/>
-      <c r="C42" s="1" t="s">
+      <c r="B42" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="C42" s="1" t="s"/>
       <c r="D42" t="s"/>
       <c r="E42" t="s"/>
       <c r="F42" t="s"/>
       <c r="G42" t="n">
-        <v>19055.80078125</v>
+        <v>17094.662109375</v>
       </c>
       <c r="H42" t="n">
-        <v>467116.25</v>
+        <v>463333.375</v>
       </c>
       <c r="I42" t="s"/>
       <c r="J42" t="s"/>
@@ -3510,18 +3296,18 @@
     </row>
     <row r="43" spans="1:21">
       <c r="A43" s="1" t="n"/>
-      <c r="B43" s="1" t="n"/>
-      <c r="C43" s="1" t="s">
+      <c r="B43" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="C43" s="1" t="s"/>
       <c r="D43" t="s"/>
       <c r="E43" t="s"/>
       <c r="F43" t="s"/>
       <c r="G43" t="n">
-        <v>74777.78125</v>
+        <v>69099.6328125</v>
       </c>
       <c r="H43" t="n">
-        <v>2338246.75</v>
+        <v>2323086</v>
       </c>
       <c r="I43" t="s"/>
       <c r="J43" t="s"/>
@@ -3539,20 +3325,20 @@
     </row>
     <row r="44" spans="1:21">
       <c r="A44" s="1" t="n">
-        <v>2018201907</v>
-      </c>
-      <c r="B44" s="1" t="s"/>
-      <c r="C44" s="1" t="s">
+        <v>2019202007</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="C44" s="1" t="s"/>
       <c r="D44" t="s"/>
       <c r="E44" t="s"/>
       <c r="F44" t="s"/>
       <c r="G44" t="n">
-        <v>2788.35595703125</v>
+        <v>1073.922973632812</v>
       </c>
       <c r="H44" t="n">
-        <v>64237.8984375</v>
+        <v>51477.0390625</v>
       </c>
       <c r="I44" t="s"/>
       <c r="J44" t="s"/>
@@ -3570,18 +3356,18 @@
     </row>
     <row r="45" spans="1:21">
       <c r="A45" s="1" t="n"/>
-      <c r="B45" s="1" t="n"/>
-      <c r="C45" s="1" t="s">
+      <c r="B45" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="C45" s="1" t="s"/>
       <c r="D45" t="s"/>
       <c r="E45" t="s"/>
       <c r="F45" t="s"/>
       <c r="G45" t="n">
-        <v>38255.13671875</v>
+        <v>27870.07421875</v>
       </c>
       <c r="H45" t="n">
-        <v>915260.0625</v>
+        <v>924610.25</v>
       </c>
       <c r="I45" t="s"/>
       <c r="J45" t="s"/>
@@ -3599,18 +3385,18 @@
     </row>
     <row r="46" spans="1:21">
       <c r="A46" s="1" t="n"/>
-      <c r="B46" s="1" t="n"/>
-      <c r="C46" s="1" t="s">
+      <c r="B46" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="C46" s="1" t="s"/>
       <c r="D46" t="s"/>
       <c r="E46" t="s"/>
       <c r="F46" t="s"/>
       <c r="G46" t="n">
-        <v>6288</v>
+        <v>2241.339111328125</v>
       </c>
       <c r="H46" t="n">
-        <v>98271.03125</v>
+        <v>139688.171875</v>
       </c>
       <c r="I46" t="s"/>
       <c r="J46" t="s"/>
@@ -3628,18 +3414,18 @@
     </row>
     <row r="47" spans="1:21">
       <c r="A47" s="1" t="n"/>
-      <c r="B47" s="1" t="n"/>
-      <c r="C47" s="1" t="s">
+      <c r="B47" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="C47" s="1" t="s"/>
       <c r="D47" t="s"/>
       <c r="E47" t="s"/>
       <c r="F47" t="s"/>
       <c r="G47" t="n">
-        <v>8036.5</v>
+        <v>7468.9111328125</v>
       </c>
       <c r="H47" t="n">
-        <v>156371.453125</v>
+        <v>134571.5625</v>
       </c>
       <c r="I47" t="s"/>
       <c r="J47" t="s"/>
@@ -3657,18 +3443,18 @@
     </row>
     <row r="48" spans="1:21">
       <c r="A48" s="1" t="n"/>
-      <c r="B48" s="1" t="n"/>
-      <c r="C48" s="1" t="s">
+      <c r="B48" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="C48" s="1" t="s"/>
       <c r="D48" t="s"/>
       <c r="E48" t="s"/>
       <c r="F48" t="s"/>
       <c r="G48" t="n">
-        <v>31406.876953125</v>
+        <v>22493.244140625</v>
       </c>
       <c r="H48" t="n">
-        <v>669377.375</v>
+        <v>643245.1875</v>
       </c>
       <c r="I48" t="s"/>
       <c r="J48" t="s"/>
@@ -3686,18 +3472,18 @@
     </row>
     <row r="49" spans="1:21">
       <c r="A49" s="1" t="n"/>
-      <c r="B49" s="1" t="n"/>
-      <c r="C49" s="1" t="s">
+      <c r="B49" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="C49" s="1" t="s"/>
       <c r="D49" t="s"/>
       <c r="E49" t="s"/>
       <c r="F49" t="s"/>
       <c r="G49" t="n">
-        <v>36561.6171875</v>
+        <v>20122.6875</v>
       </c>
       <c r="H49" t="n">
-        <v>511708.28125</v>
+        <v>442925.90625</v>
       </c>
       <c r="I49" t="s"/>
       <c r="J49" t="s"/>
@@ -3715,18 +3501,18 @@
     </row>
     <row r="50" spans="1:21">
       <c r="A50" s="1" t="n"/>
-      <c r="B50" s="1" t="n"/>
-      <c r="C50" s="1" t="s">
+      <c r="B50" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="C50" s="1" t="s"/>
       <c r="D50" t="s"/>
       <c r="E50" t="s"/>
       <c r="F50" t="s"/>
       <c r="G50" t="n">
-        <v>123844.984375</v>
+        <v>81502.3515625</v>
       </c>
       <c r="H50" t="n">
-        <v>2422237</v>
+        <v>2341969.25</v>
       </c>
       <c r="I50" t="s"/>
       <c r="J50" t="s"/>
@@ -3744,20 +3530,20 @@
     </row>
     <row r="51" spans="1:21">
       <c r="A51" s="1" t="n">
-        <v>2018201908</v>
-      </c>
-      <c r="B51" s="1" t="s"/>
-      <c r="C51" s="1" t="s">
+        <v>2019202008</v>
+      </c>
+      <c r="B51" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="C51" s="1" t="s"/>
       <c r="D51" t="s"/>
       <c r="E51" t="s"/>
       <c r="F51" t="s"/>
       <c r="G51" t="n">
-        <v>1652</v>
+        <v>1578.28955078125</v>
       </c>
       <c r="H51" t="n">
-        <v>70021.1875</v>
+        <v>51771.88671875</v>
       </c>
       <c r="I51" t="s"/>
       <c r="J51" t="s"/>
@@ -3775,18 +3561,18 @@
     </row>
     <row r="52" spans="1:21">
       <c r="A52" s="1" t="n"/>
-      <c r="B52" s="1" t="n"/>
-      <c r="C52" s="1" t="s">
+      <c r="B52" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="C52" s="1" t="s"/>
       <c r="D52" t="s"/>
       <c r="E52" t="s"/>
       <c r="F52" t="s"/>
       <c r="G52" t="n">
-        <v>33008.4375</v>
+        <v>31559.28515625</v>
       </c>
       <c r="H52" t="n">
-        <v>922584.625</v>
+        <v>881203</v>
       </c>
       <c r="I52" t="s"/>
       <c r="J52" t="s"/>
@@ -3804,18 +3590,18 @@
     </row>
     <row r="53" spans="1:21">
       <c r="A53" s="1" t="n"/>
-      <c r="B53" s="1" t="n"/>
-      <c r="C53" s="1" t="s">
+      <c r="B53" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="C53" s="1" t="s"/>
       <c r="D53" t="s"/>
       <c r="E53" t="s"/>
       <c r="F53" t="s"/>
       <c r="G53" t="n">
-        <v>2706</v>
+        <v>3083.8369140625</v>
       </c>
       <c r="H53" t="n">
-        <v>101066.03125</v>
+        <v>137807.3125</v>
       </c>
       <c r="I53" t="s"/>
       <c r="J53" t="s"/>
@@ -3833,18 +3619,18 @@
     </row>
     <row r="54" spans="1:21">
       <c r="A54" s="1" t="n"/>
-      <c r="B54" s="1" t="n"/>
-      <c r="C54" s="1" t="s">
+      <c r="B54" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="C54" s="1" t="s"/>
       <c r="D54" t="s"/>
       <c r="E54" t="s"/>
       <c r="F54" t="s"/>
       <c r="G54" t="n">
-        <v>8600.728515625</v>
+        <v>10536.6396484375</v>
       </c>
       <c r="H54" t="n">
-        <v>157653.25</v>
+        <v>165150.140625</v>
       </c>
       <c r="I54" t="s"/>
       <c r="J54" t="s"/>
@@ -3862,18 +3648,18 @@
     </row>
     <row r="55" spans="1:21">
       <c r="A55" s="1" t="n"/>
-      <c r="B55" s="1" t="n"/>
-      <c r="C55" s="1" t="s">
+      <c r="B55" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="C55" s="1" t="s"/>
       <c r="D55" t="s"/>
       <c r="E55" t="s"/>
       <c r="F55" t="s"/>
       <c r="G55" t="n">
-        <v>27178.546875</v>
+        <v>26909.984375</v>
       </c>
       <c r="H55" t="n">
-        <v>673084.125</v>
+        <v>637096.25</v>
       </c>
       <c r="I55" t="s"/>
       <c r="J55" t="s"/>
@@ -3891,18 +3677,18 @@
     </row>
     <row r="56" spans="1:21">
       <c r="A56" s="1" t="n"/>
-      <c r="B56" s="1" t="n"/>
-      <c r="C56" s="1" t="s">
+      <c r="B56" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="C56" s="1" t="s"/>
       <c r="D56" t="s"/>
       <c r="E56" t="s"/>
       <c r="F56" t="s"/>
       <c r="G56" t="n">
-        <v>26561.7109375</v>
+        <v>22739.529296875</v>
       </c>
       <c r="H56" t="n">
-        <v>521973.59375</v>
+        <v>450251.78125</v>
       </c>
       <c r="I56" t="s"/>
       <c r="J56" t="s"/>
@@ -3920,18 +3706,18 @@
     </row>
     <row r="57" spans="1:21">
       <c r="A57" s="1" t="n"/>
-      <c r="B57" s="1" t="n"/>
-      <c r="C57" s="1" t="s">
+      <c r="B57" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="C57" s="1" t="s"/>
       <c r="D57" t="s"/>
       <c r="E57" t="s"/>
       <c r="F57" t="s"/>
       <c r="G57" t="n">
-        <v>100127.921875</v>
+        <v>97495.3515625</v>
       </c>
       <c r="H57" t="n">
-        <v>2452644.25</v>
+        <v>2335668.25</v>
       </c>
       <c r="I57" t="s"/>
       <c r="J57" t="s"/>
@@ -3948,7 +3734,7 @@
       <c r="U57" t="s"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="8">
     <mergeCell ref="A2:A8"/>
     <mergeCell ref="A9:A15"/>
     <mergeCell ref="A16:A22"/>
@@ -3957,14 +3743,6 @@
     <mergeCell ref="A37:A43"/>
     <mergeCell ref="A44:A50"/>
     <mergeCell ref="A51:A57"/>
-    <mergeCell ref="B2:B8"/>
-    <mergeCell ref="B9:B15"/>
-    <mergeCell ref="B16:B22"/>
-    <mergeCell ref="B23:B29"/>
-    <mergeCell ref="B30:B36"/>
-    <mergeCell ref="B37:B43"/>
-    <mergeCell ref="B44:B50"/>
-    <mergeCell ref="B51:B57"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
@@ -3976,7 +3754,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4000,108 +3778,427 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="n">
-        <v>2018201904</v>
-      </c>
-      <c r="B2" s="1" t="s"/>
-      <c r="C2" s="1" t="s">
+        <v>2019202001</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="C2" s="1" t="s"/>
       <c r="D2" t="n">
-        <v>-0.93359375</v>
+        <v>27.1875</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1" t="n"/>
-      <c r="B3" s="1" t="n"/>
-      <c r="C3" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="B3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="1" t="s"/>
       <c r="D3" t="n">
-        <v>-0.833984375</v>
+        <v>22.080078125</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1" t="n"/>
-      <c r="B4" s="1" t="n"/>
-      <c r="C4" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="C4" s="1" t="s"/>
       <c r="D4" t="n">
-        <v>-1.765625</v>
+        <v>49.26953125</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1" t="n">
-        <v>2018201907</v>
-      </c>
-      <c r="B5" s="1" t="s"/>
-      <c r="C5" s="1" t="s">
-        <v>22</v>
-      </c>
+        <v>2019202002</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="1" t="s"/>
       <c r="D5" t="n">
-        <v>-0.75</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="1" t="n"/>
-      <c r="B6" s="1" t="n"/>
-      <c r="C6" s="1" t="s">
-        <v>26</v>
-      </c>
+      <c r="B6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="1" t="s"/>
       <c r="D6" t="n">
-        <v>-0.375</v>
+        <v>-0.185546875</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1" t="n"/>
-      <c r="B7" s="1" t="n"/>
-      <c r="C7" s="1" t="s">
-        <v>27</v>
-      </c>
+      <c r="B7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="1" t="s"/>
       <c r="D7" t="n">
-        <v>-1.125</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="1" t="n">
-        <v>2018201908</v>
-      </c>
-      <c r="B8" s="1" t="s"/>
-      <c r="C8" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="A8" s="1" t="n"/>
+      <c r="B8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="1" t="s"/>
       <c r="D8" t="n">
-        <v>-0.158203125</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="1" t="n"/>
-      <c r="B9" s="1" t="n"/>
-      <c r="C9" s="1" t="s">
+      <c r="B9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="1" t="s"/>
+      <c r="D9" t="n">
+        <v>9.3125</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="1" t="n">
+        <v>2019202003</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="1" t="s"/>
+      <c r="D10" t="n">
+        <v>-0.385009765625</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="1" t="n"/>
+      <c r="B11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="1" t="s"/>
+      <c r="D11" t="n">
+        <v>-46.12890625</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="1" t="n"/>
+      <c r="B12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="1" t="s"/>
+      <c r="D12" t="n">
+        <v>-0.044921875</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="1" t="n"/>
+      <c r="B13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="1" t="s"/>
+      <c r="D13" t="n">
+        <v>10.388671875</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="1" t="n"/>
+      <c r="B14" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D9" t="n">
-        <v>-1.935546875</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="1" t="n"/>
-      <c r="B10" s="1" t="n"/>
-      <c r="C10" s="1" t="s">
+      <c r="C14" s="1" t="s"/>
+      <c r="D14" t="n">
+        <v>-4.2880859375</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="1" t="n"/>
+      <c r="B15" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D10" t="n">
-        <v>-2.09375</v>
+      <c r="C15" s="1" t="s"/>
+      <c r="D15" t="n">
+        <v>-40.4609375</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="1" t="n">
+        <v>2019202004</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="1" t="s"/>
+      <c r="D16" t="n">
+        <v>61.033203125</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="1" t="n"/>
+      <c r="B17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="1" t="s"/>
+      <c r="D17" t="n">
+        <v>-12.385009765625</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="1" t="n"/>
+      <c r="B18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="1" t="s"/>
+      <c r="D18" t="n">
+        <v>1.1181640625</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="1" t="n"/>
+      <c r="B19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="1" t="s"/>
+      <c r="D19" t="n">
+        <v>23.658203125</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="1" t="n"/>
+      <c r="B20" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="1" t="s"/>
+      <c r="D20" t="n">
+        <v>102.525390625</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="1" t="n"/>
+      <c r="B21" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="1" t="s"/>
+      <c r="D21" t="n">
+        <v>175.953125</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="1" t="n">
+        <v>2019202005</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="1" t="s"/>
+      <c r="D22" t="n">
+        <v>-12.88671875</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="1" t="n"/>
+      <c r="B23" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="1" t="s"/>
+      <c r="D23" t="n">
+        <v>-18.583984375</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="1" t="n"/>
+      <c r="B24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="1" t="s"/>
+      <c r="D24" t="n">
+        <v>-11.28857421875</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="1" t="n"/>
+      <c r="B25" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="1" t="s"/>
+      <c r="D25" t="n">
+        <v>-64.568359375</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="1" t="n"/>
+      <c r="B26" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="1" t="s"/>
+      <c r="D26" t="n">
+        <v>-8.67578125</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="1" t="n"/>
+      <c r="B27" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" s="1" t="s"/>
+      <c r="D27" t="n">
+        <v>-116</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="1" t="n">
+        <v>2019202006</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C28" s="1" t="s"/>
+      <c r="D28" t="n">
+        <v>-3.239990234375</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="1" t="n"/>
+      <c r="B29" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C29" s="1" t="s"/>
+      <c r="D29" t="n">
+        <v>18.4296875</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="1" t="n"/>
+      <c r="B30" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C30" s="1" t="s"/>
+      <c r="D30" t="n">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="1" t="n"/>
+      <c r="B31" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C31" s="1" t="s"/>
+      <c r="D31" t="n">
+        <v>7.71044921875</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="1" t="n"/>
+      <c r="B32" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32" s="1" t="s"/>
+      <c r="D32" t="n">
+        <v>9.185546875</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="1" t="n"/>
+      <c r="B33" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C33" s="1" t="s"/>
+      <c r="D33" t="n">
+        <v>-19.599609375</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="1" t="n"/>
+      <c r="B34" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C34" s="1" t="s"/>
+      <c r="D34" t="n">
+        <v>18.984375</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="1" t="n">
+        <v>2019202007</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C35" s="1" t="s"/>
+      <c r="D35" t="n">
+        <v>34.0260009765625</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="1" t="n"/>
+      <c r="B36" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C36" s="1" t="s"/>
+      <c r="D36" t="n">
+        <v>201.994140625</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="1" t="n"/>
+      <c r="B37" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C37" s="1" t="s"/>
+      <c r="D37" t="n">
+        <v>141.748046875</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="1" t="n"/>
+      <c r="B38" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C38" s="1" t="s"/>
+      <c r="D38" t="n">
+        <v>43.39697265625</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="1" t="n"/>
+      <c r="B39" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C39" s="1" t="s"/>
+      <c r="D39" t="n">
+        <v>83.541015625</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="1" t="n"/>
+      <c r="B40" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C40" s="1" t="s"/>
+      <c r="D40" t="n">
+        <v>68.607421875</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="1" t="n"/>
+      <c r="B41" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C41" s="1" t="s"/>
+      <c r="D41" t="n">
+        <v>570.6171875</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
     <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="A5:A9"/>
+    <mergeCell ref="A10:A15"/>
+    <mergeCell ref="A16:A21"/>
+    <mergeCell ref="A22:A27"/>
+    <mergeCell ref="A28:A34"/>
+    <mergeCell ref="A35:A41"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
@@ -4113,7 +4210,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4137,108 +4234,427 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="n">
-        <v>2018201904</v>
-      </c>
-      <c r="B2" s="1" t="s"/>
-      <c r="C2" s="1" t="s">
+        <v>2019202001</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="C2" s="1" t="s"/>
       <c r="D2" t="n">
-        <v>-0.002534732194407808</v>
+        <v>0.112009683043979</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1" t="n"/>
-      <c r="B3" s="1" t="n"/>
-      <c r="C3" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="B3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="1" t="s"/>
       <c r="D3" t="n">
-        <v>-0.002777833074220707</v>
+        <v>0.4316659115854282</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1" t="n"/>
-      <c r="B4" s="1" t="n"/>
-      <c r="C4" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="C4" s="1" t="s"/>
       <c r="D4" t="n">
-        <v>-0.001702904242906481</v>
+        <v>0.07683947476475411</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1" t="n">
-        <v>2018201907</v>
-      </c>
-      <c r="B5" s="1" t="s"/>
-      <c r="C5" s="1" t="s">
-        <v>22</v>
-      </c>
+        <v>2019202002</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="1" t="s"/>
       <c r="D5" t="n">
-        <v>-0.001960482593212013</v>
+        <v>0.07512549497509603</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="1" t="n"/>
-      <c r="B6" s="1" t="n"/>
-      <c r="C6" s="1" t="s">
-        <v>26</v>
-      </c>
+      <c r="B6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="1" t="s"/>
       <c r="D6" t="n">
-        <v>-0.001025655270853121</v>
+        <v>-0.0007789735522899527</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1" t="n"/>
-      <c r="B7" s="1" t="n"/>
-      <c r="C7" s="1" t="s">
-        <v>27</v>
-      </c>
+      <c r="B7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="1" t="s"/>
       <c r="D7" t="n">
-        <v>-0.0009083854193542363</v>
+        <v>0.0320980010331544</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="1" t="n">
-        <v>2018201908</v>
-      </c>
-      <c r="B8" s="1" t="s"/>
-      <c r="C8" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="A8" s="1" t="n"/>
+      <c r="B8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="1" t="s"/>
       <c r="D8" t="n">
-        <v>-0.0005820848511555139</v>
+        <v>0.01446129637387513</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="1" t="n"/>
-      <c r="B9" s="1" t="n"/>
-      <c r="C9" s="1" t="s">
+      <c r="B9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="1" t="s"/>
+      <c r="D9" t="n">
+        <v>0.01360220200479569</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="1" t="n">
+        <v>2019202003</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="1" t="s"/>
+      <c r="D10" t="n">
+        <v>-0.02235350041003861</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="1" t="n"/>
+      <c r="B11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="1" t="s"/>
+      <c r="D11" t="n">
+        <v>-0.1638996826794441</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="1" t="n"/>
+      <c r="B12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="1" t="s"/>
+      <c r="D12" t="n">
+        <v>-0.0007407703238390196</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="1" t="n"/>
+      <c r="B13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="1" t="s"/>
+      <c r="D13" t="n">
+        <v>0.05981002474036783</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="1" t="n"/>
+      <c r="B14" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D9" t="n">
-        <v>-0.007286450209832854</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="1" t="n"/>
-      <c r="B10" s="1" t="n"/>
-      <c r="C10" s="1" t="s">
+      <c r="C14" s="1" t="s"/>
+      <c r="D14" t="n">
+        <v>-0.02873632047090132</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="1" t="n"/>
+      <c r="B15" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D10" t="n">
-        <v>-0.002091031332544047</v>
+      <c r="C15" s="1" t="s"/>
+      <c r="D15" t="n">
+        <v>-0.05728803592631292</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="1" t="n">
+        <v>2019202004</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="1" t="s"/>
+      <c r="D16" t="n">
+        <v>0.2241671386283186</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="1" t="n"/>
+      <c r="B17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="1" t="s"/>
+      <c r="D17" t="n">
+        <v>-0.3551390785789929</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="1" t="n"/>
+      <c r="B18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="1" t="s"/>
+      <c r="D18" t="n">
+        <v>0.01512688517155044</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="1" t="n"/>
+      <c r="B19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="1" t="s"/>
+      <c r="D19" t="n">
+        <v>0.1271747961035146</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="1" t="n"/>
+      <c r="B20" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="1" t="s"/>
+      <c r="D20" t="n">
+        <v>0.6131034048595333</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="1" t="n"/>
+      <c r="B21" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="1" t="s"/>
+      <c r="D21" t="n">
+        <v>0.2330991957032414</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="1" t="n">
+        <v>2019202005</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="1" t="s"/>
+      <c r="D22" t="n">
+        <v>-0.03758775698734641</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="1" t="n"/>
+      <c r="B23" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="1" t="s"/>
+      <c r="D23" t="n">
+        <v>-0.261424332629562</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="1" t="n"/>
+      <c r="B24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="1" t="s"/>
+      <c r="D24" t="n">
+        <v>-0.1490562788514872</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="1" t="n"/>
+      <c r="B25" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="1" t="s"/>
+      <c r="D25" t="n">
+        <v>-0.2626860709556723</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="1" t="n"/>
+      <c r="B26" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="1" t="s"/>
+      <c r="D26" t="n">
+        <v>-0.03828167504821621</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="1" t="n"/>
+      <c r="B27" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" s="1" t="s"/>
+      <c r="D27" t="n">
+        <v>-0.1178701948128858</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="1" t="n">
+        <v>2019202006</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C28" s="1" t="s"/>
+      <c r="D28" t="n">
+        <v>-0.2898695073922076</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="1" t="n"/>
+      <c r="B29" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C29" s="1" t="s"/>
+      <c r="D29" t="n">
+        <v>0.08026210561969133</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="1" t="n"/>
+      <c r="B30" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C30" s="1" t="s"/>
+      <c r="D30" t="n">
+        <v>0.2047610481483022</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="1" t="n"/>
+      <c r="B31" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C31" s="1" t="s"/>
+      <c r="D31" t="n">
+        <v>0.1175121711160575</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="1" t="n"/>
+      <c r="B32" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32" s="1" t="s"/>
+      <c r="D32" t="n">
+        <v>0.05167116047185889</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="1" t="n"/>
+      <c r="B33" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C33" s="1" t="s"/>
+      <c r="D33" t="n">
+        <v>-0.1145220851304799</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="1" t="n"/>
+      <c r="B34" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C34" s="1" t="s"/>
+      <c r="D34" t="n">
+        <v>0.0274814661260395</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="1" t="n">
+        <v>2019202007</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C35" s="1" t="s"/>
+      <c r="D35" t="n">
+        <v>3.272055008454207</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="1" t="n"/>
+      <c r="B36" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C36" s="1" t="s"/>
+      <c r="D36" t="n">
+        <v>0.7300620066684752</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="1" t="n"/>
+      <c r="B37" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C37" s="1" t="s"/>
+      <c r="D37" t="n">
+        <v>6.751221667630822</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="1" t="n"/>
+      <c r="B38" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C38" s="1" t="s"/>
+      <c r="D38" t="n">
+        <v>0.5844305420506642</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="1" t="n"/>
+      <c r="B39" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C39" s="1" t="s"/>
+      <c r="D39" t="n">
+        <v>0.3727894794456363</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="1" t="n"/>
+      <c r="B40" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C40" s="1" t="s"/>
+      <c r="D40" t="n">
+        <v>0.3421120370903326</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="1" t="n"/>
+      <c r="B41" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C41" s="1" t="s"/>
+      <c r="D41" t="n">
+        <v>0.7050598778175511</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
     <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="A5:A9"/>
+    <mergeCell ref="A10:A15"/>
+    <mergeCell ref="A16:A21"/>
+    <mergeCell ref="A22:A27"/>
+    <mergeCell ref="A28:A34"/>
+    <mergeCell ref="A35:A41"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
@@ -4372,10 +4788,10 @@
       <c r="C4" t="s"/>
       <c r="D4" t="s"/>
       <c r="E4" t="n">
-        <v>26818.83585248675</v>
+        <v>22262.41841561454</v>
       </c>
       <c r="F4" t="n">
-        <v>673006.7430245535</v>
+        <v>661500.7734375</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -4386,10 +4802,10 @@
       <c r="C5" t="s"/>
       <c r="D5" t="s"/>
       <c r="E5" t="n">
-        <v>30595.65143491828</v>
+        <v>25286.71080126651</v>
       </c>
       <c r="F5" t="n">
-        <v>754212.5537659391</v>
+        <v>740988.3092375267</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -4400,10 +4816,10 @@
       <c r="C6" t="s"/>
       <c r="D6" t="s"/>
       <c r="E6" t="n">
-        <v>1334</v>
+        <v>1073.922973632812</v>
       </c>
       <c r="F6" t="n">
-        <v>58088.03125</v>
+        <v>51477.0390625</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -4414,10 +4830,10 @@
       <c r="C7" t="s"/>
       <c r="D7" t="s"/>
       <c r="E7" t="n">
-        <v>3276</v>
+        <v>3401.470886230469</v>
       </c>
       <c r="F7" t="n">
-        <v>98065.052734375</v>
+        <v>134371.23828125</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -4428,10 +4844,10 @@
       <c r="C8" t="s"/>
       <c r="D8" t="s"/>
       <c r="E8" t="n">
-        <v>19953.8837890625</v>
+        <v>16998.4658203125</v>
       </c>
       <c r="F8" t="n">
-        <v>429477.453125</v>
+        <v>458175.984375</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -4442,10 +4858,10 @@
       <c r="C9" t="s"/>
       <c r="D9" t="s"/>
       <c r="E9" t="n">
-        <v>32714.84375</v>
+        <v>25114.10498046875</v>
       </c>
       <c r="F9" t="n">
-        <v>883439.765625</v>
+        <v>867694</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -4456,10 +4872,10 @@
       <c r="C10" t="s"/>
       <c r="D10" t="s"/>
       <c r="E10" t="n">
-        <v>123844.984375</v>
+        <v>98297.34375</v>
       </c>
       <c r="F10" t="n">
-        <v>2452644.25</v>
+        <v>2409430</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -4498,10 +4914,10 @@
         <v>0</v>
       </c>
       <c r="E18" t="n">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="F18" t="n">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -4512,10 +4928,10 @@
       <c r="C19" t="s"/>
       <c r="D19" t="s"/>
       <c r="E19" t="n">
-        <v>26819.01390075684</v>
+        <v>21458.25446926818</v>
       </c>
       <c r="F19" t="n">
-        <v>673006.7430245535</v>
+        <v>660920.2998246173</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -4526,10 +4942,10 @@
       <c r="C20" t="s"/>
       <c r="D20" t="s"/>
       <c r="E20" t="n">
-        <v>30595.90231391939</v>
+        <v>24312.05426421196</v>
       </c>
       <c r="F20" t="n">
-        <v>754212.5537659391</v>
+        <v>741757.0630844873</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -4540,10 +4956,10 @@
       <c r="C21" t="s"/>
       <c r="D21" t="s"/>
       <c r="E21" t="n">
-        <v>1334</v>
+        <v>1039.89697265625</v>
       </c>
       <c r="F21" t="n">
-        <v>58088.03125</v>
+        <v>51477.0390625</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -4554,10 +4970,10 @@
       <c r="C22" t="s"/>
       <c r="D22" t="s"/>
       <c r="E22" t="n">
-        <v>3276</v>
+        <v>3487.368896484375</v>
       </c>
       <c r="F22" t="n">
-        <v>98065.052734375</v>
+        <v>133770.265625</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -4568,10 +4984,10 @@
       <c r="C23" t="s"/>
       <c r="D23" t="s"/>
       <c r="E23" t="n">
-        <v>19953.8837890625</v>
+        <v>16902.26953125</v>
       </c>
       <c r="F23" t="n">
-        <v>429477.453125</v>
+        <v>459627.34375</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -4582,10 +4998,10 @@
       <c r="C24" t="s"/>
       <c r="D24" t="s"/>
       <c r="E24" t="n">
-        <v>32714.84375</v>
+        <v>24272.455078125</v>
       </c>
       <c r="F24" t="n">
-        <v>883439.765625</v>
+        <v>863191</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -4596,10 +5012,10 @@
       <c r="C25" t="s"/>
       <c r="D25" t="s"/>
       <c r="E25" t="n">
-        <v>123846.109375</v>
+        <v>98413.34375</v>
       </c>
       <c r="F25" t="n">
-        <v>2452644.25</v>
+        <v>2409430</v>
       </c>
     </row>
   </sheetData>

</xml_diff>